<commit_message>
Update product information and add new transducer
</commit_message>
<xml_diff>
--- a/data/all_products_block123.xlsx
+++ b/data/all_products_block123.xlsx
@@ -518,17 +518,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'heading': 'Advanced Navigation Algorithms', 'text': 'The advanced Seapath navigation algorithms integrate RTK GNSS data with the inertial sensor data from the MRU. This gives the Seapath 380 unique advantages compared to stand-alone RTK products. The Seapath product’s accurate roll, pitch and heading measurements allow the RTK antenna position to be referenced to any point on the vessel where accurate position and velocity are required. All data from Seapath have the same time stamp and the output is in real-time.'}</t>
+          <t>{'heading': 'Advanced Integration for Superior Performance', 'text': 'The advanced Seapath navigation algorithms integrate RTK GNSS data with the inertial sensor data from the MRU. This unique combination gives the Seapath 380 series distinct advantages over stand-alone RTK products, including accurate measurements of roll, pitch, and heading. This marriage of technologies enables the RTK antenna position to be referenced to exact points on the vessel, synchronizing every data output in real-time. The system allows subdecimetre position accuracy through online and offline satellite orbit and clock data processing.'}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'heading': 'System Configuration and Product Range', 'text': 'This Seapath series is a two-module solution with a processing unit and a HMI unit connected via Ethernet. The processing unit runs all critical computations independent from the user interface on the HMI unit to ensure continuous and reliable operation. The latest Seapath software includes Automatic Online Calibration (AOC) that significantly improves the roll and pitch accuracy. The Seapath 380 series is delivered in the following product range: Seapath 380-3, Seapath 380-H, Seapath 380-5, and Seapath 380-5+.'}</t>
+          <t>{'heading': 'Product Range and Applications', 'text': 'Offered in several configurations, the Seapath 380 series delivers a range of roll and pitch accuracy options, fulfilling demands for different marine applications. With the latest software Automatic Online Calibration, the series also ensures improved roll and pitch accuracy and eliminates the need for recalibration in motion. The Seapath 380 series is specially designed for hydrographic surveying and dredging, providing comprehensive and accurate data that meets IHO special order requirements.'}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{'heading': 'Applications and Interface', 'text': 'By using standard DGNSS, Fugro XP2/G2/G4/G4+ and RTK corrections, the Seapath 380 is a unique solution for hydrographic surveying and dredging work demanding the most comprehensive and accurate surveying data available. The processing unit has eight RS-232/422 serial lines, four Ethernet LANs and three analog output channels, making the distribution of Seapath data to various users onboard almost endless.'}</t>
+          <t>{'heading': 'System Design and Connectivity', 'text': 'The Seapath series boasts a two-module system design, comprised of a processing unit and an HMI unit connected via Ethernet for robust operation. Multiple HMI units may be added, displaying vessel motion in straightforward formats. The Seapath 380 series further impresses with a multitude of connectivity options, including eight RS-232/422 serial lines, Ethernet LANs, and analog outputs, facilitating extensive on-board data distribution and interfacing with various correction services.'}</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -606,17 +606,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'heading': 'Common Technical Specifications', 'text': 'The Simrad 12-16/60 operates at a resonant frequency of 12 kHz, designed for a maximum transducer depth of 20 m, and comes with a 20 m cable that has a diameter of 12.5 mm. Its weight is 84 kg with the cable and 78 kg without it. Designed for a variety of marine environments, it can be stored within a temperature range from -20 to 70 °C.'}</t>
+          <t>{'heading': 'Transducer Overview', 'text': "Simrad 12-16/60 transducer is known for its reliable performance and robust build. It's an advanced 12 kHz dual-beam apparatus capable of operating at a maximum depth of 20 meters. Equipped with an adequately lengthy 20-meter cable, it features a convenient cable diameter of 12.5 mm and a manageable weight that varies very slightly with or without cable, providing flexibility and ease in handling. With a storage temperature tolerance ranging from -20 to 70 °C, the device demonstrates versatility under varying environmental storage conditions."}</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'heading': 'Detailed Specifications and Performance', 'text': 'The 12-16/60 features an 18 + 1 element configuration for the narrow beam with a circular beamwidth of 16 degrees and a directivity index (DI) of 21 dB. The side lobes are less than -15 dB, and back radiation is below -30 dB. It has an impedance nominal of 60 ohms and a maximum variation in absolute impedance from 45 to 80 ohms. The transmitting response reaches 171 dB re 1µPa per V, while its receiving sensitivity is -168.5 dB re 1V per µPa. Electroacoustic efficiency stands at 0.60 with a maximum input of 2000 W pulse power and 80 W continuous power. For the wide beam configuration with 1 element, the circular beamwidth is 60 degrees, DI is 10 dB with side lobes not applicable and back radiation less than -15 dB. Its impedance nominal is 2 kohms with a variation range of 1 to 3 kohms.'}</t>
+          <t>{'heading': 'Operational Characteristics', 'text': "The transducer's functionality is enhanced by its dual beam capability with 18 + 1 elements for a narrow beam and 1 element for a wide beam, delivering a circular beamwidth of 16 degrees in the former and 60 degrees in the latter. The directional capabilities and the receiving sensitivity are optimally balanced to provide accurate readings. Directivity and beam angle details, along with side lobes and back radiation levels, reveal a design with a focus on minimizing unwanted signals and enhancing the target signal reception. The symmetrical operational parameters between transmitting response and receiving sensitivity, flanked by an impressive electroacoustic efficiency of 0.60, showcase a well-engineered product designed for the precise acoustic undertakings."}</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>{'heading': 'Manufacturer and Ordering Information', 'text': "For ordering, the product's order number is KSV-089510. The Simrad 12-16/60 is manufactured by Simrad AS, located at Strandpromenaden 50, P.O.Box 111, N-3191 Horten with telephone contact available at +47 33 03 40 00."}</t>
+          <t>{'heading': 'Manufacturer Details', 'text': 'The Simrad 12-16/60 is a product of Simrad AS, strategically headquartered at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. For queries or further details, interests can reach out to them via phone at +47 33 03 40 00, ensuring a direct line of communication between the manufacturer and the end-user or distributor.'}</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -693,17 +693,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'heading': 'Solid Construction and Deep-Water Capability', 'text': 'This Simrad single-beam transducer is encapsulated within a robust housing, ensuring its durability and reliability under extreme conditions. Designed to handle the challenges of deep-water exploration, the 120-25 is capable of operating at depths up to 1000 meters, making it a trustworthy tool for a wide range of marine applications.'}</t>
+          <t>{'heading': 'Durable and Deep Diving', 'text': "Simrad's 120-25 transducer exhibits exceptional durability. Engineered with a solid interior and encased in a robust housing, this transducer is designed to endure the pressures found at substantial depths, making it reliable for operations down to 1000 meters. This characteristic is essential for marine applications where equipment must withstand challenging underwater conditions."}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'heading': 'Manufacturer and Contact Information', 'text': 'Simrad AS stands behind the 120-25 transducer, with a reputation for engineering excellence. The company is located at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. Customers can reach out via telephone at +47 33 03 40 00 or send a fax to +47 33 04 29 87 for any inquiries or support related to their transducer technology.'}</t>
+          <t>{'heading': 'Installation and Dimensions', 'text': 'To ensure optimal performance, the 120-25 transducer comes with specific installation protocols. The package includes an outlined dimension guide that assists in proper setup, and an example configuration to visualize the end result. Correct handling during the installation phase guarantees that the transducer works effectively in its marine environment.'}</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>{'heading': 'Ordering and Product Information', 'text': 'For those interested in procuring the Simrad 120-25 transducer, the order number to reference is KSV-062615. This identification ensures accuracy in orders and assists in streamlining the acquisition process for customers seeking this specific model of the single-beam transducer.'}</t>
+          <t>{'heading': 'Contact Details', 'text': 'For any queries or additional support related to the 120-25 transducer, contact Simrad AS at the provided address. They are located at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. Customers can reach them by telephone, +47 33 03 40 00, or by telefax, +47 33 04 29 87.'}</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -749,24 +749,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The 18-11 is a large, single-beam transducer with a relatively narrow beam. It is ideal for use in ocean depth measurement to a maximum depth of 7000 m.'}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Design and Capabilities', 'text': 'Operating at a resonant frequency of 18 kHz, this transducer is capable of transmitting responses with 176 ±2 dB power and receiving sensitivity, open circuit, at -168 ±2 dB. It features a circular beamwidth of 11 ±2 degrees and showcases a directivity index (DI) of 25 ±1 dB, derived from a directivity (D) of 300 ±20%. The electroacoustic efficiency is marked at 0.60 ±0.20, displaying adept energy conversion from electrical signals to acoustic waves and vice versa.'}</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>{'heading': 'Performance Specifications', 'text': 'Built to withstand large depths, the Simrad 18-11 allows a maximum pulse power input of 2000 W and can continuously handle power up to 100 W. Equipped to operate efficiently down to 50 meters submersion, it maintains an equivalent two-way beam angle (ψ) of 0.020 ±20% and has low side lobes and back radiation, less than -18 dB and -35 dB respectively. For connectivity, it comes with a 20 m cable, ensuring flexibility and reach.'}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>Key Features:
@@ -836,22 +832,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The 200-28E is a 200 kHz single-beam transducer protected in a robust housing. The solid interior is void of air pockets or expanded foam enabling it to withstand the pressure at a depth of 1000 m.'}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust Design', 'text': "Simrad's 200-28E constitutes a 200 kHz single-beam transducer that has been meticulously constructed in a robust housing. This specific design approach ensures that the transducer's interior remains solid, free from any air pockets or the use of expanded foam. Such a structural integrity is paramount as it endows the device with the remarkable strength to endure considerable pressures found at depths reaching up to 1000 meters."}</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Performance', 'text': 'The 200-28E showcases a resonant frequency of 200 kHz and features an electroacoustic efficiency rating of 70 ±20 %. It is also equipped with a circular beamwidth of 7 degrees ±1 degree. This single-beam transducer is capable of accepting a maximum input power of 1500 W, paired with a directivity index of 28.5 dB. It is designed to operate within a maximum duty cycle of 4% at top power and can be installed at depths up to 1000 meters. With an equivalent two-way beam angle (ψ) of -21 dB re 1 steradian and nominal impedance of 60 ohm, it balances performance and resilience effectively.'}</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durability and Practicality', 'text': "This robust tool is constructed to sustain extreme storage temperatures, ranging from -20º C to 70º C, ensuring its durability in various environmental conditions. The nominal impedance consistency ranges from 45 to 80 ohm, with a maximum variation in phase of ±30 degrees. Significantly, the transducer is complemented by a 25 m cable, ensuring its practicality in deployment, while maintaining a manageable weight of 3.4 kg without cable. The transmitting response and receiving sensitivity are fine-tuned for precision, highlighting the transducer's quality and reliability."}</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -921,24 +917,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The 3710 DGNSS Receiver is a high-performance DGNSS receiver capable of receiving augmentation data from the Fugro Satellite Positioning worldwide DGNSS Service. The Fugro service is a full-time differential GNSS (DGNSS) broadcast system delivering differential corrections from an array of GNSS reference stations located around the globe. These services include independent sub-decimetre level services (Fugro Seastar G4/G2 and Fugro Seastar XP2), centimetre level services (Fugro Seastar G2+/G4+) and sub-metre level services (Fugro Seastar StdL1).'}</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced availability DGNSS processing', 'text': 'The 3710 DGNSS Receiver gives the user an unmatched availability in challenging environments where the use of differential corrections is vital for an efficient operation. The 3710 DGNSS Receiver offers reception from both internet and satellites simultaneously. It has the unique capability of simultaneously receiving and outputting data from up to three sources (two satellite links and one internet link). The signals are received via the DGNSS antenna and by internet. After selection of the desired broadcast source, the signals are made available as corrections for use in a GNSS differential capable receiver.'}</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>{'heading': 'Multiplexing Capability and Reception', 'text': 'The 3710 DGNSS Receiver comprises a software defined radio (SDR) signal processing core with advanced algorithms and true parallel processing of up to two DGNSS satellite signals and one DGNSS Ethernet signal (NTRIP format) simultaneously. DGNSS corrections from different sources are combined by the unique multiplexing capability.'}</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>• High-performance DGNSS receiver
@@ -1013,24 +1005,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The 38-7 is a large, single-beam transducer incorporating 88 Tonpilz elements. It has a relatively narrow beam with substantial range capability.'}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Superior Beam Performance', 'text': 'The resonant frequency of the Simrad 38-7 transducer is at 38 kHz with a directional beamwidth of 7 degrees ±1, ensuring focused transmission and reception. This is complemented by an impressive directivity index of 28 ±1 dB and an equivalent two-way beam angle of -20.5 ±1 dB, minimizing side lobe and back radiation interference with levels less than -15 dB and -35 dB respectively. This results in a transducer with a highly concentrated acoustic output, suitable for various marine applications.'}</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>{'heading': 'High Sensitivity and Power Handling', 'text': 'With a transmitting response of 185.5 dB ±2 re 1µPa per V and receiving sensitivity at an open circuit of -170.5 dB ±2 re 1V per µPa, the Simrad 38-7 combines exceptional sensitivity with robust power handling. The electro-acoustic efficiency ranges from a minimum of 0.50 to a typical figure of 0.70, making it highly efficient in its conversion of electrical energy to acoustic energy and back. Capable of handling a maximum input power of 4000 W and operating safely within a maximum duty cycle of 1% at the maximum power, this transducer is designed for applications requiring precise and powerful underwater acoustic transmissions.'}</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t xml:space="preserve"> - Incorporates 88 Tonpilz elements

</xml_diff>

<commit_message>
Update product data files
</commit_message>
<xml_diff>
--- a/data/all_products_block123.xlsx
+++ b/data/all_products_block123.xlsx
@@ -518,17 +518,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'heading': 'Advanced Integration for Superior Performance', 'text': 'The advanced Seapath navigation algorithms integrate RTK GNSS data with the inertial sensor data from the MRU. This unique combination gives the Seapath 380 series distinct advantages over stand-alone RTK products, including accurate measurements of roll, pitch, and heading. This marriage of technologies enables the RTK antenna position to be referenced to exact points on the vessel, synchronizing every data output in real-time. The system allows subdecimetre position accuracy through online and offline satellite orbit and clock data processing.'}</t>
+          <t>{'heading': 'Advanced Navigation Integration', 'text': 'The advanced Seapath navigation algorithms integrate RTK GNSS data with the inertial sensor data from the MRU. This gives the Seapath 380 unique advantages compared to stand-alone RTK products. The Seapath product’s accurate roll, pitch and heading measurements allow the RTK antenna position to be referenced to any point on the vessel where accurate position and velocity are required. All data from Seapath have the same time stamp and the output is in real-time.'}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'heading': 'Product Range and Applications', 'text': 'Offered in several configurations, the Seapath 380 series delivers a range of roll and pitch accuracy options, fulfilling demands for different marine applications. With the latest software Automatic Online Calibration, the series also ensures improved roll and pitch accuracy and eliminates the need for recalibration in motion. The Seapath 380 series is specially designed for hydrographic surveying and dredging, providing comprehensive and accurate data that meets IHO special order requirements.'}</t>
+          <t>{'heading': 'Functional Design and System Configuration', 'text': 'This Seapath series is a two-module solution with a processing unit and a HMI unit connected via Ethernet. The processing unit runs all critical computations independent from user interface on the HMI unit to ensure continuous and reliable operation. The Seapath is operated through the operator software installed on one or several HMI units. This software is used for performance monitoring, configuration and troubleshooting of the system.'}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{'heading': 'System Design and Connectivity', 'text': 'The Seapath series boasts a two-module system design, comprised of a processing unit and an HMI unit connected via Ethernet for robust operation. Multiple HMI units may be added, displaying vessel motion in straightforward formats. The Seapath 380 series further impresses with a multitude of connectivity options, including eight RS-232/422 serial lines, Ethernet LANs, and analog outputs, facilitating extensive on-board data distribution and interfacing with various correction services.'}</t>
+          <t>{'heading': 'Product Range and Applications', 'text': 'The Seapath 380 series is delivered in a range of models with varying roll/pitch and heading accuracies, meeting diverse operational needs. The latest software includes features such as Automatic Online Calibration (AOC), enhancing roll and pitch accuracy without needing recalibration of the IMU in motion. The Seapath 380 is designed for hydrographic surveying and dredging work demanding the most comprehensive and accurate surveying data available.'}</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -606,17 +606,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{'heading': 'Transducer Overview', 'text': "Simrad 12-16/60 transducer is known for its reliable performance and robust build. It's an advanced 12 kHz dual-beam apparatus capable of operating at a maximum depth of 20 meters. Equipped with an adequately lengthy 20-meter cable, it features a convenient cable diameter of 12.5 mm and a manageable weight that varies very slightly with or without cable, providing flexibility and ease in handling. With a storage temperature tolerance ranging from -20 to 70 °C, the device demonstrates versatility under varying environmental storage conditions."}</t>
+          <t>{'heading': 'Dual-Beam Functionality', 'text': 'As a sophisticated marine device, the Simrad 12-16/60 operates at a resonant frequency of 12 kHz, suitable for various underwater activities. It enjoys a broad spectrum of utility with a significant maximum transducer depth of 20 meters complemented by a 20-meter cable length ensuring breadth and reach in deployment. The transducer is also conveniently designed, weighing 84 kg with the cable and 78 kg without it, providing manageable movement and setup. The careful consideration given to its storage temperature tolerances, between -20 to 70 °C, contributes to its durability and lifespan in varied marine environments.'}</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'heading': 'Operational Characteristics', 'text': "The transducer's functionality is enhanced by its dual beam capability with 18 + 1 elements for a narrow beam and 1 element for a wide beam, delivering a circular beamwidth of 16 degrees in the former and 60 degrees in the latter. The directional capabilities and the receiving sensitivity are optimally balanced to provide accurate readings. Directivity and beam angle details, along with side lobes and back radiation levels, reveal a design with a focus on minimizing unwanted signals and enhancing the target signal reception. The symmetrical operational parameters between transmitting response and receiving sensitivity, flanked by an impressive electroacoustic efficiency of 0.60, showcase a well-engineered product designed for the precise acoustic undertakings."}</t>
+          <t>{'heading': 'Beam Characteristics', 'text': 'The 12-16/60 transducer is adept at offering a choice between narrow and wide beam navigations with circular beamwidths of 16 and 60 degrees, respectively. The narrow beam displays a notable directivity factor (D) of 130 with a relative directivity index (DI) of 21 dB and an equivalent two-way beam angle (Ψ) of 0.045, equating to -13.5 dB when logarithmically translated. Conversely, the wide beam’s D is substantially lower at 10 with a DI of 10 dB, while its Ψ is significantly broader at 0.6, reflecting a -2 dB rating in decibel terms.'}</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>{'heading': 'Manufacturer Details', 'text': 'The Simrad 12-16/60 is a product of Simrad AS, strategically headquartered at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. For queries or further details, interests can reach out to them via phone at +47 33 03 40 00, ensuring a direct line of communication between the manufacturer and the end-user or distributor.'}</t>
+          <t>{'heading': 'Technical and Acoustic Performance', 'text': "From an acoustic perspective, the 12-16/60 encompasses impressive technical capabilities. Featuring a nominal impedance of 60 ohms with an allowable variation between 45 to 80 ohms and a phase angle variation within ±30 degrees for the narrow beam, it showcases robust performance standards, echoed in the maximum pulse and continuous power inputs of 2000 W and 80 W respectively. The wide beam's impedance stands nominally at 2 kohms and varies between 1 to 3 kohms, complemented by a transmitting response of 142 dB re 1µPa per V and a receiving sensitivity of -168.5 dB re 1V per µPa. These distinct technical specifications, which include an electroacoustic efficiency of 0.60, speak to the transducer's efficacy in rigorous underwater operations."}</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -693,17 +693,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{'heading': 'Durable and Deep Diving', 'text': "Simrad's 120-25 transducer exhibits exceptional durability. Engineered with a solid interior and encased in a robust housing, this transducer is designed to endure the pressures found at substantial depths, making it reliable for operations down to 1000 meters. This characteristic is essential for marine applications where equipment must withstand challenging underwater conditions."}</t>
+          <t>{'heading': 'Order Number and Technical Overview', 'text': 'Order number KSV-062615 provides a reference for the 120 kHz single-beam Simrad 120-25 transducer. This device boasts a maximum input power of 1000 W and a beamwidth that is circular, 10 deg. ±2 deg. Its design ensures a directivity index of 25 dB and it can operate with a maximum duty cycle of 5% at the highest power setting. The transducer has an impressive maximum installation depth of 1000 m, making it suitable for deep-water applications.'}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'heading': 'Installation and Dimensions', 'text': 'To ensure optimal performance, the 120-25 transducer comes with specific installation protocols. The package includes an outlined dimension guide that assists in proper setup, and an example configuration to visualize the end result. Correct handling during the installation phase guarantees that the transducer works effectively in its marine environment.'}</t>
+          <t>{'heading': 'Performance and Construction Details', 'text': "The Simrad 120-25 transducer is engineered for efficiency and durability. It has an equivalent two-way beam angle (ψ) of -17.5 dB re 1 steradian and a cable length of 25 m that facilitates its usage in a variety of settings. With a nominal impedance of 60 ohm, the equipment is designed to maintain a consistent performance with the maximum variation in |Z| ranging from 45 to 80 ohm. The device's weight without cable is kept at a manageable 4 kg. Additionally, the maximum variation in phase is within ±30 deg, exhibiting its precision in operation."}</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>{'heading': 'Contact Details', 'text': 'For any queries or additional support related to the 120-25 transducer, contact Simrad AS at the provided address. They are located at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. Customers can reach them by telephone, +47 33 03 40 00, or by telefax, +47 33 04 29 87.'}</t>
+          <t>{'heading': 'Acoustic Qualities and Efficiency', 'text': "The transmitting response of the Simrad 120-25 is finely tuned at 176.5 ±2 dB re 1µPa per V, while its receiving sensitivity (open circuit) is marked at -183.0 ±2 dB re 1V per µPa. Such characteristics reflect the transducer's high level of sensitivity and signal quality. An electroacoustic efficiency of 70 ±20 % is indicative of the transducer’s effective conversion of electrical power into acoustic energy. This efficiency, combined with its robust construction, makes the 120-25 an excellent choice for various underwater acoustic applications."}</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -754,15 +754,19 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{'heading': 'Design and Capabilities', 'text': 'Operating at a resonant frequency of 18 kHz, this transducer is capable of transmitting responses with 176 ±2 dB power and receiving sensitivity, open circuit, at -168 ±2 dB. It features a circular beamwidth of 11 ±2 degrees and showcases a directivity index (DI) of 25 ±1 dB, derived from a directivity (D) of 300 ±20%. The electroacoustic efficiency is marked at 0.60 ±0.20, displaying adept energy conversion from electrical signals to acoustic waves and vice versa.'}</t>
+          <t>{'heading': 'Key Specifications', 'text': 'The Simrad 18-11 is designed for large depths, characterized by a resonant frequency of 18 kHz and a circular beamwidth of 11 ±2 deg. It boasts a transmitting response of 176 ±2 dB and a receiving sensitivity, open circuit, of -168 ±2 dB. The effective directivity of the transducer is 300 ±20 % with an electroacoustic efficiency of 0.60 ±0.20. It can handle a maximum pulse power input of 2000 W and a maximum continuous power input of 100 W, ensuring reliable performance in demanding conditions.'}</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'heading': 'Performance Specifications', 'text': 'Built to withstand large depths, the Simrad 18-11 allows a maximum pulse power input of 2000 W and can continuously handle power up to 100 W. Equipped to operate efficiently down to 50 meters submersion, it maintains an equivalent two-way beam angle (ψ) of 0.020 ±20% and has low side lobes and back radiation, less than -18 dB and -35 dB respectively. For connectivity, it comes with a 20 m cable, ensuring flexibility and reach.'}</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>{'heading': 'Physical Attributes and Operating Parameters', 'text': 'Built for enduring the pressures of the deep, the Simrad 18-11 can be immersed to a depth of up to 50 meters. It has a hefty structure, weighing 85 kg without the cable, which extends 20 meters long and has an 11 mm diameter. For storage, it has a temperature range tolerance from +70 to -20 °C, showcasing robustness in various environmental conditions.'}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{'heading': 'Manufacturing Details', 'text': 'The Simrad 18-11 transducer is manufactured by Simrad AS, located at Strandpromenaden 50, P.O.Box 111, N-3191 Horten. Clients can reach them via telephone at +47 33 03 40 00 or by telefax at +47 33 04 29 87. Further information can be obtained through the company’s website at www.simrad.com.'}</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>Key Features:
@@ -837,17 +841,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{'heading': 'Robust Design', 'text': "Simrad's 200-28E constitutes a 200 kHz single-beam transducer that has been meticulously constructed in a robust housing. This specific design approach ensures that the transducer's interior remains solid, free from any air pockets or the use of expanded foam. Such a structural integrity is paramount as it endows the device with the remarkable strength to endure considerable pressures found at depths reaching up to 1000 meters."}</t>
+          <t>{'heading': 'Robust Design &amp; Deepwater Capability', 'text': 'This 200 kHz single-beam transducer is encased in robust housing, ensuring its durability and reliability in challenging marine environments. The design is meticulously crafted to be free of air pockets or expanded foam, a feature that allows the 200-28E to operate effectively at the considerable depth of 1000 meters underwater.'}</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'heading': 'Optimized Performance', 'text': 'The 200-28E showcases a resonant frequency of 200 kHz and features an electroacoustic efficiency rating of 70 ±20 %. It is also equipped with a circular beamwidth of 7 degrees ±1 degree. This single-beam transducer is capable of accepting a maximum input power of 1500 W, paired with a directivity index of 28.5 dB. It is designed to operate within a maximum duty cycle of 4% at top power and can be installed at depths up to 1000 meters. With an equivalent two-way beam angle (ψ) of -21 dB re 1 steradian and nominal impedance of 60 ohm, it balances performance and resilience effectively.'}</t>
+          <t>{'heading': 'High Performance and Efficient Operation', 'text': 'The transducer operates at a resonant frequency of 200 kHz with an electroacoustic efficiency of 70±20%. It features a circular beamwidth of 7 degrees±1 degree, allowing for precise readings. The high directivity index of 28.5 dB and transmitting response of 180.0±2 dB re 1µPa per V promote efficient sonar performance with a maximum input power of 1500 W.'}</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>{'heading': 'Durability and Practicality', 'text': "This robust tool is constructed to sustain extreme storage temperatures, ranging from -20º C to 70º C, ensuring its durability in various environmental conditions. The nominal impedance consistency ranges from 45 to 80 ohm, with a maximum variation in phase of ±30 degrees. Significantly, the transducer is complemented by a 25 m cable, ensuring its practicality in deployment, while maintaining a manageable weight of 3.4 kg without cable. The transmitting response and receiving sensitivity are fine-tuned for precision, highlighting the transducer's quality and reliability."}</t>
+          <t>{'heading': 'Durable Construction and Environmental Range', 'text': "With a maximum installation depth of 1000 m, the 200-28E is constructed to endure significant underwater pressure. Its operating temperature range, with a maximum storage temperature of 70º C and a minimum of -20º C, supports functionality in various environmental conditions. The unit's cable is 25 meters in length, accommodating a range of installation scenarios."}</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -927,10 +931,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{'heading': 'Multiplexing Capability and Reception', 'text': 'The 3710 DGNSS Receiver comprises a software defined radio (SDR) signal processing core with advanced algorithms and true parallel processing of up to two DGNSS satellite signals and one DGNSS Ethernet signal (NTRIP format) simultaneously. DGNSS corrections from different sources are combined by the unique multiplexing capability.'}</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>{'heading': 'Multiplexing Capability', 'text': 'The 3710 DGNSS Receiver comprises a software defined radio (SDR) signal processing core with advanced algorithms and true parallel processing of up to two DGNSS satellite signals and one DGNSS Ethernet signal (NTRIP format) simultaneously. DGNSS corrections from different sources are combined by the unique multiplexing capability.'}</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{'heading': 'Receiver and Antenna Information', 'text': 'The DGNSS IALA antenna (300) and GPS antenna (310) with Fugro Seastar™ XP/XP2/G2/G2+/G4/G4+/StdL1 capability provide configurable output for external interfaces. The integrated system includes a 2-line LCD display and keypad for configuration and status, accompanied by easy software updates via USB. Additionally, an Ethernet interface and a serial interface enhance the connectivity of the receiver.'}</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>• High-performance DGNSS receiver
@@ -1010,15 +1018,19 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{'heading': 'Superior Beam Performance', 'text': 'The resonant frequency of the Simrad 38-7 transducer is at 38 kHz with a directional beamwidth of 7 degrees ±1, ensuring focused transmission and reception. This is complemented by an impressive directivity index of 28 ±1 dB and an equivalent two-way beam angle of -20.5 ±1 dB, minimizing side lobe and back radiation interference with levels less than -15 dB and -35 dB respectively. This results in a transducer with a highly concentrated acoustic output, suitable for various marine applications.'}</t>
+          <t>{'heading': 'Transducer Overview', 'text': 'The Simrad 38-7 transducer operates at a resonant frequency of 38 kHz and is equipped with a cable length of 20 meters. Its beamwidth is circular at 7 degrees with a variability of ±1, and the directivity index comes in at 28 ±1 dB. Additionally, it has a side lobe level of less than -15 dB and back radiation less than -35 dB, which play a crucial role in minimizing unwanted signal reception and transmission.'}</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{'heading': 'High Sensitivity and Power Handling', 'text': 'With a transmitting response of 185.5 dB ±2 re 1µPa per V and receiving sensitivity at an open circuit of -170.5 dB ±2 re 1V per µPa, the Simrad 38-7 combines exceptional sensitivity with robust power handling. The electro-acoustic efficiency ranges from a minimum of 0.50 to a typical figure of 0.70, making it highly efficient in its conversion of electrical energy to acoustic energy and back. Capable of handling a maximum input power of 4000 W and operating safely within a maximum duty cycle of 1% at the maximum power, this transducer is designed for applications requiring precise and powerful underwater acoustic transmissions.'}</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>{'heading': 'Performance Characteristics', 'text': 'Optimized for performance, the 38-7 transducer has an equivalent two-way beam angle of -20.5 ±1 dB and an impedance with a nominal 60 ohms. Transmitting response is impressive at 185.5 dB re 1µPa per V, with a receiving sensitivity of -170.5 dB re 1V per µPa. The electroacoustic efficiency is rated typical at 0.70 and not less than the minimum of 0.50.'}</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{'heading': 'Operational Parameters', 'text': 'To suit high-power applications, the transducer can handle a maximum input power of 4000 W and a maximum duty cycle at max. power of 1 percent. The maximum transducer depth is noted at 50 meters, appropriate for various marine survey and operational environments. It exemplifies the robust design suitable for the rigorous demands of marine exploration and data collection.'}</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t xml:space="preserve"> - Incorporates 88 Tonpilz elements
@@ -1086,22 +1098,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The 50-18 is a small, single-beam transducer incorporating seven Tonpilz elements in a polyurethane housing. Its compact design requires little space and it is employed extensively with navigational echo sounders. A compatible steel tank and mounting ring are also available.'}</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Compact and Extensively Used Transducer', 'text': 'Simrad 50-18, 50 kHz Single-beam transducer is known for its small footprint. The use of seven Tonpilz elements within a durable polyurethane housing ensures a robust design with minimal space requirements. Frequently employed with navigational echo sounders, this single-beam transducer demonstrates versatile application. To aid installation, there is also a compatible steel tank and mounting ring available for users.'}</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for Performance and Ease of Installation', 'text': "The transducer's beamwidth is circular, quantified at 18 degrees with a variance of plus or minus 3, ensuring precise readings. Its maximum transducer depth reaches down to 10 meters, making it suitable for a range of maritime environments. For efficient communication, the transducer is paired with a 20-meter-long cable, with a diameter of 10.9 millimeters, providing ample length and durability for various vessel configurations."}</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Detailed Specifications', 'text': "The 50-18 transmits with a resonant frequency of 50 kHz and maximum continuous power input of 10 W. Its directivity is strong, with side lobes significantly less than -15 dB and back radiation lower than -25 dB, ensuring focused signal transmission. The transducer has a nominal impedance of 60 ohms, with a maximum variation in absolute impedance from 45 to 80 ohms, and a phase angle variation within plus or minus 30 degrees. These thorough specifications underline the transducer's reliability and efficiency in maritime explorations."}</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1166,22 +1178,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': '500 kHz transducer for shallow water surveying. The transducer has a narrow 3° beam width and high depth resolution.'}</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Shallow Water Surveying Capability', 'text': 'The 500 kHz transducer is designed for shallow water surveying. It provides a small beam width, high resolution, and a high bandwidth with a Q value of 2.3. The design is robust and rugged, and the transducer is recommended for portable applications.'}</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Performance and Specifications', 'text': 'Resonant frequency 500 kHz with a circular beam width 3º and an impedance nominal value of 60 Ω. Transmitting Voltage Response is 186 ±2 dB (re 1 μPa per 1 V), Receiving Voltage Response at -189 ±2 dB (re 1 V per μPa). Maximum pulse power input is 500 W @ 2% duty cycle, with a maximum transducer depth of 10 m, and cable length of 10 m.'}</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Physical Characteristics and Operating Range', 'text': "The transducer's weight with cable is 3.4 kg. Operational temperature ranges from -6 to +48 ºC and storage temperature from -20 to +70 ºC. Dimensions and thread details are provided (in mm), and the cable diameter is measured at 7.0 mm."}</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1259,22 +1271,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The ACS500 system is the new generation of the Kongsberg Martime Acoustic Control System. It is developed to increase the operational depths and is rated to 4000 metres. The ACS500 system is divided into two units: Surface system (portable) and Subsea system. The ACS may also be operated from the HiPAP system.'}</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Surface and Subsea Units', 'text': 'The surface system includes an Acoustic Command Unit with a charger cable, a splash-proof portable case, and operational interfaces via computer (touch screen/trackball). It has an internal rechargeable battery providing over 10 hours of operation. Paired with this is the Dunking Transducer Unit, portable and designed for varying water depths, delivering operational excellence. The subsea system, now with interseal test ports, consists of sophisticated subsea control and communication units, facilitating reliable underwater operations. These advanced units interface with valve packages via multiple cable configurations for seamless operation.'}</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Comprehensive Applications and Portable Solutions', 'text': "The ACS500 is adaptable for a variety of applications including the Emergency BOP backup control system, Pipeline Valve Control, Workover system, Offshore loading, and other subsea control systems. Acknowledging the demands of on-board safety equipment, the portable and compact design of the surface system's Acoustic Command Unit caters to dynamic marine environments, offering splash-proof robustness and dependable communication between the deck and subsea units."}</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Technical Excellence and Environmental Performance', 'text': "The ACS500 boasts high environmental performance, with a wide operational temperature range for both the surface and subsea systems. Notably, the SCUs are intricately designed for deep-sea operations and constructed from materials like Super Duplex Steel to withstand harsh underwater conditions. Accompanying technical specifications such as operational frequencies, wake-up channels, transmission power, and battery details, underscore the ACS500's technical prowess, aligning with rigorous standards and certifications from respected maritime authorities."}</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1337,22 +1349,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS 300 is the 4th generation AIS class A mobile station from Kongsberg and is designed to be fully integrated in a ship’s bridge environment. An improved receiver sensitivity of -115 dBm gives an increased range compared to AIS units with the standard sensitivity of -107 dBm. The AIS 300 is tested and approved in accordance with international regulations and has the Wheelmark certification. In addition, the AIS 300 is tested and approved in accordance with the inland AIS regulations.'}</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Integration and Maintenance', 'text': 'The AIS 300 is designed to be fully integrated with other navigation systems and can be delivered without an external display (MKD - Minimum Keyboard and Display), provided that the ECDIS is listed in MED-B for AIS-300. All operations and functionalities are handled from the ECDIS in an integrated bridge system. The AIS 300 is hence type approved with ECDIS from different manufacturers and brands, to avoid installing a redundant display/keyboard. One important principle of e-navigation is to reduce the number of displays on the bridge. The navigator needs to have important information easily available in order to reduce response time for decisions. Better integration will lead to a better bridge environment as well as a simpler installation.'}</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Interface and Compatibility', 'text': 'Interface to ECDIS/ECS and radar is provided via the Presentation Interface (PI) available on network or serial interface (RS-422). It is implicit that the system supports chart systems, AIS, and GNSS data distribution. The built-in web-based user interface (UI) provides an interface for configuration and status monitoring. Software updates are supported via the WEB UI and the USB interface will automatically detect new software when a USB stick is inserted. The update will be accomplished without interfering with the existing configuration. Kongsberg continuously makes the latest software available for download from their FTP server.'}</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'System Integration and Certificate Information', 'text': 'The AIS 300 is tested for EC Type-Examination (Module B) and holds a certificate under the Marine Equipment Directive (MED) 2014/90/EU. This certification remains valid unless suspended, expired, or withdrawn and is subject to the specified conditions. The product name is officially listed as AIS 300 under the AIS systems, and it meets the relevant technical requirements set by the notified bodies. The address and contact information for the manufacturer Kongsberg Seatex AS is included within the PDF file.'}</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1398,22 +1410,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS 300S is an AIS Unit built to support special operations. The AIS 300S utilises the AIS technology beyond standard AIS functionality and is a powerful tool for different maritime operations. It can be configured to output a set of virtual AIS objects that can describe an area of operation, dynamic and/or static. Such an area of operation can be the rectangle constituting the streamer area behind a seismic vessel or a safety area around an offshore operation. The implementation is based on relevant international standards.'}</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'AIS for Special Operations', 'text': 'In some operations the activity is below the surface, such as for operations involving remotely operated underwater vehicles (ROV) or seismic streamer operations. This constitutes an operational problem and there are risks related to some main issues: vessels coming in conflict with the operation and damage to vessels or equipment because of this, damage to underwater equipment in the operation area, and unwanted interference with the maritime operation and financial loss because of delays and mission abort. Even if all vessels are carrying standard AIS Class A equipment, AIS capabilities can be used to better support navigation in areas where special operations are taking place. Complex operations such as coordinated lifting or towing activity are also target applications for AIS 300S. An effective way to warn vessels in the Area Of Responsibility (AOR) about actual movements below the surface is by use of AIS.'}</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Tracking and Communication', 'text': 'The AIS 300S is delivered with a feature for transmission of automatic notifications. Area filters can be applied to the AIS data stream. If a vessel enters the area, an addressed user configurable text message will be transmitted to the vessel. The message can contain information about the on-going operation. The intention is to reduce the amount of VHF voice communication and release more time for the operators to focus on the operation. Information, such as the position of submerged objects, can be transferred to the AIS system and embedded in the AIS message used for virtual AIS transmission. Vessels receiving the transmissions will get a real-time update of underwater movements and use this information in coordinated activities or to avoid the moving structure.'}</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Operational Efficiency', 'text': 'By selecting the icon, more information will be available and the virtual AIS AtoN will hence be a carrier of information. Further, AIS can also be used as a data carrier for the distribution of important operational data such as weather data and mooring tension values. The AIS 300S employs advanced AIS technology to facilitate the efficient handling of special maritime operations, effectively contributing to the safety of life at sea and the seamless execution of underwater activities.'}</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1483,22 +1495,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS AQ610 is based upon the new generation AIS Base Station range from Kongsberg, designed in accordance with all relevant international standards including IEC 62320-1/-2 and ITU M-1371-5. It has a sensitivity better than -115 dBm and a 1U 19’’ rack mountable smooth design.'}</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized for Maritime Operations', 'text': 'The Kongsberg AIS AQ610 is specially designed for use in offshore maritime operations, such as wind energy and aquaculture farms. The AIS AQ610 receives and communicates AIS data from all AIS sources: AIS mobile stations, AIS base stations, AIS Aids to Navigation units, Search and Rescue (AIS SAR) units, and Man-over-Board (AIS MOB) units within the VHF coverage area. The AIS system has proven to be a valuable tool to increase the situation awareness and the efficiency of operations and safety.'}</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Sensitivity for Enhanced Reception', 'text': 'Kongsberg Seatex has also developed satellite based AIS receivers and this space-based AIS technology has strong focus on receiver sensitivity. The high sensitivity has been incorporated in the AIS AQ610. The increased sensitivity exceeds the requirements in international standards and regulations, and is an incredible enhancement in terms of signal reception.'}</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Special Functions and Remote Configuration', 'text': 'Special functions of the AIS AQ610 include electronic AIS marking of the real position of infrastructure, and virtual marking of the outer perimeter of the operational area. All vessels equipped with AIS will receive information indicating the area of operation of the aquaculture location. Integration with meteorological sensors for local distribution of weather data, local vessel AIS monitoring, and remote monitoring of vessel activity from the main control centre for logistic purposes are also featured. The AIS AQ610 has an Ethernet/LAN interface for easy interfacing with other equipment or data networks. From the AIS Central Monitor Application, a single AIS AQ610, or a network of these, can be remotely operated and maintained. The AIS AQ610 supports configuration and firmware update via a web interface.'}</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1569,22 +1581,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS BS600 is the fourth generation RoHS compatible AIS Base Station from Kongsberg Seatex with built-in storage capability, sensitivity better than -115 dBm, software defined radio (SDR) and a smooth design of a 2U 19” rack mountable platform. The BS600 is designed and tested in accordance with all relevant international standards including: IEC 62320-1 and ITU M-1371.'}</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Critical Component in AIS Networks', 'text': 'The AIS Base Station is the primary component in an AIS Hot stand-by Physical Shore Station (PSS), and therefore the most vital component in a coastal AIS network. The AIS BS600 receives and communicates AIS data from all AIS sources: AIS mobile stations, other AIS Base Stations, AIS Aids to Navigation units, Search and Rescue units etc, within the VHF coverage area. The AIS system provides a valuable tool to increase the situation awareness, the efficiency of operations and safety. Experience shows that the workload for operators involved in vessel tracking and monitoring is considerably decreased after the introduction of AIS.'}</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Sensitivity and Remote Capabilities', 'text': 'Kongsberg Seatex has also been developing satellite based AIS receivers and this space-based AIS technology has strong focus on receiver sensitivity. The high sensitivity has been incorporated in the AIS BS600. The increased sensitivity exceeds the requirements in international standards and regulations, and is an incredible enhancement in terms of signal reception. The AIS BS600 has several serial interfaces and an Ethernet/LAN interface, making it easy to interface the base station to other equipment or data networks. From the AIS Service Management Application Suite a single AIS BS600, or a network of base stations, can be remotely operated and maintained. The AIS BS600 supports configuration and firmware upgrade via a web interface.'}</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Efficient Deployment and DGNSS Correction Distribution', 'text': 'An integrated display and keyboard enables easy configuration of essential parameters. Detailed setup can be carried out via the web interface. The AIS BS600 is able to broadcast DGNSS corrections through the standardized AIS Msg 17. Hence, differential corrections can be transmitted to all vessels which carries an AIS mobile station if the vessel is located within the base stations coverage area. The AIS BS600 supports RTCM via serial and LAN interface.'}</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1652,22 +1664,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS BS610 is a product in the new generation AIS Base Station range from Kongsberg Seatex. It has a sensitivity better than -115 dBm and 1U 19’’ rack mountable smooth design. The AIS BS610 is designed and tested in accordance with all relevant international standards including IEC 62320-1 and ITU M-1371.'}</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Essential Component of AIS Network', 'text': 'The AIS Base Station is the primary component in an Hot stand-by AIS Physical Shore Station (PSS), and therefore the most vital component in a coastal AIS network. The AIS BS610 receives and communicates AIS data from all AIS sources: AIS mobile stations, other AIS Base Stations, AIS Aids to Navigation units, Search and Rescue units etc, within the VHF coverage area. In order to obtain a very high level of service and availability, a redundant base station configuration can be established. Two AIS BS610 units will operate autonomously in such a configuration when connecting them with a 0-modem cable and enabling the redundancy functionality. In case of an automatic change in redundancy status, the control centre will be notified.'}</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Sensitivity and Remote Operations', 'text': 'The AIS system provides a valuable tool to increase the situation awareness, the efficiency of operations and safety. Experience shows that the workload for operators involved in vessel tracking and monitoring is considerably reduced after the introduction of AIS. Kongsberg Seatex has also developed satellite based AIS receivers and this space-based AIS technology has strong focus on receiver sensitivity. The high sensitivity has been incorporated in the AIS BS610. The increased sensitivity exceeds the requirements in international standards and regulations, and is an incredible enhancement in terms of signal reception. The AIS BS610 has an Ethernet/LAN interface, making it easy to interface the base station to other equipment or data networks. From the AIS Central Monitor Application Suite a single AIS BS610, or a network of base stations, can be remotely operated and maintained. The AIS BS610 also supports configuration and firmware upgrade via a web interface. All base station functions can be configured and effectuated remotely via this interface.'}</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Transmission and Reception Capabilities', 'text': 'The AIS BS610 is able to broadcast DGNSS corrections through the standardized AIS message 17. Hence, differential corrections can be transmitted to all vessels which carry an AIS mobile station if the vessel is located within the base station’s coverage area. The AIS BS610 boosts its functionality with a VHF antenna and supports various power configurations and interfaces for operational flexibility. It also features RTCM v.2.3 support for reception of DGPS corrections on LAN, and can manage three remotely configurable receivers (TDMA/DSC). Other functionalities include USB interface for firmware upgrades, transmission of virtual AtoN, and AIS repeater functionality in accordance with IEC 62320-3. It also offers redundancy support and can support 10 parallel consecutive TCP connections.'}</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1739,22 +1751,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS RX610 is based upon the new generation AIS Base Station range from Kongsberg, designed and tested in accordance with all relevant international standards including IEC 62320-1 and ITU M-1371-5, where applicable. It has a sensitivity better than -115 dBm and 1U 19’’ rack mountable smooth design.'}</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Signal Reception', 'text': 'The Kongsberg AIS RX610 is an AIS receiver specially designed for optimal signal reception. It can receive from all AIS sources: AIS mobile stations, AIS base stations, AIS Aids to Navigation units, Search and Rescue (AIS SAR) units, and Man-over-Board (AIS MOB) units within the VHF coverage area. The AIS reception-only system has proven to be a valuable tool in increasing the situation awareness and the efficiency of operations and safety.'}</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Sensitivity', 'text': 'Kongsberg Seatex has developed satellite-based AIS receivers with a strong focus on receiver sensitivity. The high sensitivity has been incorporated into the AIS RX610, exceeding the requirements of international standards and regulations. This incredible enhancement in signal reception ensures that the AIS RX610 sets a new benchmark for sensitivity better than -115 dBm.'}</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Remote Accessibility &amp; Configuration', 'text': 'The AIS RX610 features an Ethernet/LAN interface, enabling easy interfacing with other equipment or data networks. With the AIS Central Monitor Application, a single unit or a network of AIS RX610s can be remotely operated and maintained. It supports configuration and firmware updates via a web interface, offering SNMP v.2, WEB interface for remote configuration and software update, three remotely configurable receivers (TDMA/DSC), and additional interfaces for maximum flexibility in operation.'}</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1815,22 +1827,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'AIS Physical Shore Stations can operate in a network in order to extend the AIS coverage area. The remote operation and maintenance of a network of AIS Base Stations is Internet Protocol (IP) based. The KONGSBERG AIS base stations have network interfaces and the AIS messages are sent to the centralized location (port center) for visualization in e.g. the AIS CM. The base station can use UDP Unicast, Multicast or TCP/IP. New AIS base stations can be added without additional SW license cost. The solution provides data directly to clients.'}</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'AIS Central Monitor (AIS CM)', 'text': 'The AIS CM is a utility developed in order to operate an AIS Base Station network including monitoring of all AIS vessels and AIS AtoN (Aid to Navigation) within range. The User Interface can utilize different types of electronic charts. The AIS CM is receiving a data stream of VDM messages (vessel data) received by AIS Base Stations connected to the network.'}</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Main functions', 'text': 'AIS Base Station management incl. status monitoring, alarm monitoring and configuration. Geographical displaying of AIS targets (Vessels, AIS Base Stations and AIS AtoN) as an electronic map overlay. A tabular listing of AIS targets incl. sorting and filtering functionality. AIS target detail window (Vessels, AIS Base Stations, AIS AtoNs).'}</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'User Interface', 'text': 'The User Interface will provide a seamless entry to other modules like data storage, data replay, addressed and broadcast message transmission, area definition tool etc.'}</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1877,22 +1889,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'BLUE INSIGHT - The digital ocean toolbox. Seamless data acquisition, fusion, processing, visualization, contextualization and management of ocean data. Kongsberg Blue Insight is an open and flexible digital infrastructure product designed to meet the increasing demand for accurate information from the oceans, focusing on internet security and seamless integration. The Blue Insight automates the data stream from a wide range of sensors and platform types and visualizes them in a common framework. The solution facilitates modern data processing and machine learning, providing new understanding and in-depth knowledge.'}</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Benefits of Blue Insight', 'text': 'Through a range of dedicated modules, Blue Insight offers flexibility, security and robustness required by any ocean data stakeholder: scientific, observational, or commercial. It is a one-stop solution that provides real time overview across platforms and data types; flexible and scalable, suitable for both small and large organizations; built on an open ecosystem adhering to FAIR data principles; allows for the deployment of customized machine learning algorithms; and is a cyber secure solution.'}</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Blue Insight Core', 'text': 'The Blue Insight Core module provides solutions for secure interactions between sensor platforms, cloud storage and data management enabled by the industrialized Internet of Things modules found in the Kognifai digital ecosystem. The Core module includes required common functionality to prepare the data for automated analytics and advanced data handling, with the full benefits of a modern, cyber secure cloud environment. It includes a basic visualization framework with dashboard functionalities and graph view of data. This module integrates with your existing information technology systems and is a requisite for deploying the other Blue Insight modules.'}</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Blue Insight Modules', 'text': 'Sensor Fusion is an on-board/on-premise application which receives and prepares data from selected sensors and onboard databases for streamlined distribution to the Blue Insight cloud. It provides the interface with Sensor Remote and Ocean View modules and optionally, real time visualization dashboard. The Data Forwarder module automates conversion of data into common formats for efficient data sharing across solutions and databases. Ocean View offers real-time and historic sensor data visualization in a map overlay. Analytics introduces in-depth data handling like quality assurance and AI-based automated data analysis, including remote deployment of algorithms.'}</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1940,22 +1952,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2013,22 +2025,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "APOS Survey - Surveyor's independent Operator Station for HiPAP, APOS Survey has been developed to provide a cost effective solution for subsea survey and construction operations, making it possible for the surveyor to utilise a vessel's HiPAP system. Acoustic interrogations are interleaved or run simultaneously with the DP system updates, without making changes to the vessel’s APOS software or installation parameters."}</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seamless Integration and Enhanced Flexibility', 'text': "APOS Survey offers full LBL and SSBL, quicker mobilisation times and is designed for both permanent and temporary installation on vessels. The software communicates directly with the HiPAP transceiver, enabling the surveyor to operate independently of the bridge. The software safely integrates into the vessels HiPAP system through a high speed, optically-isolated, serial connection to maintain independence from the vessel's Dynamic Positioning (DP) network, and removes restrictions normally associated with operating a HiPAP system for subsea survey purposes."}</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Operational Capabilities', 'text': 'The surveyor can interface local survey grade sensors, IMU, GYRO and GNNS, set up lever arms and load velocity profiles independently of the vessel, unlocking the full potential of HiPAP. The cPAP LBL transceiver for ROV positioning and portable HiPAP transceivers are easily interfaced, providing flexibility for a full range of operations. Both the vessels APOS and APOS Survey can compute position off the same SSBL transponders with independent calculation. HiPAP transducer alignment for both the vessel and APOS Survey system can be run simultaneously.'}</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Survey Functionality', 'text': 'APOS Survey OS version 6 or later allows to select which of the vessels HiPAP transducers are available for survey. The opto-isolated serial interface ensures a secure connection to the vessel’s HiPAP. It is possible to use vessels or local survey sensors such as GNSS MRU, Gyro. Configuration of lever arms and offsets are done independent of the ship. Moreover, the system includes Cymbal digital acoustics, capable of over 500 channels, and a variety of positioning modes including SSBL Fast Track, LBL, and Sparse LBL. Post-calibration and alignment functionalities such as SSBL Alignment and LBL boxin are also supported.'}</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2087,22 +2099,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Based on proven KONGSBERG technology, the AQUACULTURE MONITORING SYSTEM is a sophisticated tool designed for the aquaculture industry, which offers unique insight into environmental conditions, fish behavior, and welfare. This system encapsulates KONGSBERG’s comprehensive approach from sensor to cloud, ensuring safe and efficient operation and data handling.'}</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Functionality and Monitoring Capabilities', 'text': 'The AQUACULTURE MONITORING SYSTEM is equipped with an enhanced sensor suite for environmental monitoring and advanced echo sounders to observe fish distribution both vertically and horizontally. This setup allows for constant monitoring of fish behavior and distribution, integrating sensor data for real-time and historical analytics. It features an array of sensors including cameras, echo sounders, and tools to monitor feeding points, oxygen levels, temperature, water current profiles, salinity, and turbidity. Additionally, the system comes with secure cloud storage for data and is prepared for machine learning applications.'}</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'K-Fins Operation Support and System Benefits', 'text': 'KONGSBERG facilitates maximum situational awareness through the K-Fins operation support tool, which interprets and visualizes sensor data. The benefits include the ability to gain knowledge for optimizing overall operation, saving costs through precision feeding, strategically positioning underwater cameras, documenting fish behavior and welfare via automated analyses, and availing data interpretation support and advisory from Kongsberg domain experts. The operation support modules available are K-Fins Environment, K-Fins Feed, K-Fins Welfare, and K-Fins Birdseye, each focusing on specific areas of aquaculture operations.'}</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Cyber Security and Support', 'text': "Kongsberg ensures the security and integrity of the monitoring system through features like Kongsberg Edge Hardware and its Global Secure Network. The Edge Hardware is responsible for capturing sensor data with unique identity features that prevent device tampering, and all captured data is encrypted and transmitted to data centres securely. Additionally, the network is certified by DNV-GL and Bureau Veritas, reaffirming its reliability. Kongsberg's Global Customer Support operates 24/7, providing prompt responses, technical expertise, and global assistance."}</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2146,22 +2158,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'ASR x50 is the 4th generation SAT-AIS receiver from Kongsberg and part of the extended lifetime product series. The receiver is a reconfigurable SDR based receiver, designed to support simultaneous on-board AIS decoding and digital sampling. ASR x50 has, through new enhanced algorithms, multi-antenna support and superior dynamic range, an improved end-to-end performance. It is designed for a 7+ year lifetime and takes vessel detection via AIS to the next level.'}</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative technology', 'text': 'This generation SAT-AIS receiver from Kongsberg is the latest achievement of years of continuous innovations resulting in highest decoder performance, multi-antenna support, built-in redundancy, low power, miniaturized housing, large mass memory, and improved lifetime. The end-to-end performance exceeds existing SAT-AIS receivers, where the superior sensitivity of the ASR x50 makes the receiver capable of detecting even AIS class B vessels. Reconfigurable software-defined radio (SDR) technology is used, enabling support for future enhancements in algorithms or changes in AIS/VDES standards.'}</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Vessel detection performance to the next level', 'text': 'Kongsberg started working with AIS twenty years ago and is the AIS equipment manufacturer with the broadest experience. ASR x50 is Kongsberg’s 4th generation AIS Space Receiver and builds on this foundation of expertise. A multiple set of decollision algorithms is optimised for best possible vessel detection in high-density and medium-density areas. ASR x50 will give the end user a giant leap in vessel detection compared with existing SAT-AIS receivers.'}</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Space grade using latest technologies', 'text': 'The extended lifetime series from Kongsberg is designed for a lifetime of 7+ years in LEO. ASR x50 uses the latest generation EEE parts from best-in-class manufacturers. This enables Kongsberg to design for leading capabilities at low power and miniature size. All EEE parts have been carefully selected and extensively tested. Active components have been subject to heavy ion, proton, and Co-60 test campaigns to ensure radiation-tolerant design.'}</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2238,22 +2250,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HUGIN Edge is a next generation mid-size Autonomous Underwater Vehicle to join the HUGIN Family. Exceptional reliability, durability and performance has been drawn from the HUGIN, coupling ease of operations from uncrewed surface vessels to the most advanced AUV features on the market. Capabilities include truly autonomous missions making the system an optimal choice in applications from commercial survey to advanced defence operations.'}</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Unique in Design', 'text': 'The smallest most lightweight member of the HUGIN family, a fresh low drag body at four metres in length using a wet flooded carbon monocoque design, unique in its class. It allows low logistics without compromise on sensor performance. The vehicle combines the latest advances in autonomy and operability with the exceptional navigation performance for which the HUGIN family is renowned. HUGIN Edge collects high resolution data without the need for in-mission supervision. No other vehicle provides this performance in this form factor.'}</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Autonomous by Design', 'text': 'The HUGIN Edge solution is autonomous by design. That means that all parts of the system have been designed with full autonomy and remote operations in mind, all the way from autonomous launch and recovery, through to uncrewed charging and data offloading. Equally at home working from shore or over the horizon the HUGIN EDGE is always flexible and can be delivered with USV or uncrewed launch and recovery systems maximizing operational cycles. The goal-based mission planning employs Artificial Intelligence where missions are organized based on objectives rather than long lists of waypoints. EDGE takes full advantage of all any priori knowledge to plan and then using integrated on-board sensors adapts in mission to the most optimal solution removing human dependency.'}</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Payloads for All Scenarios', 'text': 'HUGIN Edge is equipped with side-scan sonar or next generation synthetic aperture sonar (upgradeable) for ultra high-resolution imagery and bathymetry. This combination provides the highest area coverage and performance from any AUV in this class. With an ultra high-frequency multi-beam echo sounder providing clean, interference free, wide-swath bathymetry along with a magnetometer for precise magnetic mapping. A flexible Payload Bay enables interchangeable options on low-light colour camera solutions (including strobe light) or sub-bottom profilers allowing tracking and classification, or geological work.'}</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2297,22 +2309,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'HUGIN Endurance is the newest member of the HUGIN AUV family and enables unsupervised shore-to-shore operations over long ranges. HUGIN Endurance can be configured with a range of sensors focused on mission capabilities and situational awareness. This includes the proven hydro-acoustic instruments for mapping and inspection purposes, such as the KONGSBERG HISAS family of synthetic aperture sonars and the EM family of multibeams. Both underwater and surface awareness sensors are used for autonomous decision making.'}</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Operational Capabilities', 'text': 'HUGIN Endurance collects consistent, high-resolution data without the need for in-mission supervision using KONGSBERG’s advanced underwater navigation system Sunstone. This advanced level of autonomy and accuracy reduces the carbon footprint of survey operations by eliminating the need for a dedicated support vessel. Consequently, it mitigates health and safety concerns by relocating personnel onshore and allows the largest potential weather window for any operation.'}</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Product Evolution', 'text': 'With continuous evolution from 1991, and commercial surveys starting in 1997, HUGIN has seen consistent advancements. KONGSBERG and our partners at the Norwegian Defense Research Establishment (FFI) have significantly contributed to underwater robotic technology. The new HUGIN Endurance capitalizes on 30 years of expertise to offer the most capable commercial solution within the large-diameter AUV segment.'}</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Autonomy and Data Integration', 'text': 'HUGIN Endurance is a truly autonomous system designed to operate for extended periods without human intervention. With state-of-the-art technology such as the latest generation pressure-tolerant Li-Ion batteries, sensor redundancy, in-mission processing, and Sunstone inertial navigation system with HISAS micronavigation, HUGIN Endurance exceeds commercial offerings for high-quality data collection. Equipped to handle unpredictable events, switch to redundant operation modes, and communicate securely with remote operating centers, HUGIN Endurance represents a leap in shore-to-shore operations for commercial surveying.'}</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2356,22 +2368,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2500,22 +2512,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'AVR 100 is a recording system for offshore helicopter operations, logging radio communication between helicopter- and helideck crew, as well as video recordings of the helideck, for 30 days. The AVR is an add-on to the Helideck Monitoring System (HMS), enabling the HMS to be compliant to BSL D5-1 §40 and §41 requirements.'}</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Recording Features', 'text': 'The AVR 100 provides state-of-the-art solutions to store and manage helideck operation data with its combined audio-visual recording functionalities. It ensures that pertinent information such as communication between the helicopter and helideck crew is securely logged while capturing high-resolution video footage of the helideck activities. With a storage capacity of 2 TB, the system maintains an extensive history of 30 days, all made accessible through user-friendly data retrieval options such as a USB graphical interface or SFTP.'}</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Quality Video Standards', 'text': 'Equipped with the capability to accept input signals via SDI or RTSP, the AVR 100 makes no compromises on video quality. The system supports a diverse range of resolutions up to Full HD 1920 x 1080, with aspect ratios of 16:9 or 4:3 to capture comprehensive views of the helideck. Ensuring smooth playback, it operates with framerates between 15 to 30 fps and maintains a versatile bitrate range of 500 – 6000 kbps while leveraging the efficient h.264 codec.'}</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliable Audio Integration', 'text': 'Not only does the AVR 100 handle video with utmost proficiency, but it also integrates high-quality audio recording using an Opus codec. With two available channels for stereo recording, the system offers a wide bitrate selection ranging from 6 to 510 kbps and sample rates from 8 to 48 kHz. This flexibility in audio settings ensures that communication clarity is never compromised during offshore helicopter operations.'}</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2570,22 +2582,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The AIS 300BF is an enhanced version of the type approved AIS 300 class A mobile station, which also offers secure communication in addition to standard AIS functionality. In secure mode the AIS 300BF will still be able to detect all AIS mobile stations in its coverage area but it will not reveal its own position to any other than friendly forces.'}</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Integration for Heightened Security', 'text': 'Blue Force (BF) is a common term for own units or friendly forces. The AIS 300BF, being the 3rd generation secure AIS mobile from Kongsberg, is designed for seamless integration with navigation equipment such as ECDIS and radar. It boasts an improved receiver sensitivity, offering an increased range over standard units. The unique operational modes of the AIS 300BF cater to varying levels of security requirements, with the ability to switch from a standard AIS class A mobile station to a secure mode that encrypts transmitted AIS data for exclusive visibility to Blue Force units.'}</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Connectivity and User Interface', 'text': 'Ease of installation and maintenance is a hallmark of the AIS 300BF, equipped with a bracket for strain relief and a user-friendly built-in WEB user interface for straightforward configuration. Offering a hassle-free software upgrade process through the WEB UI and USB interface, Kongsberg ensures that the AIS 300BF remains updated with the latest software available via download from a Kongsberg-hosted FTP server.'}</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Comprehensive Navigation Interfaces', 'text': 'The AIS 300BF goes beyond standard functionality with a focus on integration and improved reliability of received navigation data from other vessels. Interfaces for ECDIS and radar are provided through the Presentation Interface, allowing for easy decryption and internal encryption. These capabilities ensure that AIS target information, such as position, heading, course, and speed are readily available to mariners, enhancing situational awareness and maritime safety.'}</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2649,22 +2661,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Kongsberg Blue Insight is an open and flexible digital infrastructure product designed to meet the increasing demand for accurate information from the oceans, focusing on internet security and seamless integration. The Blue Insight automates the data stream from a wide range of sensors and platform types and visualizes them in a common framework. The solution facilitates modern data processing and machine learning, providing new understanding and in-depth knowledge.'}</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Benefits', 'text': 'Blue Insight offers a range of dedicated modules, ensuring flexibility, security, and robustness necessary for meeting the needs of every ocean data stakeholder, be it scientific, observational, or commercial. It stands as a one-stop solution providing real-time overview across platforms and data types, scalable to accommodate both small and large organizations. Blue Insight is built on an open ecosystem guided by FAIR data principles, facilitates the deployment of customized machine learning algorithms, and boosts cyber security.'}</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Blue Insight Core', 'text': 'The Blue Insight Core module provides solutions for secure interactions between sensor platforms, cloud storage, and data management, leveraging the Kognifai digital ecosystem. It includes requisite common functionality essential for automated analytics and advanced data handling, capitalizing on a modern, cyber secure cloud environment. With its basic visualization framework, it integrates seamlessly with existing IT systems and serves as the foundation for other Blue Insight modules.'}</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Module Overview', 'text': 'Blue Insight encompasses a suite of modules such as Sensor Fusion, which prepares sensor data for cloud distribution, and the Data Forwarder module, ensuring efficient and seamless data sharing across various platforms. Remote control via the Sensor Remote module and real-time visualization within the Ocean View module are also integral parts, facilitating data oversight and management. The Analytics module, at its core, utilizes machine learning to process ocean data, enabling automated analysis and quality assurance for more profound data insights.'}</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2712,22 +2724,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cNODE Modem Embed electronics board, together with a transducer and external power, functions as a modem and transponder. Designed for integration into custom subsea housings the transponder is fully compatible with HiPAP, cPAP and µPAP positioning systems.'}</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seamless Integration and Performance', 'text': 'The cNODE Modem Embed provides flexibility to integrate KONGSBERG modem electronics into a custom pressure housing. This provides advantages to reduce size, weight and the need for subsea interface cabling. The same SSBL, LBL and telemetry capability is featured on the board as per a standard cNODE providing the same performance when positioning the modem with any HiPAP SSBL or cPAP LBL system.'}</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatility in Acoustic Navigation and Positioning', 'text': 'A variety of flush mount and remote transducers are available, to provide optimal performance in shallow, deep water or horizontal modem and positioning applications for AUVs, ROVs, gliders, towed fish or nodes. Operating in the Medium Frequency 20khz to 30Khz band, both FSK and Kongsberg Cymbal navigation codes are available. Cymbal wideband offers 560 unique navigation codes and range accuracies of better than 2cm, are achievable.'}</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Communication Protocol', 'text': "The modem utilizes Cymbal acoustic protocol, which incorporates wideband codes (560+) and HPR 400 (FSK) channels within a 21 – 31 kHz band. It's capable of fulfilling both responder and transponder functions, providing telemetry for sensor and LBL data. It supports SSBL as well as LBL positioning modes and interfaces with a variety of transducers. An internal tilt sensor enables precise and versatile functionality."}</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2800,22 +2812,22 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'cNODE Modem Explorer is designed for integration onto AUVs, ROVs or other vehicles where space and weight are restricted. The cNODE electronics can be supplied in a pressure rated underwater housing or in compact lightweight non pressure rated housing for full third party integration.'}</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Integration and Compatibility', 'text': 'cNODE Modem Explorer is a compact transponder and modem fully compatible with HiPAP, cPAP and μPAP underwater positioning systems. Both Low Frequency and Medium Frequency models are available. cNODE Modem Explorer interfaces to the subsea vehicle via a serial interface to transfer modem data. The transparent modem capability allows commands and data to be transmitted to and from the subsea vehicle from the customers topside control system, via the vessels HiPAP system.'}</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Positioning and Telemetry', 'text': 'cNODE Modem Explorer may be connected with up to three remote transducers. The transducers may be selected and switched electronically by the subsea vehicle control system or acoustically, to optimize for example vertical or horizontal telemetry and positioning performance. The modem use Cymbal acoustic protocol.'}</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Transducer Options and Specifications', 'text': 'cNODE Modem Explorer provides various transducer options including MODEL TDR30H for MF, TDR180 for MF, TDR30V for MF, TDR40V for MF, TDR180 for LF, and TDR50V LF. Each transducer model has specific part numbers and characteristics such as beam width, depth rating, and material composition. Not all transducer models are shown please contact your local Kongsberg representative for more information. Specifications subject to change without any further notice.'}</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2884,22 +2896,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cNODE Mantis can work as ‘a second set of eyes’ in underwater operations. The live video is streamed from the camera unit to a receiver installed either on the ROV’s TMS (Tether Management System) or on the vessel itself, at ranges of up to 500 m. Data can also be transmitted from a Mantis transmitter on AUV to a surface vessel or USV.'}</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Performance Video Streaming', 'text': 'Video stream with up to 4 frames per second leverages a high-speed acoustic link. This allows the cNODE Mantis to function in both murky and clear water conditions unaffected by background light. Transmitter uses a typical composite video camera while delivering quality of 420 x 380 pixels at four frames per second with a bitrate of up to 70 kbit/s. The receiver interfaces via ethernet, and sensor data and status from the camera unit are interleaved with the video stream.'}</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Interface and Viewer Application', 'text': 'The received video stream, status, and sensor data is displayed in the supplied Mantis Viewer Windows application. The video stream can be recorded and redirected to other users over an ethernet connection as a RTP stream. This capability ensures versatility in the use and management of the streamed underwater video footage.'}</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Control and Depth Capability', 'text': 'The cNODE Mantis transmitter is controlled via a high-speed command link and has a depth rating of up to 800 m. With a 30° directional transducer beam and an operating frequency of 200 kHz, the cNODE Mantis is designed to maintain reliable communication and control of the camera unit, thus enhancing its performance in a variety of underwater environments.'}</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2970,22 +2982,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cNODE Modem MiniS is designed for the Point 2 Point transfer of data between two cNODE’s or to a surface vessel equipped with any HiPAP and µPAP systems. The data telemetry operates on CYMBAL digital protocols, Kongsberg field proven robust proprietary link. One cNODE Modem MiniS can address several other cNODE Modems during operation using the Kongsberg Link User Protocol. The data telemetry operates on CYMBAL, Kongsberg’s field proven and robust proprietary link. Data rates of up to 6 kb/s are available. The cNODE Modem MiniS is simple to configure with the TTC Light software.'}</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Data Telemetry and Configuration', 'text': 'The cNODE Modem MiniS enables high speed telemetry capabilities with clear communication facilitated through the robust CYMBAL digital protocols. Rated for 4000 meter depths, it features an anodized aluminium housing and offers different transducer options, including an omnidirectional and a narrow beam transducer suitable for varying operational environments. The simplicity of its configuration using TTC Light software ensures ease of use for various applications.'}</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Design and Functionality', 'text': 'With a transparent Modem function and internal rechargeable Li-Ion battery, the cNODE Modem MiniS is crafted for efficient field operations. It provides functionalities such as SSBL and LBL positioning, range measurements between transponders and an internal tilt sensor. This equipment secure operation with its integrated features, like the fast battery charger, pressure relief valve, and external on/off functions, enhancing its performance in diverse underwater conditions.'}</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence', 'text': 'Built for demanding underwater environments, the device is equipped with capabilities like RS-232/485/422 modem interface, multiple CYMBAL channels, and a frequency band of 21-31 kHz. The cNODE Modem MiniS showcases operational adaptability with its range of features including a pressure relief valve and temperature range adaptability, cementing its operational excellence in telemetry and positioning applications.'}</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -3046,22 +3058,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cNODE Embed electronics board, together with a transducer and external power, functions as a transponder. Designed for integration into custom subsea housings the transponder is fully compatible with HiPAP, cPAP and µPAP positioning systems. The cNODE Embed provides flexibility to integrate KONGSBERG transponder electronics into a custom pressure housing. This provides advantages to reduce size, weight and the need for subsea interface cabling.'}</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Custom Integration and Broad Compatibility', 'text': 'A variety of flush mount and remote transducers are available, to provide optimal performance in shallow, deep water or horizontal positioning applications for AUVs, ROVs, gliders, towed fish or nodes. Operating in the Medium Frequency 20khz to 30Khz band, both FSK and Kongsberg Cymbal navigation codes are available. Cymbal wideband offers 560 unique navigation codes and range accuracies of better than 2cm, are achievable.'}</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Positioning and Navigation Capabilities', 'text': 'The same SSBL, LBL and telemetry capability is featured on the KONGSBERG transponder electronics board as per a standard cNODE providing the same performance when positioning the transponder with any HiPAP SSBL or cPAP LBL system. The cNODE Embed 33-80V brings versatile functionality in a form designed for seamless integration with various subsea platforms.'}</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3127,22 +3139,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'cNODE is a family of transponders for underwater acoustic positioning and data link, and operates with both HiPAP, HPR and cPAP transceivers. The cNODE transponders operates with either the HiPAP/HPR 400 channels and telemetry or with the new Cymbal acoustic protocol. The cNODE Maxi 31 Exd transponders are made especially for operating in an explosive atmosphere.'}</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Explosive Atmosphere Compliance', 'text': 'The cNODE Maxi 31 Exd transponders comply with several important standards, making them ideal for operations in environments classified as explosive atmospheres. These standards include IEC/EX 60079-1:2007, IEC 60079-0:2011, IEC 60086-1, and EN 60079-0:2012. Two models are available for use in such conditions: the cNODE Maxi 31-80V-90-Exd and the cNODE Maxi 31-80V-Exd.'}</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable Materials and Operational Depth', 'text': 'The construction of cNODE Maxi 31 Exd transponders involves robust materials, ensuring durability and reliability under extreme underwater conditions. Bolts and tube are made from Super Duplex stainless steel, and the transducer, top end cap, and bottom end cap consist of Titanium grade 5. These transponders have an impressive operating depth limit of 1000 meters, matching the demanding requirements of underwater operations.'}</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Communication and Environmental Specifications', 'text': 'To facilitate effective underwater communication, cNODE Maxi 31 Exd transponders use Phase Shift Keying (Cymbal) and Frequency Shift Keying (FSK) principles. The units are designed to withstand a temperature range from -5°C to +55°C during operations and can be safely stored within a temperature range from -30°C to +70°C. These environmental specifications ensure that the transponders can function in a variety of underwater climates and conditions.'}</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3186,22 +3198,22 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -3251,22 +3263,22 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'cNODE is a family of transponders for underwater acoustic positioning and data link, which operates with HiPAP, HPR and cPAP transceivers. The medium frequency (MF) cNODE family is distinguished by a variety of types, including cNODE Maxi and cNODE Midi - both rated for medium frequency operations at depths of up to 4000 meters. These types are described in separate product specification sheets. The cNODE transponders serve a modular design suited for a broad range of applications, benefitting from multiple transducer options, internal and external sensors, and different housing materials.'}</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Modular and Versatile Design', 'text': 'The cNODE design stands out for its modularity, offering a vast range of applications through its array of transducers, internal and external sensors, housing materials and various add-on functions. The convenience of its design is further highlighted by the ability to add new configurations and update software easily from the Transponder Test and Configuration unit (TTC30) without having to open the transponder. Moreover, its floating collar and release design simplify the launch and recovery operations, ensuring safety and ease.'}</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence and Compatibility', 'text': 'cNODE transponders seamlessly operate with both the HiPAP/HPR 400 channels and telemetry or the new Cymbal acoustic protocol. They encompass a range of functionalities such as acoustic data link for command and data transfer, transponder and responder operations, and compatibility with different acoustic protocols and positioning systems. Notably, the internal tilt sensor in the cNODE provides a significant accuracy level, and safety devices such as the pressure relief valve and vent screw are incorporated into the design. An external connector facilitates the configuration and software updates, demonstrating the operational excellence and versatility of cNODE transponders.'}</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Positioning and Measurement Capabilities', 'text': "cNODE transponders are not only designed for SSBL and LBL positioning but also excel in range measurements between transponders, offering a remarkable standard deviation and accuracy. These advanced positioning and measurement capabilities assert cNODE's role in precision underwater navigation. Additionally, the integration of high-accuracy sensors in the Top section module, the possibility of replacing individual components, and the wide selection of transducers emphasize the advanced technological aspects and adaptability of these transceivers."}</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3338,22 +3350,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cNODE Micro transponder is rated to 600 metres and is small and light enough to be used by divers and shallow water ROV’s. Operating on Kongsberg Cymbal digital acoustic protocols, the cNODE Micro provides the optimal positioning performance with the Kongsberg range of SSBL systems, from µPAP through to HiPAP.'}</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexibility and Precision', 'text': 'The cNODE Micro is extremely flexible featuring Cymbal digital telemetry and both SSBL &amp; Long Baseline positioning capabilities. With range accuracies of better than 2 cm achievable, measured baselines between transponders on the seabed provide capabilities for simple diver metrology or archeology.'}</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Functionality', 'text': 'The telemetry capability allows the battery status to be read during operation and the integrated tilt sensor can be turned on and off with positioning updates. Multiple cNODE Micro transponders can be interrogated simultaneously in SSBL positioning mode using the µPAP and HiPAP Fast track feature to ensure the fastest possible updates during operation.'}</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Features', 'text': 'Some common features of the cNODE Micro include: Coated Anodised aluminium housing, Cymbal channels (500+), Internal rechargeable Li-Ion battery, Acoustic telemetry for battery status and tilt sensor, Responder and transponder functionalities, SSBL positioning, LBL positioning, Range measurements between transponders, 600 metre depth rated, 180º omnidirectional beam, frequency band 21-31 kHz, and operating temperature -5 ºC to +55 ºC.'}</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -3421,22 +3433,22 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'cNODE is a family of transponders for underwater acoustic positioning and data link and operates with both HiPAP, HPR and cPAP transceivers. cNODE operates with either the HiPAP/HPR 400 channels and telemetry or with the new Cymbal acoustic protocol. The Medium frequency (MF) cNODE family consists of the following types, each with a separate product specification sheet: \n\n• cNODE Maxi and cNODE Midi (Medium frequency, 4000 m)\n• cNODE Mini (Medium frequency, 4000 m)'}</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Modular and Flexible Design', 'text': 'The cNODE design is very modular and covers a large range of applications with its variety of different transducers, internal and external sensors, housing materials and other add-on functions. Both new configurations and software can easily be downloaded from the Transponder Test and Configuration unit (TTC30) without opening the transponder. The floating collar design makes the launch/recovery operation safe and easy. Spare parts for cNODE are based on the main modules with a housing rated for 4000m manufactured in coated anodized aluminium. Transducer options include an 180 degree omni directional and 40 degree vertical transducer to ensure the link can be optimized based on water depth and environment.'}</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Performance and Compatibility', 'text': "Offering both transponder and responder functions, the cNODE Mini's compatibility with the Cymbal acoustic protocol and HiPAP/HPR 400 channels showcases its versatility in underwater positioning and data link. Features like internal tilt sensor accuracy, pressure relief valve, vent screw, and external connector for configurations enhance its functionality. Additionally, it supports SSBL and LBL positioning, acoustic data link for command and data transfer, and precise range measurement between transponders for impactful and reliable performance."}</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'System Overview - Mini Models', 'text': 'The Mini Models within the cNODE series come with specific features that denote their capabilities. For instance, the cNODE Mini 34-180-St indicates a 30 kHz operating band, a 4000m depth rating, a 180° transducer beam width, and all modules made of stainless steel. Common features for all Mini Models include a 4000m depth rating, operating temperatures ranging from -5°C to +55°C, and options for either aluminum or stainless steel construction. The array of models and transducers along with their corresponding beam widths, sensitivities, and source levels accommodate various environmental demands and preferences.'}</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3539,22 +3551,22 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Kongsberg Maritime’s cNODE MiniS Transponder comes with an impressive array of features, designed to meet the versatile demands of underwater acoustic positioning and data telemetry. The cNODE MiniS Transponders are equipped to handle 560+ Cymbal digital acoustic channels and FSK B channels, making them suitable for diverse marine applications. Available with pressure-rated housings of 4000 m and 7000 m, along with various transducer options, this robust equipment is tailored for use in deep-sea environments.'}</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Positioning and Data Transmission', 'text': 'The cNODE MiniS Transponders are paramount for precise positioning, most significantly observed when positioning a Work Class Remotely Operated Vehicle (WROV) or Towfish in SSBL mode. The technology allows for flexible operational modes, accommodating noisy vehicles through a responder mode for quicker positional updates. Moreover, with the integration of an internal tilt sensor, the transponders provide comprehensive data by transmitting both the position and attitude of the tracked targets simultaneously without the need for additional telemetry equipment.'}</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Functionality', 'text': 'Alongside high versatility in positioning modes, the cNODE MiniS offers full Long Baseline (LBL) capability, meaning it can accurately measure baselines, become an integral part of an LBL array, or be tracked as an LBL target transponder. Configuration of the transponder is effortless, either via RS232 line or acoustically through telemetry channels. Maintaining compatibility is vital, thus the cNODE MiniS fully supports Kongsberg’s HiPAP, µPAP, and cPAP positioning systems, ensuring precise ranging and secure underwater communication.'}</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliable and Convenient Design', 'text': "Kongsberg ensures that the practical aspects of the cNODE MiniS are as formidable as its technical capabilities. The compact housing of the cNODE MiniS3x ensures that it remains unintrusive in operation, accompanied by a Li-Ion rechargeable battery for extended duration missions. Additionally, it can be alternatively powered by an external supply, providing flexibility depending on the mission's requirements. With an operability at depths of up to 7000 m, it stands as a reliable choice for various underwater applications."}</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3600,22 +3612,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Combi 50/200 D combines two transducers and one temperature sensor in a single housing. It is designed with a streamlined shape for hull mounting on small vessels.'}</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Common Specifications and Performance', 'text': 'The nominal impedance of the transducer is 75 ohms, with a maximum pulse power input of 1000 W and a continuous power input of 10 W. It has a receiving sensitivity with an open circuit of -179 dB re 1V per µPa and an electroacoustic efficiency of 0.50. The resistance NYC thermistor at 25°C is 10 kohm, and the transducer can be submerged to a maximum depth of 20 m. With a cable length of 15 m and diameter of 10.6 ±0.5 mm, the weight with cable is around 8 kg. The device also has a specified storage temperature range from -20 to 70°C.'}</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': '200 kHz Technical Specifications', 'text': 'At 200 kHz, the transducer has a resonant frequency of 200 kHz, with a beamwidth longitudinal of 7 degrees and transverse of 7 degrees. The directivity (DI=10logD) is 28.5 dB, and side lobes are less than -18 dB with back radiation being less than -30 dB. The source level at 1000 W power is 227 dB re 1µPa, and the transmitting response is 178 dB re 1µPa per V. Its receiving sensitivity at an open circuit is -185 dB re 1V per µPa with an electroacoustic efficiency of 0.60.'}</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': '50 kHz Technical Specifications', 'text': "Operating at 50 kHz, the transducer's resonant frequency is set at 50 kHz, with a beamwidth longitudinal of 10 degrees and a transverse beamwidth of 16 degrees. It possesses a directivity (DI=10logD) of 23 dB. Side lobes and back radiation are less than -15 dB and -25 dB respectively. The source level is capable of reaching 221 dB re 1µPa when transmitting at 1000 W and the transmitting response equals 172 dB re 1µPa per V."}</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -3675,22 +3687,22 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Kongsberg Blue Insight is an open and flexible digital infrastructure product designed to meet the increasing demand for accurate information from the oceans, focusing on internet security and seamless integration. The Blue Insight automates the data stream from a wide range of sensors and platform types and visualizes them in a common framework. The solution facilitates modern data processing and machine learning, providing new understanding and in-depth knowledge.'}</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Benefits', 'text': 'Blue Insight delivers a suite of advantages to its users, emerging as a one-stop solution that provides real-time overview across platforms and data types. It is flexible and scalable, making it suitable for both small and large organizations. Built on an open ecosystem adhering to FAIR data principles, the product allows for the deployment of customized machine learning algorithms. It stands out as a cyber secure solution, ensuring data integrity and protection.'}</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'BLUE INSIGHT CORE', 'text': 'The Blue Insight Core module ensures secure interactions between sensor platforms, cloud storage, and data management. This foundation is enabled by industrialized Internet of Things modules found in the Kognifai digital ecosystem. It encompasses common functionalities required for automated analytics and advanced data handling, while providing benefits of a contemporary, cyber secure cloud environment, complete with basic visualization framework, dashboard functionalities, and data graph views.'}</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Analytics and Sensor Integration', 'text': 'The Analytics module affords more in-depth data handling capabilities including quality assurance steps or automated data analysis based on artificial intelligence. It provides an infrastructure for both onboard and cloud-based machine learning from ocean data to, for instance, enable automated classification of echo sounder data. Concurrently, the Sensor Fusion Data Forwarder and Sensor Remote modules harmonize and facilitate data sharing and sensor control for interconnected and streamlined operations.'}</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3734,22 +3746,22 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The cPAP MK II subsea transceiver is specifically designed for the precision positioning of ROVs and other underwater vehicles in both subsea long baseline (LBL) and Sparse LBL array configurations. Utilizing the advanced Kongsberg Cymbal wideband acoustic protocol, the cPAP MK II delivers centimetric accuracy for ranges and high data rates for telemetry purposes.'}</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Power and User Control', 'text': "Boasting a rechargeable battery pack, the cPAP MK II reduces the peak current drawn from the external power supply, which also acts as an uninterruptible power supply for the transceiver in case of external voltage disruption. This ensures continuous, reliable operation. Accommodating user control, the unit is compatible with Kongsberg's APOS navigation software for comprehensive LBL functionality as well as third-party control through a dedicated NMEA command port."}</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durability and Construction', 'text': 'The cPAP MK II is built robustly to withstand the pressures of the deep ocean, with depth ratings of 4000 m and 6000 m. The 6000 m variant is constructed with titanium, and its transducers from stainless steel, to ensure longevity and resistance to corrosion whereas the 4000 m variant features an aluminum housing, providing a lightweight solution without compromising on strength or functionality.'}</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'External Housing and Transducers', 'text': "cPAP MK II is accommodated in a housing dimensioned at 279 x Ø 79 mm, with weight differentials when in air or submerged. The transducers, essential for the accurate underwater communications, come in different models – TDR180, TDR40V, and TDR30H, each with respective beam patterns and source levels to cater to a range of operational requirements. This diversity in transducer specifications underscores the transceiver's adaptability to various subsea missions."}</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -3793,22 +3805,22 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Please format this text using the same words and language as the text. Do not change the text too much, and do not add information that is not there.'}</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3919,22 +3931,22 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The CUBELINE AIS space receiver series is an innovative software-defined radio optimized for reception of AIS and ASM signals in LEO orbit. The AIS receiver is specially designed for the CubeSat segment. ASR c50 is ideal for small- and nanosat missions, where KONGSBERG’s successful heritage on high quality and leading performance is maintained.'}</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Space grade using latest technologies', 'text': 'The ASR c50 is designed for use in LEO. Product assurance methods used for our extended lifetime product series are refined to reduce mission risks. The latest technologies are embedded, providing a high level of on-board processing power for using KONGSBERG’s renowned AIS and ASM decoding algorithms.'}</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible solutions', 'text': "ASR c50 is designed to embed the function to do both on-board processing as well as digital sampling for post processing. In addition, the receiver has a built-in RF spectrum analyzer. This spectrum analyzer functionality is an excellent tool during the test phase of the satellite and commissioning. Noise components from the platform or other payloads might be detected at an early stage using the receiver's spectrum analyzer functionality."}</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Continuous innovations', 'text': 'The ASR c50 is unique by its excellent performance in a CubeSat housing. KONGSBERG has delivered AIS equipment for almost two decades and has more than 60 years of accumulated in-orbit LEO heritage. The CUBELINE AIS space receiver series now embeds all AIS bands available as well as reception of the new Application Specific Message (ASM) protocol. The receiver also supports a separate antenna port that can be adapted for applications in the frequency band 100 to 6000 MHz.'}</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -3980,22 +3992,22 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -4039,22 +4051,22 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DARPS 232 is a DP position reference system tailor made for offshore loading operations. The DARPS system combines high performance sensors for reliable and accurate absolute and relative positioning of two vessels such as a shuttle tanker and a FPSO/FSU.'}</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Positioning Capabilities', 'text': 'DARPS 232 is a GPS/GLONASS based system which uses simultaneously gathered GPS/GLONASS data from high performance sensors on remote and own vessel to compute distance to target (DT) and bearing to target (BT). The system is capable of providing relative position with a worldwide accuracy of 20 cm and is independent of differential correction data. For computation of absolute position, differential corrections are used achieving a global accuracy of 20 cm in High Precision mode utilising commercial subscription services. Moreover, the DARPS system also utilizes free-to-air SBAS correction signals like WAAS, EGNOS, and MSAS, available at no additional cost.'}</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Communication and Compensation', 'text': 'Data between the two DARPS systems is communicated by UHF high performance transceivers operating in multiple bands. The use of a TDMA protocol enables efficient two-way communication, providing flexibility and reliability even in areas with dense radio activity. Additionally, the system includes a built-in lever arm compensation feature, which allows for the selection of numerous measurement points across the vessel to correct loading and offloading points on both the shuttle tanker and the FPSO/FSU. This feature relies on heading input to ensure accurate distance calculations during relative position mode operation.'}</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence and Diagnostics', 'text': 'A new operator software has been developed alongside DP operators for the next-generation DARPS system, enabling real-time situational awareness and quick, effective responses to critical situations. For maintenance and troubleshooting, DARPS offers graphical views for simple on-board system diagnostics. System data are automatically logged, and an export tool is provided for easy data transfer to USB media. A verification tool also exists for the DARPS UHF radios to reduce the risk of costly downtime by confirming system correctness prior to offshore operations.'}</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -4154,22 +4166,22 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'KONGSBERG TELEMETRY SYSTEM, Kongsberg Telemetry system is based on dual (fault tolerant) SeaGnal MB45 controller units with built-in UHF transceivers for safe and reliable ‘Green-line’ control in offloading operations.'}</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhancing Offloading Operations', 'text': 'Kongsberg Telemetry system enhances control and safety during offloading operations by providing real-time ‘green-line’ offloading control activated manually or automatic. A built-in mechanism preventing 2 or more SHT to connect to the same FPSO, to avoid false ‘Green-line’ status received by the FPSO. Unapproved attempt to connect to the FPSO will be rejected by the FPSO.'}</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Redundancy and Communication', 'text': 'The system is based on dual SeaGnal MB 45 controllers operating in parallel on different frequencies for enhanced redundancy. SeaGnal MB 45 is a software defined radio and provides internal processing capacity for complex computations. Exclusive ‘one-to-one’ communication links are established between the Telemetry systems on the FPSO and the Shuttle Tanker in the 450 MHz frequency band.'}</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Integration and Monitoring', 'text': 'The Telemetry system can work as a standalone system on both the FPSO and the Shuttle Tanker, but can also be integrated with the vessel’s DARPS system for control and monitoring of ‘Green-line’ status. Example shuttle set-up.'}</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -4227,22 +4239,22 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'BLUE INSIGHT. The digital ocean toolbox. Seamless data acquisition, fusion, processing, visualization, contextualization and management of ocean data. Kongsberg Blue Insight is an open and flexible digital infrastructure product designed to meet the increasing demand for accurate information from the oceans, focusing on internet security and seamless integration. The Blue Insight automates the data stream from a wide range of sensors and platform types and visualizes them in a common framework. The solution facilitates modern data processing and machine learning, providing new understanding and in-depth knowledge.'}</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Benefits of Blue Insight', 'text': 'KEY BENEFITS: Blue Insight offers a one-stop solution that provides a real-time overview across platforms and data types. It is flexible and scalable, suitable for both small and large organizations. The product is built on an open ecosystem that adheres to FAIR data principles and allows for the deployment of customized machine learning algorithms, all wrapped in a cyber secure solution.'}</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Blue Insight Core Module', 'text': 'BLUE INSIGHT CORE. The Blue Insight Core module provides solutions for secure interactions between sensor platforms, cloud storage and data management enabled by the industrialized Internet of Things modules found in the Kognifai digital ecosystem. The Core module includes required common functionality to prepare the data for automated analytics and advanced data handling, with the full benefits of a modern, cyber secure cloud environment. It integrates with existing IT systems and is essential for deploying other Blue Insight modules.'}</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensor Fusion and Data Forwarder', 'text': 'SENSOR FUSION DATA FORWARDER. Sensor Fusion is an on-board/on-premise application that receives and prepares data from selected sensors and onboard databases for streamlined distribution to the Blue Insight cloud. It provides interfaces with selected third-party sensors and links with the Sensor Remote and Ocean View modules. Optionally, a real-time visualization dashboard is available for monitoring purposes. The Data Forwarder module automates the conversion of data in the cloud into common formats and empowers efficient and seamless data sharing across cloud solutions and user databases.'}</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -4290,22 +4302,22 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Clariscan is KONGSBERG’s latest innovation in domed sonar technology. Clariscan combines the Company’s wide-bandwidth composite transducer with a patented acoustic lens to provide unprecedented image clarity from a domed sonar head.'}</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Domed Sonar Background', 'text': 'In the 1990s, designers enclosed the transducer in an oil-filled dome to provide mechanical protection and eliminate flooding due to O-ring failure on the traditional exposed transducer shaft. While the oil-filled dome solved the O-ring flooding failures, it introduced beam defocusing in two conditions, warm &amp; shallow and cold &amp; deep. The beam defocusing effect becomes more extreme in warm shallow water as temperature increases and cold deep water as depth increases. Until now, there has been no solution to this problem, aside from using a high-resolution scanning sonar head.'}</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative Lens Technology', 'text': 'Our engineers solved this problem by designing a patented acoustic lens that maintains beam focus through operational temperature and depth changes, significantly improving sonar performance and resulting in images that are much sharper. The Clariscan acoustic lens behaves like an optical contact lens, correcting the refraction caused by the oil in the dome. Clariscan is currently available in a 4000M depth-rated version.'}</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Applications', 'text': 'Obstacle avoidance, Pipeline survey, Target detection, and Underwater construction support are key applications of the Clariscan domed scanning sonar. Deep water testing in the Gulf of Mexico clearly showed the difference in image quality between the Clariscan sonar head and the standard domed sonar with composite transducer. The two sonar heads were mounted side by side on an ROV and thus exposed to the same temperature, pressure and salinity conditions, and were operated simultaneously during image capture. The three images below clearly show the image quality of the Clariscan sonar (left image) is superior and rivals that of a high-resolution scanning sonar head.'}</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -4345,22 +4357,22 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DPS 112 is a robust and reliable DGNSS (DGPS/DGLONASS) sensor suitable for a wide range of marine applications. It utilises the Seastar G2 service capable of worldwide decimeter accuracy.'}</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'A member of the DPS Family GPS and GLONASS', 'text': 'The Kongsberg Seatex award-winning DPS product line is well-proven and in use by professional marine and offshore users worldwide. The addition of GLONASS increases system availability and the performance of DPS 112 is greatly enhanced compared to traditional DGPS systems when operating in highly obstructed environments and under challenging signal tracking conditions.'}</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seastar G2 service Applications', 'text': 'DPS 112 is a cost-efficient DGNSS solution designed for users where availability and reliability are paramount, with a meter-level position accuracy and the possibility to have decimeter accuracy with the Fugro Seastar G2 service. Additionally, it has a built-in display for easy system configuration and status monitoring. An external display unit with an intuitive and easy-to-use graphical interface tailored for DP operations is available, forming an ideal solution for workboats and platform support vessels.'}</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'GNSS Spotbeam IALA', 'text': 'DPS 112 features a combined GPS L1/L2, GLONASS L1/L2, and SBAS receiver. It includes IALA beacon capability and a built-in L-band receiver with Fugro Seastar G2 capability. Easy software updates via USB and Ethernet interface are also notable features. An embedded keypad and display facilitate on-device operation, and the system is configurable for output to external interfaces.'}</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -4415,22 +4427,22 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DPS 114 is a robust and reliable DGNSS (DGPS/DGLONASS) sensor suitable for a wide range of marine applications. It utilises the Seastar G4 service capable of world wide decimeter accuracy.'}</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Satellite Coverage', 'text': 'A member of the Kongsberg Seatex award-winning DPS product line, DPS 114 utilises GPS, Glonass, Galileo, and Beidou, yielding enhanced satellite coverage compared to single- or dual- GNSS solutions. The utilisation of all available systems contributes to an enhanced operational availability in areas where obstructions and signal tracking can be challenging.'}</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence and Accuracy', 'text': 'Designed for applications where confident position solutions are essential in safety-critical environments, the DPS 114 is a cost-efficient DGNSS solution offering meter-level accuracy and potential decimeter precision with the Fugro Seastar G4 service. This makes it ideal for users where availability and reliability are paramount. Additionally, DPS 114 boasts a built-in display for easy system configuration and status monitoring.'}</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Intuitive and User-Friendly Interface', 'text': 'An external display unit with an intuitive and easy-to-use graphical interface tailored for Dynamic Positioning (DP) operations is available, forming an ideal solution for workboats and platform support vessels. Features such as multi-frequency receiver capability, built-in L-band receiver, and easy software updates via USB highlight the functionality suited for the demanding maritime industry.'}</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -4476,22 +4488,22 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "DPS 5D offers a hybrid GNSS-based position, attitude and heading system optimized for dynamically positioned (DP) vessels. This all-in-one solution caters to the extremes of precision and reliability, ensuring accurate positioning along with GNSS-based heading. It's the superior choice for installations that demand the utmost from their navigational systems."}</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed to be Trusted', 'text': 'The DPS 5D targets vessels with problematic infrastructure, using multi-sensor fusion techniques to deliver accurate and reliable positioning where traditional GNSS signals might be obstructed. It encompasses position and velocity data with unmatched precision, taking advantage of multiple GNSS signals and a plethora of differential correction data. Worldwide accuracy, extended by RAIM and the IMU, maintains high reliability under challenging GNSS conditions.'}</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensors Teaming Up', 'text': 'For optimal stability and reliability, especially when signal outages due to masking are common, DPS 5D integrates a dual GNSS receiver with an Inertial Measurement Unit (IMU). This powerful combination bridges reception gaps and augments position stability during periods of limited GNSS availability. Employing both GPS and IMU systems compensates for their individual limitations and jointly offers a superior navigational solution.'}</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Active Decision Support', 'text': "Enhancing the DPS 5D's user experience, an intuitive graphical user interface has been developed through close co-operation with experienced DP operators. It provides multi-layered information for a customized visual presentation and equips operators with the tools to assess the quality of their positioning. The system also incorporates features such as dual GNSS antenna solutions, maximum interference reduction, and robust computation of positions, improving both the accessibility and the integrity of data provided to the DP system."}</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -4589,22 +4601,22 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The DPS Display Unit is an optional monitor for DPS i1. With a 10-inch maritime panel computer and touch display, this design is tailored for both panel and bracket mounting. Installation is quick, operation is user-friendly, and communication with the Processing Unit is efficiently handled via Ethernet.'}</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Design and Installation', 'text': 'The design of the DPS Display Unit allows for both panel and bracket mounting, providing versatility to meet various operational requirements. It is designed for swift installation and ease of use, ensuring an optimal ergonomic interface for interaction with the DPS i1 system.'}</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Communication', 'text': 'To ensure seamless functionality, the DPS Display Unit communicates with the Processing Unit through an Ethernet connection. This industry-standard protocol facilitates reliable and fast data transfer, enabling efficient system performance and real-time monitoring.'}</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Durability', 'text': 'The DPS Display Unit is built to withstand challenging maritime conditions. Encased in die cast and painted aluminium, with enclosure protections rated IP 56 for console or flush mounting and IP 22 for VESA mounting, the unit is robustly designed to operate within a broad range of temperatures, from -10°C to +55°C.'}</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -4650,22 +4662,22 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DPS i1 MARITIME DGNSS SENSOR FOR WORLDWIDE OPERATIONS DPS i1 is a robust and reliable DGNSS sensor suitable for a wide range of marine applications. It utilises the Fugro Seastar™ G4 service which is capable of worldwide decimeter accuracy.'}</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Satellite Coverage', 'text': 'A member of the DPS family GNSS infrastructure, the Kongsberg Seatex award-winning DPS product line is well-proven and used by professional marine and offshore operators worldwide. The DPS i1 utilises GPS, Glonass, Galileo, and BeiDou, providing enhanced satellite coverage compared to single and dual GNSS solutions. The utilisation of all available systems contributes to an enhanced operational availability in areas where obstructions and signal tracking can be challenging.'}</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seastar G4 Service Integration', 'text': 'The DPS i1 uses regional SBAS services such as WAAS, EGNOS, GAGAN, and MSAS, and local DGNSS services such as IALA DGPS. In addition, the DPS i1 can utilise the Fugro Seastar G4 service, delivered by Fugro’s own network of dual system reference stations. This service provides consistent decimetre level accuracy positioning with ‘orbit and clock’ corrections with a global validity.'}</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for Precision and Ease of Use', 'text': 'DPS i1 is a cost-efficient DGNSS solution designed for users where availability and reliability are paramount. The system has a meter-level position accuracy and the possibility to have decimeter accuracy with the Fugro Seastar G4 service. DPS i1 has a built-in display for easy system configuration and status monitoring. An external display unit with an intuitive and easy-to-use graphical interface tailored for DP operations is available, forming an ideal solution for workboats and platform support vessels.'}</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -4711,22 +4723,22 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DPS i2 SENSOR FUSIONED GNSS SOLUTION FOR DYNAMIC POSITIONING By the introduction of the DPS i-series, KONGSBERG fuses decades of experience within GNSS and inertial technology in order to create a fully scalable and future-proof reference solution with emphasis on operational efficiency for DP applications.'}</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensors teaming up Increased operational efficiency', 'text': 'An unmatched integration of the latest within multi-GNSS technology and KONGSBERG’s unique motion gyro compass (MGC™) facilitate the possibility to operate with no additional augmentation services without compromising on DP performance. The DPS i-series is fully prepared to utilize differential corrections and SBAS services when required. DPS i2 utilizes data from GPS and GLONASS.'}</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for robust performance', 'text': 'The integration between GNSS and INS ensures a continuous position solution by bridging gaps in the GNSS reception and increasing position stability in periods with limited GNSS availability due to masking, scintillation, and interference. GNSS and INS are perfectly matched as they overcome each others limitations. Using both systems is superior to using either system alone. RAIM (Receiver Autonomous Integrity Monitoring) extended by data from the INS provides ultimate reliability of the position and velocity data under difficult GNSS conditions.'}</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Scalable solution', 'text': 'The flexible design of the DPS i-series ensures a scalable and expandable reference solution that can adapt to the specific requirements of any vessel. For the more demanding applications, a combination of multiple DPS systems and MGC/MRU sensors will enable precise heading determination world wide and provide spoofing detection capabilities. The DPS i-series may utilize existing or dedicated MGC or MRU sensors for the integration.'}</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -4800,22 +4812,22 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'By the introduction of the DPS i-series, KONGSBERG fuses decades of experience within GNSS and inertial technology in order to create a fully scalable and future-proof reference solution with emphasis on operational efficiency for DP applications.'}</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensors Teaming Up for Increased Operational Efficiency', 'text': 'An unmatched integration of the latest within multi-GNSS technology and KONGSBERG’s unique motion gyro compass (MGC™) facilitate the possibility to operate with no additional augmentation services without compromising on DP performance. The DPS i-series is fully prepared to utilize differential corrections, SBAS and Galileo HAS services when required. DPS i3 utilizes data from GPS and Galileo.'}</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for Robust Performance', 'text': 'The integration between GNSS and INS ensures a continuous position solution by bridging gaps in the GNSS reception and increasing position stability in periods with limited GNSS availability due to masking, scintillation and interference. GNSS and INS are perfectly matched as they overcome each others limitations. Using both systems is superior to using either system alone. RAIM (Receiver Autonomous Integrity Monitoring) extended by data from the INS provides ultimate reliability of the position and velocity data under difficult GNSS conditions.'}</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Scalable and Expandable Solution', 'text': 'The flexible design of the DPS i-series ensures a scalable and expandable reference solution that can adapt to the specific requirements of any vessel. For the more demanding applications, a combination of multiple DPS systems and MGC/MRU sensors will enable precise heading determination world wide and provide spoofing detection capabilities. The DPS i-series may utilize existing or dedicated MGC or MRU sensors for the integration.'}</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -4861,22 +4873,22 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'By the introduction of the DPS i-series, KONGSBERG fuses decades of experience within GNSS and inertial technology in order to create a fully scalable and future-proof reference solution with emphasis on operational efficiency for DP applications.'}</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensors Teaming Up for Increased Operational Efficiency', 'text': 'An unmatched integration of the latest within multi GNSS and KONGSBERG’s unique motion gyro compass (MGC™) facilitate the possibility to operate with no additional augmentation services without compromising on DP performance. The DPS i-series is still fully prepared to utilize differential corrections and SBAS services when required. DPS i4 utilizes data from all available GNSS constellations including GPS, GLONASS, Galileo and BeiDou.'}</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for Robust Performance', 'text': 'The integration ensures a continuous position solution by bridging gaps in the GNSS reception and increasing position stability in periods with limited GNSS availability due to masking, scintillation and interference. GNSS and INS are perfectly matched as they overcome each others limitations. Using both systems is superior to using either system alone. RAIM (Receiver Autonomous Integrity Monitoring) extended by data from the INS provides ultimate reliability of the position and velocity data under difficult GNSS conditions.'}</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Multi-Use of Sensor and Active Decision Support', 'text': 'By using the MGC as the inertial sensor, a high-quality WheelMark gyro compass becomes a part of the solution. In addition, MGC can serve other on-board systems such as navigation equipment and other systems that require attitude data. The DPS i-series has an intuitive and easy-to-use graphical user interface developed in close co-operation with experienced DP operators. The HMI (Human-Machine Interface) enables the operators to assess the quality of their positioning quickly and effectively during operation.'}</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -4970,22 +4982,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'By the introduction of the DPS i-series, KONGSBERG fuses decades of experience within GNSS and inertial technology in order to create a fully scalable and future-proof reference solution with emphasis on operational efficiency for DP applications. DPS i6 provides a superior solution to the most challenging installations. In addition to precise positioning, DPS i6 also offers precise GNSS based heading. The flexibility with regard to installation of the dual GNSS antennas ensures optimum tracking of multi-constellation satellite signals under all conditions.'}</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sensors Teaming Up for Multi-use', 'text': 'An unmatched integration of the latest within multi GNSS technology and KONGSBERG’s unique motion gyro compass (MGC™) facilitate the possibility to operate with no additional augmentation services without compromising on DP performance. The DPS i-series is still fully prepared to utilize differential corrections, SBAS and Galileo HAS services when required. By using the MGC as the inertial sensor, a high-quality WheelMark gyro compass becomes a part of the solution. In addition, MGC can serve other on-board systems such as navigation equipment and other systems that require attitude data.'}</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for Robust Performance', 'text': 'The integration between GNSS and INS ensures a continuous position solution by bridging gaps in the GNSS reception and increasing position stability in periods with limited GNSS availability due to masking, scintillation, and interference. GNSS and INS are perfectly matched as they overcome each others limitations. Using both systems is superior to using either system alone. RAIM (Receiver Autonomous Integrity Monitoring) extended by data from the INS provides ultimate reliability of the position and velocity data under difficult GNSS conditions.'}</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Active Decision Support', 'text': 'The DPS i-series has an intuitive and easy-to-use graphical user interface developed in close co-operation with experienced DP operators. The HMI (Human-Machine Interface) enables the operators to assess the quality of their positioning quickly and effectively during operation. The DPS i-series is ready for K-IMS remote services for operational support and troubleshooting. Cases that previously required a visit from a service engineer, may now be resolved remotely.'}</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -5084,22 +5096,22 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'DRS 500 and IMS 500 are the third generation DGNSS reference products from Kongsberg Seatex. The products feature a new graphical user interface for real time operation and system control. The new Human Machine Interface (HMI) is optimised for easy identification of, and fast operator response to events. The DRS 500 and IMS 500 are fitted with a state-of-the art GNSS receiver supporting future signals in space.'}</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'DGNSS Network Integration', 'text': 'In a DGNSS network infrastructure, the DRS 500 and the IMS 500 are integrated enabling both pre and post integrity control. A Central Monitor application (DGNSS CM) enables full remote operation of all stations in a network. The RTCM data will be checked for availability, position accuracy and other quality criteria. Alarms and warnings will be displayed and stored in an alarm file. Based on predefined fault criteria, the IMS 500 will switch between the two DRS 500 units in a redundant configuration.'}</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'DRS 500 Transmitters', 'text': 'The DRS 500 is a DGNSS reference station designed for permanent installation as a stand-alone system or as part of regional GNSS infrastructure systems. The DRS 500 generates differential GNSS (DGNSS) corrections. Raw pseudo-range observations and other pertinent data from the GNSS receiver are used to calculate optimal sets of corrections at every measurement cycle. The DRS 500 is fully compatible with the DGPS Reference Station Transmitters from all leading manufacturers of such equipment. The transmitters amplify the signals generated from the DGNSS reference stations and are fully configurable from the DRS 500 and the IMS 500.'}</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Redundancy and Integrity', 'text': 'The DRS 500 offers data integrity, check and quality control of each individual GNSS satellite. The data quality control algorithms implemented in the DRS 500 will detect errors not detected by the GNSS receiver itself. Kongsberg Seatex delivers a cost-effective fully redundant solution consisting of two DRS 500 and one IMS 500 unit. One of the DRS 500 units can be reconfigured remotely or automatically to take the role of an IMS in case of failure in the IMS 500.'}</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -5176,22 +5188,22 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Long-Term Offshore Monitoring Solution', 'text': "The Dual-Axis Scanning (DAS) Sonar is a profiling system designed for long-term seabed or structure monitoring. This scanning sonar is compatible with both the MS1000 software program and can operate in a 'standalone mode' where the data is logged in the head and transmitted to shore via cable or wireless telemetry."}</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Dynamic 3D Surveying and Design', 'text': 'The continuous 3D-surveying capability of the DAS provides crucial information on the dynamics of sediment scour and aggregation. Its rugged design makes it ideal for deployment on structures located in high-current or harsh offshore environments. The DAS outputs an X, Y, Z serial data string of profile points that can be processed by many digital terrain modeling software packages.'}</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible Deployment and Area Coverage', 'text': 'The sonar head is primarily designed for pole-mount deployment which can be attached to the structure of interest or to the side of a vessel. A single or multiple DAS heads can be integrated to cover and monitor a large area effectively.'}</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Operating Modes', 'text': 'The DAS Sonar offers multiple operating modes for diverse monitoring needs. In Standalone Mode, it uses host or third-party power to acquire data per predefined configurations, interfacing with other equipment in remote locations. The MS1000 Mode allows the MS1000 processing software on a PC to control the sonar, visualize data on screen, and record it for further processing.'}</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -5239,22 +5251,22 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Simrad PxPos is a multifunction gear monitoring and positioning sensor. It operates using a wireless communication link between the sensor and the transducer on your vessel. We have designed the Simrad PxPos sensor to improve your control of the trawl operation and thus the overall efficiency of your fishing.'}</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Stay in touch...', 'text': 'Stay in touch for product information and software updates. Join us on Facebook, follow us on Twitter, and visit us on LinkedIn.'}</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Where to buy Simrad products', 'text': 'If you want to purchase Simrad equipment, you can rely on a world wide sales organization.'}</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Support Simrad Products', 'text': 'The "Simrad" brand name is owned by Kongsberg Maritime. All Simrad products are thus supported by Kongsberg Maritime. We offer world wide support and training on our professional fish finding and…'}</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
@@ -5286,22 +5298,22 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'EA440 is a high performance hydrographic wide band single beam echo sounder. Developed for hydrographic use in shallow to medium depth waters, it facilitates hydrographic observations ranging from 30 kHz to 500 kHz. The EA440 supports applications from 0.2 m to 3000 m water depths. It also enhances hydrographic operations with its capability for sidescan sonar and sub-bottom profiling.'}</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Hydrographic Capabilities', 'text': 'The EA440 excels in delivering advanced hydrographic capabilities. With its 4-channel standard WBT, the EA440 operates across a range of 10 kHz to 500 kHz, transmitting and receiving data simultaneously. This feature enables versatility in applications and redundancy setup. Besides, the EA440 ensures high-quality signal and range resolution through its wide band frequency sweep and advanced signal processing.'}</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Intuitive User Experience and Compatibility', 'text': "The user-friendly interface of the EA440 software offers an intuitive experience with customizable display options for echograms, map views, and depth readings. Compatibility with standard Windows 10 systems and a variety of transducer interfaces, including Kongsberg and third-party transducers, ensures a flexible and inclusive operation. Splashproof hardware and true raw data logging further assert the EA440's efficiency and robustness in hydrographic operations."}</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Precise Tracking and Geographical Mapping', 'text': "EA440's map view feature empowers users with precise tracking and comprehensive coverage display, enhancing navigation and surveying with geographic visualization. The map view, supported by user-supplied WMS or GeoTIFF services, provides an accurate representation of the vessel's path and sidescan sonar coverage. This instrumental functionality is supplemented by the system's facility to record and store all raw sample data, including external sensor inputs for detailed replay and analysis."}</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -5369,22 +5381,22 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EA440 hydrographic echo sounder is a high performance device, versatile for applications from 0.2 m to 3000 m water depths. With capabilities spanning from 30 kHz to 500 kHz for various hydrographic depth observations and additional functionalities such as sidescan sonar and sub-bottom profiling, the EA440 is a powerful tool for a wide range of marine surveying tasks. The EA440SP represents a splashproof variant designed specifically for operability in shallow water depths aboard small and open boats, encased in a protective suitcase.'}</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Applications and Advanced Technology', 'text': 'The EA440 is a versatile hydrographic wide band single beam echo sounder, optimized for use in shallow to medium depth waters. It includes a Wide Band Transceiver (WBT) that is rugged and splashproof, suitable for harsh marine conditions. With a transceiver capable of interfacing with both Kongsberg and third-party transducers, the system provides a range of options for echo sounding. Offering CW and FM pulse forms, true raw data logging, and world-class bottom detection, the EA440 delivers exceptional signal to noise ratio and range resolution due to its wide band frequency sweep and advanced signal processing.'}</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Use and Durable Design', 'text': 'Ease of operation is central to the EA440 hydrographic echo sounder. Its intuitive software configures, operates, logs, and monitors surveying activities, displaying vessel track and sidescan coverage on the map view. The splashproof EA440SP is designed specifically for small or open boat operations where exposure to the elements is a concern. The design allows for straightforward connection of the transducer and computer, providing a durable solution that can be powered by 12 VAC. With the ability to handle diverse survey applications through the right choice of transducers and licenses, the EA440 interprets high-precision depth measurements and can be adapted for sidescan sonar surveys and sub-bottom profiling.'}</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Customization and Support', 'text': "The EA440 echo sounder offers a high degree of customization through the selection of transducers and available licenses, which can be easily managed by the user. This customization extends the capabilities of the EA440, allowing it to perform tasks like seabed imaging and profiling the upper sediment layers. For convenience and precision, Kongsberg also provides a tailor-made bracket designed for the combination of EA440 sidescan sonar and its transducers, emphasizing the system's flexibility and Kongsberg's commitment to supporting client needs with a complete hydrographic depth view solution."}</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -5444,22 +5456,22 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EA640 Wideband hydrographic echo sounder is suitable for full ocean depths, offering applications from extreme shallow to full ocean depths. It is designed for high performance hydrographic single beam echo sounder depths, deployable in all water conditions, from very shallow to full ocean depths. The EA640 is capable of operating from 12 kHz to 500 kHz using the WBT wideband transceiver unit, enabling it to function simultaneously with various transducers.'}</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Echo Sounder Capabilities', 'text': 'For hydrographic tasks in full ocean depths, the high-performance EA640 presents an advanced echo sounder that operates with an extensive frequency range from 12 kHz to 500 kHz. It accommodates high-power output from 10 kHz to 50 kHz for deep-water explorations. With a wide array of transducer interfaces compatible with both Kongsberg transducers and third-party options, the EA640 offers incredible versatility. Its world-class bottom detection algorithms deliver reliable, high-precision depth determination, complemented with valuable bottom slope information.'}</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'The EA640 Wide Band Transceiver - WBT', 'text': "The EA640 features a standard 4-channel WBT that transmits and receives data across a frequency range of 10 kHz to 500 kHz, simultaneously. Each channel is configurable for various applications or redundancy with a standard transmit power of 500W per channel. High-power WBT options provide 2 channels from 10 to 50 kHz with up to 2000W transmit power. Communication with the EA640 software is made possible through an ethernet link to a Windows 10 computer, with support for multiple configurations of WBTs. License management and power supplied by a 12-15 VDC source underscore this versatile transceiver's capabilities."}</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Data Interpretation and Display', 'text': "The EA640 software, an intuitive and user-friendly interface, allows operation from a Hydrographic Operation Station (HOS) or any Windows 10 compatible PC. Users can personalize their display settings, choose between various screen presentations, and save settings for different operations. The EA640 ensures internal storage of all raw sample data, including external input sensor data for replay purposes. Additionally, the map view offers a comprehensive geographical display of the vessel's position, tracks, and sidescan coverage based on user-supplied WMS or GeoTIFF services."}</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -5522,22 +5534,22 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "Use the EK Mission Planner to plan an autonomous mission from deployment to recovery. This EK mission planner is a planning and programming tool for autonomous echo sounders such as Simrad WBAT and Simrad WBT Mini. You can set up all necessary parameters related to 'wakeup' and 'sleep' times for the echo sounder, as well as transmission modes, intervals, and other parameters. After you have planned the deployment carefully, all settings are uploaded to the transceiver."}</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'End-user Documentation and Software Control', 'text': "In addition to running a predefined schedule, you can first use the EK Mission Planner to define the ping configurations and send these to the instrument. Then you can use the 'interactive mode' (or 'command mode' if you like) to control the transmissions from an external source such as an onboard controller. 'Interactive mode' also enables the reading of key information such as mean volume backscattering strength in layers in real-time."}</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Features and Applications', 'text': 'Control of all necessary parameters needed to program a mission plan is a pivotal feature with the mission plan being set by programming in Ping Groups, Ping Group Libraries, Phases, and Ensembles as part of license-free software. Typical applications include Ocean observatories, Fish migration studies, Long-term biological studies, Improved fish stock assessment, and Water column profiling.'}</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Mission Planning and Deployment', 'text': "When making a mission plan you start by selecting the transducer(s) you will use for the deployment. The next step is to define ping groups, i.e. all parameters for a ping, such as CW (Continuous Wave) versus FM (Frequency Modulated), pulse duration, transmit power, and so on. The third step is to define the duration of the deployment which can be divided into several phases. Usually, it's sufficient to use only one single phase. The last step in the mission planning is to put the ping groups you defined into ensembles. You can choose if the ensembles shall be repeated for a fixed number of iterations or for as many times as possible within the time span you choose. After planning the mission, you can set the environmental parameters. After completing these steps, you are ready to connect to the transceiver, send the mission plan to the transceiver and deploy."}</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -5577,22 +5589,22 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EK80 Portable is a complete echo sounder system for scientific use. It is an all in one rugged solution with compact PC, echo sounder and GPS. Built in WiFi lets you control and operate the system from any handheld device or laptop.'}</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Comprehensive Portability', 'text': 'The EK80 Portable is a compact solution that can be deployed from a small vessel in a rough environment. Built around the WBT Mini transceiver, it utilizes the EK80 software on an integrated computer with built-in GPS. Remote desktop access via WiFi allows control by handheld device or laptop. For backup, a small touch-screen is built into the solution. The system is compatible with any Simrad echo sounder transducer, and a selection of EK80 licenses are available. The integrated transceiver supports chirp (FM) and continuous wave (CW) pulse forms and has four individual transceiver channels with multiplexing functionality.'}</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Applications', 'text': 'The EK80 Portable serves various fields such as marine and freshwater research, enabling portable setup for mobile surveys from small boats in lakes, fixed location fish counting in rivers, and monitoring fish passage at hydropower dams. Additional uses include habitat mapping and plankton studies. The system’s rugged and splash-proof design, with an integrated computer running the EK80 echo sounder software, provides complete functionality. Essential data is recorded to the integrated SSD or a USB flash drive.'}</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Features for Scientific Exploration', 'text': "Featuring a ready-to-use, rugged, and compact design, the EK80 Portable includes an integrated computer and display, GPS receiver, and WiFi. It boasts a built-in calibration tool and is compatible with a wide range of transducers. Furthermore, it provides RAW echo sounder data recording and is a member of the Simrad EK80 wideband echo sounder family. The device's splash-proof cabinet facilitates easy handling and rapid deployment, ensuring reliable performance in the field."}</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -5676,22 +5688,22 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Simrad EK80 Portable entry is all you need for ecosystem monitoring and analysis in one package – at a reasonable price. This is a complete rugged echo sounder with a built-in computer, GPS and WiFi for remote operation.'}</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'All-in-One Echo Sounding Solution', 'text': 'The core of the product is the WBT Mini, a compact EK80 wideband transceiver with four channels. The Entry bundle uses three of these channels for the 38 kHz split beam, while the last channel is used for the 200 kHz single beam. The Simrad EK80 Portable entry is provided with the ES38-18/200-18 transducer. This is a dual frequency transducer combining 38 and 200 kHz in one housing. The beam width is 18 degrees at both frequencies to secure a large sampling volume in shallow water.'}</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Data Analysis and Support', 'text': 'The Echoview post-processing module offers traditional fish survey analysis. This includes measurement of biomass and size distribution, species separation, ecosystem mapping and habitat classification. The license can import data only from the EK80 Portable entry. Three months of maintenance and technical support is included. Combining high and low frequencies and FM pulse is ideal for mapping ecosystem components and separating fish from plankton.'}</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Upgradeable and Customizable', 'text': 'The 38 kHz is also split-beam for accurate target strength measurements and target tracking. The Simrad EK80 Portable entry can be upgraded to additional frequencies and FM pulse transmissions at a later stage. Likewise, the Echoview software license is permanent. We can offer upgrades to other EK80 configurations as well as training and extensions of maintenance and support for the entry module.'}</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -5735,22 +5747,22 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'EK80 is a high-precision scientific echo sounder and ADCP system designed to quantify and monitor underwater ecosystems. The EK80 is a modular system capable of operating several different transceiver and transducer combinations, all through the same operator station. Based on more than 60 years of research and development in close collaboration with leading marine scientists, this wide band echo sounder system has succeeded the famous EK60, which became an international standard for fish stock assessment. The EK80 is now a wideband system with an operational range from 10 kHz to 500 kHz. The extreme range resolution and improved target characterization allow for a wide range of oceanographic applications.'}</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible System Integration', 'text': 'A wide selection of high-quality accurate surface- and depth transceivers and transducers are available for a flexible system, capable of integration on sensor platforms from small to large. Real-time echo integration and target strength analysis in an unlimited number of layers are provided as well as storage of raw data for replay or analysis in one of several post-processing software packages. The Ocean Science product EK80 has a defined and publicly available output format which is specified in the product’s interface description. For post-processing of the output data we refer you to this documentation, or use commercially available software applications like for example Echoview.'}</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'User Interface and Documentation', 'text': '(A) Top bar gives you fast access to key functionality and navigational information. (B) Replay bar allows you to retrieve saved files and control the playback. (C) Echogram views (D) Information panes provide additional and detailed data from the EK80 presentation. (E) Main menu system (F) Secondary menus (G) Bottom bar. End-user documentation, current software version, and data sheets are available to support the EK80 users.'}</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Features and Applications', 'text': 'Key Features include High dynamic range, Raw data recording, High ping rate, Multifrequency application for species identification, Simultaneous transmission of all frequencies, Several frequencies covering the same sampling volume, Wideband frequency sweep ("chirp") in combination with advanced signal processing gives an exceptionally good signal to noise ratio and range resolution, Echo sounder calibration module included, Remote control via web interface, Store and reload personal settings, Network interface for raw data recording, Acoustic Doppler Current Profiler (ADCP) functionality, License-free software for replay purposes. Typical applications are Ocean Observatories, Fish migration studies, Long-term biological studies, Improved fish stock assessment, Oceanographical studies, Water column profiling.'}</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -5802,22 +5814,22 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The modular, state-of-the-art EM 124 performs accurate, high resolution seabed mapping in shallow to full ocean depth. The successor to the EM 122, the EM 124’s broad range of functionality supports simultaneous collection of multiple data types, saving time in the planning, execution and analysis phase. A low noise echo sounder, EM 124 delivers superior data that requires minimal post-processing.'}</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Modular and Flexible Design', 'text': 'The EM 124 consist of new state-of-the-art electronics and separate transmit and receive transducers in a Mills Cross configuration. It utilizes the same field-proven transducers as the EM 122, making it easy to upgrade. Care has been taken to design a highly, modular and flexible solution with compact electronics for easier and faster installation. Due to a flexible transducer design, the system can be tailored to almost any required size. The largest standard size, 0.5 x 1 degrees, gives the ultimate system performance in terms of resolution and range, while a smaller 4 x 4 degrees solution allowing full ocean depth surveys even on smaller vessels.'}</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Clean and High Resolution Data', 'text': 'Due to the sector transmission technique, the system produces a strong dampening of multi-bounce interference from false echo, resulting in significantly cleaner data. Near field beam focus is applied in real time, both during transmission and reception. Due to sector transmission the focal point will be individual for each sector, resulting in a much sharper transmit beam over the entire swath. On reception, the focus is done dynamically for each beam. The result is a much higher resolution representation of the seabed.'}</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Full Seabed Coverage', 'text': 'The transmit fan is divided into up to 16 individual sectors in dual swath mode. This allows for unique control of the transmit fan, enabling active stabilization in real time to correct for any yaw and pitch movement of the vessel, while roll stabilization is applied on the receiving beams. The result is a stabilized system for full ensonification of the seabed with equally distributed footprints, even in bad weather conditions, leaving no gaps or holes in the mapped area. All beams are maintained and automatically adjusted according to achievable coverage or operator defined limits. Up to 1600 individual beams are available in dual swath mode. Two individual transmitting fans are generated with a small difference in tilt giving a constant sounding pattern on the seafloor.'}</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -5863,22 +5875,22 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EM 2040 MKII is a true wide band high resolution shallow water multibeam echo sounder, an ideal tool for any high resolution mapping and inspection application. With this release, Kongsberg Maritime has upgraded the hardware and software to increase the swath and improve the data quality of our EM 2040 series.'}</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced System Capabilities', 'text': 'The system fulfils, and even surpasses, IHO-S44 Exclusive Order and the more stringent LINZ specification. The EM 2040 was the first 3-sector broadband multibeam echo sounder in the market, now available as a 200 - 700 kHz system. The operator can on the fly choose the best operating frequency for the application: 300 kHz for near bottom, 200 kHz for deeper waters and 400 - 700 kHz for very high resolution inspection. 600 kHz wide area high frequency mapping mode offers an unprecedented 100 - 120° swath width. 700 kHz inspection mode provides the highest resolution available contained within a narrow 30° swath.'}</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Multifrequency Operation', 'text': 'By alternating between the frequency modes per ping, the system is capable of providing the operator with Multi Frequency Backscatter of up to 5 frequencies in a single pass. The same functionality allows the system to alternate between a full swath mode and a high resolution mode providing full coverage while maintaining ultra high resolution over a target. The angular coverage for the 200 and 300 kHz is up to 170° on slopes and piersides, with coverage up to 8 times water depth on a flat bottom. For a dual transducer system, 220° angular coverage or 10 times the water depth is achieved on a flat bottom.'}</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Modular and Versatile Design', 'text': 'The EM 2040 MKII is a modular system, fully prepared for upgrading to cater for more demanding applications. The basic system has four units: a transmit transducer, a receive transducer, a processing unit and a hydrographic workstation. The EM 2040 MKII receiver is 0.5° and is delivered with a 0.25° or 0.5° transmitter(s). The transmit fan is divided into three sectors pinging simultaneously at separate frequencies ensuring a strong and beneficial dampening of multibounce interference. As an option the EM 2040 MKII can be delivered with dual swath capability, allowing a sufficient sounding density to meet survey coverage standards along track while maintaining a high vessel speed.'}</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -5941,22 +5953,22 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'This document has undergone several revisions to update and correct information regarding Kongsberg multibeam and single beam systems. Notable revisions include the removal of Systems EM 1002 and EM 2000, the addition of Systems EM 2040 and EM 2040C, and corrections to the table at the end of the document. Subsequent updates have added source level data for single beams, calculations for reduced power affecting source level, and the inclusion of MKI and MKII for EM304.'}</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Understanding Sound Levels', 'text': 'The power output level of an echo sounder is typically specified by its source level in dB relative to 1 μPa at a distance of 1 m from the transmit transducer. This measure, however, is directly applicable only in the farfield. The intensity of a sound wave is related to the pressure level and can be calculated using the relation I = p2/ρc. The source level is given by SL = 170.8 + 10lgP + DI, where P is the acoustic power and DI is the transducer’s directivity index. The nearfield limit is conventionally given by R = L2/λ, and the pressure levels in the nearfield can be derived from the source level of an echo sounder by calculating the pressure level at the largest farfield limit and adjusting for distance to the transducer.'}</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Pressure Level Calculations', 'text': 'In the nearfield, the pressure level will be nominally constant as there is no spreading, and if the transmit transducer is rectangular, there will be a transition region with cylindrical spreading. The maximum possible pressure level can be estimated based on the maximum acoustic power intensity that can be applied to a transducer to avoid cavitation. The calculations outlined are for the on-axis direction, and off-axis, the pressure level will fall rapidly for a narrow beam. For multibeams using sectorized transmission, beam defocusing is applied in shallow waters, which shortens the nearfield and starts the drop-off in pressure level earlier.'}</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Multibeam and Single Beam Parameters', 'text': 'Tables provided in the document list relevant parameters for Kongsberg multibeam echo sounders, including beamwidth, source level, nearfield distances, and pressure levels. Absorption loss is accounted for in the second table with pressure levels at fixed distances and the range at which the pressure level is 180 dB re 1 μPa. Additionally, a table for single beam transducers shows the Source Level (SL), Transmit Power (TP), Band Width (BW), Transmit Response (TR), and Receive Response (RS). It is noted that source levels are reduced by 3dB when the transmit power is halved, and by 6dB when the voltage is reduced by 50%.'}</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -6000,22 +6012,22 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EM 2040C MKII is a shallow water multibeam echo sounder based on EM 2040 technology. It is an ideal tool for any high resolution mapping and inspection application. With the release of the EM 2040 MKII series Kongsberg Maritime has upgraded the hardware and software to increase the swath and improve the data quality of our EM 2040 series.'}</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key facts and Operating Performance', 'text': 'The system fulfils, and even surpasses, IHO-S44 Exclusive with one sonar head, allowing coverage of 5.5 times water depth and the more stringent LINZ specification. For a dual transducer system, 200° angular coverage or 10 times the water depth is achieved on a flat bottom. The operating frequency range is from 200 to 400 kHz with frequency selection in steps of 10 kHz. The operator can on the fly choose the best operating frequency for the application: 300 kHz for near bottom, 200 kHz for deeper waters and 400 or 700 kHz for very high resolution inspection. 700 kHz inspection mode provides the highest resolution available contained within a narrow 30° swath.'}</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Functionality and Component Integration', 'text': 'By alternating between the frequency modes per ping, the system is capable of providing the operator with Multi Frequency Backscatter of up to 5 frequencies in a single pass. The same functionality allows the system to alternate between a full swath mode and a high resolution mode providing full coverage while maintaining ultra high resolution over a target. By utilizing both CW and FM chirp pulses, the system can achieve long range capability and still maintain a high resolution. The maximum depth range for a dual head system in cold ocean water is 520 m at 200 kHz with a swath width up to 700 m.'}</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Use and Practical Component Design', 'text': 'All electronics are contained in the sonar head(s) which is interfaced to the processing unit via GBit Ethernet. The processing unit also supplies 48 VDC power via the same cable. Operator control, data quality inspection and data storage is handled by the hydrographic workstation running SIS software or by 3rd party software. As an option the EM 2040C MKII can be delivered with the dual swath capability, allowing a sufficient sounding density to meet survey coverage standards along track while maintaining a high vessel speed.'}</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -6090,22 +6102,22 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EM 2040P MKII is a shallow water multibeam echo sounder based on EM 2040 technology, an ideal tool for any high resolution mapping and inspection application. With this release, Kongsberg Maritime has upgraded the hardware and software to increase the swath and improve the data quality of our EM 2040 series.'}</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced System Capabilities', 'text': 'Key facts about the system include surpassing the IHO-S44 Exclusive Order and the more stringent LINZ specification. The enhanced EM 2040P MKII is delivered with three essential components: A sonar head, a processing unit, and a workstation. The three-sector broadband multibeam echo sounder, now offered from 200 to 700 kHz, allows operators to select the best operating frequency for varied applications, such as 300 kHz for near bottom, 200 kHz for deeper waters, and 400-700 kHz for very high resolution inspection.'}</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatility and High-Definition Performance', 'text': 'The EM 2040P MKII excels in versatility, enabling the operator to achieve Multi Frequency Backscatter of up to five frequencies in a single pass by alternating between frequency modes per ping. The same functionality supports switching between a full swath mode and a high resolution mode which ensures full coverage and ultra high resolution over targeted areas. With the capability of working effectively with very short pulse lengths and a raw range resolution of 10.5 mm, this system redefines high-definition seabed mapping.'}</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Rugged Design and Real-time Data Processing', 'text': 'Built for the rugged demands of marine environments, the EM 2040P MKII features a sonar head with protective bumpers and carrying handles. The system can be upgraded to include an IP67 rated portable processing unit, ensuring durability and ease of use in various conditions. Real-time motion stabilization and compensation require data from motion sensors, heading, and positioning systems for accuracy. The sonar head contains all electronics and facilitates data quality inspection, operator control, and storage via a hydrographic workstation.'}</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -6149,22 +6161,22 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The modular, state-of-the-art EM 304 MKII performs accurate, high resolution seabed mapping in shallow waters to full ocean depth. The EM 304 MKII’s broad range of functionality supports simultaneous collection of multiple data types, saving time in the planning, execution and analysis phase. A low noise echo sounder, EM 304 MKII delivers superior data requiring minimal post-processing.'}</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Modular and Flexible Design', 'text': 'The EM 304 MKII consists of new, state-of-the-art electronics and separate transmit and receive transducers in a Mills Cross configuration. It utilizes the same field-proven receive transducer as its predecessor, EM 302, and a new redesigned wide band transmit transducer increasing the depth and coverage. Care has been taken to design a highly modular and flexible solution with compact electronics for easier and faster installation. Due to a flexible transducer design, the system can be tailored to almost any required size.'}</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Full Seabed Coverage', 'text': 'The transmit fan is divided into up to 16 individual sectors in dual swath mode. This allows for unique control of the transmit fan, enabling active stabilization in real time to correct for any yaw and pitch movement of the vessel, while roll stabilization is applied on the receiving beams. The result is a stabilized system for full ensonification of the seabed with equally distributed footprints, even in bad weather conditions, leaving no gaps or holes in the mapped area.'}</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Clean, High Resolution Data', 'text': 'The system fulfills, and even surpasses, IHO S-44 order 1A. Due to the sector transmission technique, the system produces a strong dampening of multi-bounce interference from false echo, resulting in significantly cleaner data. Near-field beam focus is applied in real time, both during transmission and reception. As a result, there is a much higher resolution representation of the seabed.'}</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -6229,22 +6241,22 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The EM 712 multibeam echo sounder is a high to very high resolution seabed mapping system capable of meeting all relevant survey standards. The minimum acquisition depth is from less than 3 m below its transducers, to a maximum of 3600m dependent upon array size. Across track coverage (swath width) is up to 5.5 times water depth, with a maximum of up to 4400 m.'}</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Echo Sounder Models', 'text': 'There are four basic versions of the EM 712 system, with different range performances: EM 712 - Full performance version, very high resolution; EM 712 USV - Full performance for Unmanned Surface Vehicles (USV), wide frequency range; EM 712S - CW pulse forms only, FM chirp; and EM 712RD - Reduced Depth (600m), no Export License required, roll, pitch and yaw stabilization. EM 712 USV is reinvigorated for USVs with features such as transmit and receive nearfield focusing, seabed image, dual swath, modular design, water column display, water column logging, and extra detections, with a choice of beamwidths depending on the transducer configuration.'}</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative Acoustic Principles', 'text': 'The EM 712 operates at a frequency range of 40 to 100 kHz. The system excels due to its innovative design, where the transmit fan is divided into three individual sectors that aid in maximizing range capability and suppressing interference from strong bottom echoes. This results in strong reflectors outside the current TX sector receiving twice the sidelobe suppression on TX and RX in comparison to sounders with only one wide TX sector. These sectors are transmitted sequentially within each ping, utilizing distinct frequencies or waveforms. Moreover, the EM 712S and EM 712RD use CW pulses, while the full performance version, EM 712, supports longer, compressible waveforms (FM sweep).'}</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Stabilized and Focused Beam Technology', 'text': 'Fully stabilized and focused beams are implemented where the system applies beam focusing to both transmit and receive beams to achieve maximum resolution, even within the acoustic near-field of the antenna. There is dynamic focusing on all receive beams, and roll, pitch and yaw stabilization is applied in real time. The active elements of the EM 712 transducers are based upon composite ceramics, offering advantages like increased bandwidth and tighter performance tolerances. The electronics system of the EM 712 involves a true wideband design with customizable components and circuitry that enable it to support a wide range of frequencies and pulse forms.'}</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -6290,22 +6302,22 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'By providing AquaLink, KONGSBERG introduces an innovative product for the aquaculture industry, which will increase safety for personnel and equipment achieving reduced risk of damage to vessel and fish farm. AquaLink is a product that will increase the operational weather window, reduce preparation time for vessel approach to the aquaculture site, and ensure maximum loading / offloading rates. AquaLink is suited for both refit and newbuilding projects. Typical applications are Live Fish Carriers, Forage Carriers and Service Vessels in addition to vessels servicing exposed fish farms.'}</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Live Fish Carriers', 'text': 'KONGSBERG AquaLink transfers key process data between the live fish carrier and fish farm through the Maritime Broadband radio (MBR) link. Live CCTV streaming gives the crew real time visual information of status on the fish farm. In addition, water quality parameters are transmitted for evaluation and appropriate actions. With AquaLink, the Live Fish Carrier receives valuable weather data to the ship’s dynamic positioning and manoeuvring system. AquaLink transfers weather data such as wind, local surface and sea current at multiple depths via KONGSBERG’s unique Maritime Broadband radio.'}</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Forage Carriers', 'text': 'KONGSBERG’s AquaLink transfers key process data between forage carrier and fish farm through the Maritime Broadband radio link. The offloading process is monitored and controlled from a dedicated operator station onboard the forage carrier, which is interfaced with the fish farm silo system. This enables maximum offloading rate without the risk of spillage or unexpected stops. AquaLink also transfers weather data, such as wind, local surface current and sea current for multiple water depths, giving valuable data to the forage carrier’s dynamic positioning and manoeuvring system. With AquaLink, the forage carrier is prepared for intensive offloading operations in challenging weather conditions.'}</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "KONGSBERG's Services", 'text': 'Effective project execution is at the heart of KONGSBERG’s success when refitting vessels. By taking the time to gain in-depth knowledge of the customer’s needs, we can ensure optimal vessel performance by upgrading the right hardware and software systems. K-Remote uses online systems and health monitoring to provide KONGSBERG customer support with remote access to ensure system reliability. The system is designed to address the challenge of establishing a secure and reliable remote session to the vessel control system via satellite communication. The technical solution is using well proven technology adapted to maritime environments. Our Follow the Sun 24 hour support concept ensures support that never sleeps. With three high-tech support centres in Europe, America and Asia, someone will always answer the phone at KONGSBERG, no matter what time of day.'}</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -6362,22 +6374,22 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'A professional echo sounder needs high-quality transducers. We manufacture high quality and high-performance transducers for all single beam, split-beam and dual beam echo sounders. The transducer is the subsea element of the echo sounder. Our transducers are characterised by high quality, precision and accuracy. The frequencies cover from extreme shallow water to full ocean depth.'}</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Quality Transducers', 'text': 'Our transducers are characterised by high quality, precision and accuracy, making them essential for fish-finding applications. They are designed to meet the rigorous demands of all single beam, split-beam and dual beam echo sounders, ensuring that professionals have reliable equipment for their fish detection needs.'}</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Fish-Finding Transducers', 'text': 'We offer a broad range of transducers, including the Simrad C-All, Simrad 18-11, Simrad ES18, Simrad 38-7, Simrad 38-9, Simrad 38/200 Combi C, and many others, each tailored for specific fish-finding operations. The targeted frequencies allow detailed scanning from extreme shallow waters to the full depth of the ocean.'}</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Support and Contact Information', 'text': "The 'Simrad' brand name is owned by Kongsberg Maritime. All Simrad products are thus supported by Kongsberg Maritime. We offer world wide support and training on our professional fish finding and underwater science systems. For ease of access to Simrad's professional fish finding and underwater science systems, contact information is readily available."}</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -6419,22 +6431,22 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The SeaPos 300 series navigation sensors features type approved instruments for use on-board SOLAS vessels. All sensors are designed for integration with other navigation equipment, and will as default be configured and operated from an ECDIS without the need for separate external displays. The sensors are tested and approved in accordance with international regulations, and have the Wheelmark certification.'}</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Installation and Maintenance', 'text': 'The SeaPos 300 series is by default delivered with a bracket containing a solution for strain relief in both ends. The unit is easily configured via a built-in WEB user interface (UI). Software updates are supported via the WEB UI but also the USB interface will automatically detect new software when a USB storage device is inserted. The update will be accomplished without interfering with the existing configuration. The latest software will continuously be available for download from an FTP server hosted by Kongsberg.'}</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Integration and Display Reduction', 'text': 'The SeaPos 300 series of navigation sensors is designed to be fully integrated with other navigation systems. This means that these models are per default delivered without external display for configuration and operation. All operation and functionality are handled from typically the ECDIS in an integrated bridge system. The SeaPos 300 sensors are hence type approved with ECDIS from different manufacturers and brands, in order to avoid installing a redundant display/keyboard. One important principle of e-navigation is to reduce the number of displays on the bridge. The navigator needs to have important information easily available in order to reduce response time for decisions. Better integration will lead to a better bridge environment as well as a simpler installation.'}</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Interface and Wheel Mark Certification', 'text': 'The interface to other navigation systems is provided via network or serial interface (RS-422), in accordance with international standards. When used for type approved applications the MFD must be used. The SeaPos is delivered with a 7’’ MFD (MFD 307 panel computer) that is connected to the SeaPos via LAN. The MFD 307 is made for flush mount, but a variation of brackets can optionally be delivered.'}</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -6510,22 +6522,22 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Seatrack 220 represents the state-of-the-art in relative GNSS tracking systems combined with over 20 years of operational experience in extreme maritime environments. Utilizing the latest in GNSS technology, the Seatrack 220 transponder is tailored to applications demanding a high-end solution in reliability and accuracy. Seatrack 220 transmits data through serial interface or UHF-radio.'}</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Precision Engineering', 'text': 'Seatrack 220 provides unprecedented accuracy with an update rate up to 1 Hz, ensuring real-time tracking of maritime activities. Its precise 1-meter accuracy is pivotal for applications that require high-end solutions. The transponder’s compact and robust design boasts a diameter of 15 cm and a height of 80 cm, meeting the needs of demanding maritime environments.'}</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Communication Capabilities', 'text': 'Equipped with UHF radio frequencies ranging from 450-470 MHz and channel separation of 12.5 kHz, the Seatrack 220 excels in data communication. This advanced system can transmit crucial data up to a considerable range of 15 km (line-of-sight), with a transmission power of 0.5 W.'}</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable and Reliable', 'text': 'Designed to withstand rough maritime conditions, the Seatrack 220 operates flawlessly in a temperature range of -10°C to +55°C. With storage temperature capabilities stretching from -30°C to +70°C and an impressive enclosure protection rated at IP 68, the transponder can handle submersions up to 10 meters.'}</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -6599,22 +6611,22 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Seatrack 320 represents the state-of-the-art in relative GNSS tracking systems combined with over 20 years of operational experience in extreme maritime environments. Utilizing the latest in GNSS technology, the Seatrack 320 transponder is tailored to applications demanding a high-end solution in reliability and accuracy. Seatrack 320 transmits data through serial interface or UHF-radio.'}</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Cutting-Edge Tracking Performance', 'text': "In terms of performance, the Seatrack 320 boasts an exceptional level of accuracy, achieving 1 meter. With the ability to update at a rate of Up to 1 Hz, it ensures timely and precise tracking information. The system's UHF radio frequency ranges between 450-470 MHz with a channel separation of 12.5 kHz and a transmission power of 0.5 W, facilitating an impressive typical range of 15 km (line-of-sight), making it a formidable tool in the professional tracking landscape."}</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Reliable Design', 'text': 'The rugged and durable design of the Seatrack 320 is evident in its form—the device features a compact diameter of 15 cm and a height of 80 cm, with a weight of 4.7 kg. This sturdy construction is complemented by its substantial environmental capabilities, including an operational temperature range of -10°C to +55°C and a storage temperature range of -30°C to +70°C. The enclosure is IP 68 compliant, capable of withstanding immersion up to 10 m, attesting to its resilience in challenging environments.'}</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High Standards of Compliance and Safety', 'text': 'When it comes to safety and regulatory standards, the Seatrack 320 meets stringent criteria. The system demonstrates compliance with the Electromagnetic Compatibility Directive, maintaining immunity and emission standards according to IEC 60945/EN 60945. Additionally, it satisfies Product Safety requirements in line with the Low Voltage Directive, utilizing standards such as IEC 60950/EN 60950. These compliance factors ensure that the Seatrack 320 is a tracking solution that you can rely on for professional maritime operations.'}</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -6677,22 +6689,22 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Seatrack 222 represents the state-of-the-art in relative GNSS tracking systems combined with over 20 years of operational experience in extreme maritime environments. Utilizing the latest in GNSS technology, the Seatrack 222 transponder is tailored to applications demanding extremes in reliability and accuracy using both GPS and GLONASS L1&amp;L2 band. Seatrack 222 transmits data through serial interface or UHF-radio.'}</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced GNSS Capabilities', 'text': 'Incorporating cutting-edge GNSS technology, the Seatrack 222 leverages both GPS and GLONASS L1&amp;L2 bands, ensuring unparalleled reliability and precision. Its capability to mitigate multipath effects enhances the accuracy of tracking in various conditions, making it a powerhouse for applications that require pinpoint positional data.'}</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust Environmental Performance', 'text': 'Designed to withstand the challenges of the maritime environment, the Seatrack 222 boasts impressive operational and storage temperature ranges. It is constructed to meet the IP 68 standard, capable of remaining submerged under 10 meters of water, clearly demonstrating its robustness in harsh conditions.'}</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable Communication and Power Efficiency', 'text': "Communication is made efficient and reliable with the Seatrack 222's UHF radio, offering a typical range of 15 km line-of-sight, supporting 12.5 kHz channel separation and providing a transmission power of 0.5W. Power requirements are modest, necessitating only 10-36 V DC and averaging a lean 4 W power consumption, ensuring that it conserves energy while maintaining optimal performance."}</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -6763,22 +6775,22 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Seatrack 222B represents the state-of-the-art in relative GNSS tracking systems combined with over 20 years of operational experience in extreme maritime environments. Utilizing the latest in GNSS technology, the Seatrack 222B transponder is tailored to applications demanding a high-end solution in reliability and accuracy. Seatrack 222B has an internal battery for operation up to 48 hours while transmitting data over UHF-radio.'}</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced GNSS Capabilities', 'text': 'Employing GPS L1/L2 and GLONASS L1/L2, the Seatrack 222B is equipped to mitigate multipath effects, ensuring enhanced accuracy with less than 10 cm error and a reliable update rate of up to 1 Hz. This precision is the culmination of leveraging advanced GNSS technology, pivotal for high-stakes applications where every centimeter counts.'}</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Reliable Design', 'text': 'Designed to withstand the challenges of maritime use, the Seatrack 222B ensures operational functionality in temperatures ranging from -10°C to +55°C and is stored safely within -30°C to +60°C. The unit’s resilient enclosure is IP 68 rated, indicating a robust seal against ingress of water and dust, suitable for submersion up to 10 meters.'}</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Efficient and Durable Power Management', 'text': 'The Seatrack 222B is powered by a robust Li-ion battery that can operate the system for up to 72 hours on a full charge, with a mean power consumption of only 4 W. The impressive battery life is complemented by a rapid recharging capability, going from 10% to full charge in just 12 hours, ensuring that the Seatrack 222B is ready for prolonged deployments and minimal downtime.'}</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -6855,22 +6867,22 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MGC R2 product represents a new family of products combining motion sensing and gyro compass functionality. Included in this innovation are three Ring Laser Gyros and three linear accelerometers, making the MGC R2 product a full inertial navigation system (INS). Capable of outputting an array of navigational data such as heading, roll, pitch, heave, and position, this system is tailored for high precision maritime applications such as offshore operations and seabed mapping.'}</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Modes and Data Output', 'text': 'The MGC R2 is versatile in its operational capabilities, functioning both as a stand-alone unit or integrated within other systems. It has two primary modes: Gyrocompass mode, simplifying the typical applications where only the input of speed is needed to output crucial parameters including heading, roll, pitch, and heave; and an Integrated Navigation mode, which further necessitates inputs from a GNSS receiver (VTG, GGA, ZDA) for comprehensive outputs that additionally include position. This product consistently outputs both processed and raw sensor data, supporting detailed motion analysis.'}</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Heave Measurement and Navigation Algorithms', 'text': 'An impressive feature of the MGC R2 is its integrated navigation algorithms that facilitate the output of aided position and heading data when linked with a GNSS receiver. The acclaimed PFreeHeave algorithms are integrated to enable highly accurate heave outputs, both in real-time and delayed, offering precision down to 2 cm. Moreover, the unique mounting bracket ensures easy alignment with the vessel axis, guaranteeing optimal deployment and precise measurements for various maritime applications.'}</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Configuration Software and Data Distribution', 'text': "The unit comes with a Windows-based configuration and data presentation software, MRC+, which allows for precise calibration including vector arms, center of gravity (CG), and monitoring points. Coupled with digital I/O protocols that accommodate Ethernet interface and serial lines, this system ensures the MGC R2's outputs are readily accessible for distribution to multiple users onboard the vessel. As a result, the MGC R2 delivers high data availability in formats required by common marine survey equipment and systems."}</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -6939,22 +6951,22 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'A new family of products with motion sensing and gyro compass functionality is introduced. The first product in this family is the MGC R3 which includes three Ring Laser Gyros and three linear accelerometers. Typical applications will output heading, roll, pitch and heave accurately.'}</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Marine Technology', 'text': 'The MGC R3 product is a fully inertial navigation system (INS). It can output heading, roll, pitch, heave, position, acceleration, and velocity of linear motions, as well as angular rates. The unit is suitable for high precision maritime applications such as offshore operations and seabed mapping. It includes integrated navigation algorithms with input from a GNSS receiver for output of aided position and heading data.'}</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized for Accuracy and Performance', 'text': 'Proven PFreeHeave algorithms are part of the MGC R3 navigation algorithms that enable down to 2 cm accuracy in delayed heave output and 5 cm accuracy in real-time heave output. The MGC R3 outputs both processed and raw (gyro and accelerometer) sensor data and comes with Windows based configuration and data presentation software, the MRC+. This enhanced technology allows the delivery of precise high output data rates (200 Hz) and the management of relative (dynamic) heave position, velocity, and acceleration.'}</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'User-Friendly Integration and Functionality', 'text': 'The design of the MGC R3 includes a specialized mounting bracket for easy alignment, ensuring precise measurements upon installation. The product can operate in both Gyrocompass mode, requiring only speed input, and Integrated Navigation mode, which requires additional inputs. The MGC outputs are accessible via both Ethernet interface and serial lines, facilitating data distribution to multiple users on board. The versatility of the unit allows for heave measurements at four different locations, aiding in complex maritime tasks.'}</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -7024,22 +7036,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'A new family of products with motion sensing and gyro compass functionality is introduced. This MGC R4 product, with emphasis on position drift, includes three Ring Laser Gyros and three linear accelerometers.'}</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Navigation Precision and Versatility', 'text': 'The MGC R4 is a fully inertial navigation system (INS) capable of outputing heading, roll, pitch, heave, and position. It includes integrated navigation algorithms with input from a GNSS receiver for output of aided position and heading data, enriched by PFreeHeave algorithms that ensure down to 2 cm accuracy in delayed heave output and 3 cm in real-time heave output. The unit can also serve as an IMU in other systems, designed for high precision maritime applications including offshore operations and seabed mapping.'}</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible Configuration and Output Options', 'text': 'Configurable with the Windows based MRC+ software, the MGC R4 outputs both processed and raw sensor data through multiple options. It can provide heave measurements at four different locations and supports various digital I/O protocols for easy data distribution. The unit operates in both Gyrocompass and Integrated Navigation modes, depending on the demand for either speed input only, or additional speed, position, and PPS from a GNSS receiver. Moreover, it offers high output data rate and precise heave even during long wave periods.'}</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable, Efficient, and Certified', 'text': 'Aimed for sustained high performance, the MGC R4 is compact, exhibits low power consumption, and is delivered with a Calibration Certificate for quality assurance. To accommodate the needs of various nautical equipment, selectable communication protocols are included. The robust algorithmic design and durable materials meet rigorous standards ensuring reliable operation within the specified environmental conditions.'}</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -7116,22 +7128,22 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'A new family of products with motion sensing and gyro compass functionality is introduced. This MGC R5 product, with emphasis on position drift, includes three Ring Laser Gyros and three linear accelerometers.'}</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Navigation Capabilities', 'text': 'The MGC R5 product is a fully inertial navigation system (INS). It can output heading, roll, pitch, heave, and position. Acceleration and velocity of linear motions, as well as angular rates, are output from the unit. The MGC R5 product outputs both processed and raw (gyro and accelerometer) sensor data. With integrated navigation algorithms that incorporate input from a GNSS receiver, the product delivers output of aided position and heading data.'}</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimal Performance for Maritime Applications', 'text': 'Designed for high precision maritime applications such as offshore operations and seabed mapping, the MGC R5 excels in variable environments. It supports various modes, including Gyrocompass mode, which requires only the input of speed to deliver accurate heading, roll, pitch, and heave, and Integrated Navigation mode, which leverages additional inputs from a GNSS receiver for comprehensive navigation data.'}</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Data Distribution and Output', 'text': "The MGC R5 provides data through both Ethernet interface and serial lines to facilitate easy data distribution on board the vessel. Multiple users can access the data, which is compatible with commonly used survey equipment. Output protocols are available on two individually configurable serial lines as well as Ethernet/UDP. The product's sophisticated Digital I/O protocols ensure seamless integration and communication with other systems."}</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -7229,22 +7241,22 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MGC R2 COMPASS system is IMO type approved as a gyro compass for navigation purposes for use together with a heading and bearing repeater. Very high reliability is achieved by using Ring Laser Gyros with no rotational or mechanical wear-out parts.'}</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Applications and Communication', 'text': 'The system can be operated as an inertial navigation system as well as a gyro compass with output of position and heading. Linear position and velocity measurements can then be output in up to four different points on the vessel. MGC data is available through both Ethernet interface and serial lines enabling easy distribution of data to multiple users on board the vessel. Output protocols for commonly used equipment are available on five individually configurable serial lines and five Ethernet/UDP ports.'}</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Performance Functionality', 'text': 'Incorporating High Rate Gyros (HRG), the MGC R2 COMPASS ensures exceptional performance with its sets of sensors. It is designed to meet the demands of even the most challenging maritime navigation and orientation environments. The MGC R2 operates as an advanced Heading and Attitude Reference System (AHRS) and can also output additional data such as speed and latitude data (VBW/VTG and GGA/GLL) as required for optimal functioning.'}</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Built for Marine Conditions', 'text': 'MGC R2 COMPASS is built with consideration for the challenging conditions at sea. It offers a high degree of reliability and durability for different types of maritime vessels, including ships and high-speed crafts. The gyro compass effectively functions while providing accuracy in heading, roll, and pitch, as well as heave, thanks to its quality design and technical sophistication. The system has been thoroughly tested to ensure it stands up to maritime operational demands.'}</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -7284,22 +7296,22 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "MGC R3 COMPASS is a type approved compass system, suitable for ships and high-speed crafts, which provides high reliability, utilizing Ring Laser Gyros for navigation purposes. It's approved for use with a heading and bearing repeater and boasts high reliability due to the absence of rotational or mechanical wear-out parts."}</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Applications and Connectivity', 'text': "The MGC R3 COMPASS system offers versatile application as both an inertial navigation system and a gyro compass, providing position and heading outputs. It can handle linear position and velocity measurements, allowing for multiple data output points on a vessel. Enhanced connectivity is facilitated through both Ethernet interface and serial lines, ensuring easy distribution of data to multiple users onboard. The system's digital I/O protocols include output protocols for commonly used equipment, configurable across serial lines and Ethernet/UDP ports."}</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High Performance and Durability', 'text': 'The MGC R3 COMPASS system delivers in terms of performance and durability. Very high reliability is achievable through the state-of-the-art technology of Ring Laser Gyros (RLG), which are devoid of any rotational or mechanical components that would require maintenance or are prone to wear. This innovative design ensures that the compass system can withstand operational demands without the need for frequent replacements or repairs. With a robust construction that negates the need for mechanical parts, the MGC R3 stands as a resilient navigation tool capable of delivering stable and reliable data for maritime operations.'}</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Commitment to Quality and Reliability', 'text': "Kongsberg Seatex AS, located in Trondheim, Norway, oversees the production of the MGC R3 COMPASS. Each unit is not only type approved but also delivered with a Calibration Certificate, underscoring the company's commitment to quality and reliability. The focus on creating a dependable product extends to its supporting software, which allows for selectable communication protocols, ensuring the system's compatibility and configurability for diverse maritime navigation requirements."}</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -7339,22 +7351,22 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MGC R1 COMPASS system is IMO type approved as a gyro compass for navigation purposes for use together with a heading and bearing repeater. Very high reliability is achieved by using Ring Laser Gyros with no rotational or mechanical wear-out parts.'}</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Performance Navigation', 'text': 'The system can be operated as an inertial navigation system as well as a gyro compass with output of position and heading. Linear position and velocity measurements can then be output in up to four different points on the vessel. Typical applications include bridge systems where heading, position, speed, and rate of turn information, as well as heading and latitude data (VBW/VTG and GGA/GLL), is required.'}</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Communication Capabilities', 'text': 'MGC data is available through both Ethernet interface and serial lines enabling easy distribution of data to multiple users on board the vessel. Output protocols for commonly used equipment are available on five individually configurable serial lines and five Ethernet/UDP ports.'}</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Reliable Design', 'text': 'The high reliability of the MGC R1 COMPASS is due to its Ring Laser Gyros (RLG), which boast no rotational or mechanical wear-out parts. The MGC R1 COMPASS integrates advanced technologies to deliver accurate and reliable navigational data, becoming an indispensable tool for ships and high-speed crafts.'}</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -7407,22 +7419,22 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The ES38-18/200-18C is a combined transducer operating at two frequencies. It has a large bandwidth designed for fishery and research applications. The transducer includes two different transducers, a single-beam and a three-sector split-beam transducer. These can be operated simultaneously. The beamwidth remains 18° for both split-beam and single-beam transducer operation.'}</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile and High-Performing Transducer Design', 'text': "For the split-beam transducer, the operating frequency is 38 kHz, and for single-beam operation, the frequency is 200 kHz. The ES38-18/200-18C's compact size and light weight make it possible to mount on various subsea platforms. It is provided with a subsea cable having two termination options, fitting for WBT Mini and EK80 Portable, or an open-ended cable for broader connectivity."}</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Connectivity Options', 'text': "The transducer offers flexibility in connectivity with an 8-pin male MCIL8M connector or an open-ended cable option, complementing a wide array of subsea instruments. This combo transducer's specifications are developed to perform at high standards with a maximum transmit power of 500 W for the split-beam and 200 W for the single-beam, aligning with robust research and fishery application demands."}</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimal Handling for Accurate Performance', 'text': "To ensure longevity and precise readings, it's crucial to handle the transducer correctly, avoiding activation out of water, exposure to rough treatment, intense sunlight, high temperatures, and damage from improper cleaning methods. Proper handling instructions include not using high-pressure water or strong solvents on the face of the transducer and ensuring the protective skin and cable are not compromised."}</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -7466,22 +7478,22 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "Offshore helicopter operations are carried out in hostile environments. The HMS 300 is designed to measure helideck motion during helicopter pre-landing and on-deck operations to improve flight and passenger safety in these conditions. The system monitors the helideck's acceleration, heave velocity, inclination, roll, and pitch together with meteorological data in real-time."}</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Helideck Compliance and Web Access', 'text': 'The HMS 300 is fully compliant with the prevailing Web access recommendations and guidelines issued by the Civil Aviation Authorities in UK, Norway, and Brazil. The HMS 300 is compliant with the CAP 437 from September 2018 and accompanying Helideck Certification Agency (HCA) document revision 9b. This implies that the helideck must be equipped with repeater lights connected to the HMS 300 system to indicate to the pilot whether the on-deck or pre-landing conditions are within the landing limits or not. The system is also compliant with NOROG ver. 9.2 for the Norwegian sector and NORMAM-27 for the Brazilian sector.'}</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Data Monitoring and Enhanced Safety', 'text': 'The HMS 300 will calculate and present the Motion Severity Index (MSI) and Wind Severity Index (WSI) data together with significant heave rate (SHR), inclination, roll, and pitch of the helideck in real-time. The system utilizes the KONGSBERG MRU models (E, H, 5, or 5+) or the MGC models (R2 or R3) to precisely monitor vessel motion and accelerations at the helideck center. These data are transferred to the HMS Processing Unit that processes helideck motion data together with MSI and WSI figures to determine whether the helicopter operation is safe or not.'}</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Real-Time Monitoring and Cyber Security', 'text': 'Both onboard and onshore personnel can monitor helideck movements and meteorological data in real-time and see the same operational picture in order to increase operational awareness. Cyber security is an integral part of the system. With the cloud-based service, storage of helideck data for periods exceeding a month is included. Moreover, live vessel data can be made available from the HMS 300 installation when connected through the KONGSBERG Kognifai cloud-based digital platform (optional), which supports planning for helicopter operators before take-off from the heliport.'}</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -7527,22 +7539,22 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -7598,22 +7610,22 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP and HPR operation system is now available as a Trainer version supplied on a CD-ROM for installation on your own computer. The APOS Trainer is operated as a normal HiPAP/HPR system, where a simulator replaces the transceiver and the transponders. Suitable for training, planning and demonstration purposes, it presents a typical LBL and SSBL operator presentation as shown in the accompanying figure.'}</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Trainer Version Benefits and Operations', 'text': 'The APOS Trainer is suitable for training, planning and demonstration purposes. A typical LBL and SSBL operator presentation is shown in the accompanying figure. The APOS Trainer emulates the operation of a normal HiPAP/HPR system, only using simulation in place of actual transceiver and transponders. Users have access to a full APOS software package on the CD provided, excluding certain specialized functions. It supports tasks such as calibration of LBL arrays, telemetry communications with simulated transponders, and sound velocity ray-trace calculations.'}</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Simulation Features for Advanced Training', 'text': 'Within the Trainer, users can experience realistic LBL positioning by calibrating an array within the simulator. An example of such an array, marked with locations 1, 2, 3, and 4, positions the vessel and the SSBL transponder B27 relative to it. The Trainer also allows the setup of LBL arrays for accuracy examination, enabling efficient planning for real-world operations. Users can expect features like online help, detailed instruction manuals, and data output interfaces for testing communications with external computer systems.'}</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Software and System Requirements', 'text': 'The HiPAP and HPR 400 Series are designed to be controlled and operated via the APOS software, which features a standard Windows graphical interface and runs on a Windows NT platform. When delivered as part of a stand-alone system, APOS operates on an APC 10 computer, or on a COS 100 unit when integrated within a Dynamic Positioning and HiPAP/HPR system. For the APOS Trainer program, requirements include a personal computer with CD-ROM drive, Windows NT 4 service pack 3 or newer, a minimum monitor resolution of 800 x 600, and a network card installed with TCP/IP protocols.'}</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -7669,22 +7681,22 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP 102P with full ocean depth positioning and modem capability is designed for tracking ROV’s, tow fish and other subsea targets. HiPAP 102P is a portable acoustic positioning system designed for operation from a surface vessel to track ROV’s, tow fish and any other subsea targets at several thousand meters range in ultra deep water.'}</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seamless Integration and Calibration Efficiency', 'text': 'HiPAP 102P has built in motion sensors for compensating the position for vessels roll and pitch movements. These models have no need for calibration of roll and pitch alignments and only need to calibrate for heading alignment W.R.T. to the vessels’ gyro compass. The system can be interfaced to the vessel heading sensor and GNSS system. Data output to users are available in established formats. The calibration free HiPAP 102P-MGC contains attitude and heading sensor. This model has no need for calibration to determine roll, pitch and heading alignments.'}</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Portable and Versatile Positioning System', 'text': 'HiPAP 102P is designed to be a portable system for easy installation on surface vessels without the need for a through hull deployment unit. APOS, the operator station for HiPAP, provides the full range of functions for acoustic positioning and data communication. The Cymbal digital acoustic protocol provides accurate position and robust telemetry. HiPAP 102P has full LBL calibration and positioning capabilities and can be used for position box in, calibration and positioning.'}</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Diverse Model Options to Suit Various Needs', 'text': 'To meet various demands in the market, HiPAP 102P transducer is available in several models with respect to motion sensors: HiPAP 102P-MGC Motion Gyro Compass and HiPAP 102P-5 MRU 5 Motion Sensor. The system is offering the user a wide range of transponder channels and cNODE transponder models for depths down to 7000 meters and beyond.'}</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -7740,22 +7752,22 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP and HPR operation system is now available as a Trainer version supplied on a CD-ROM for installation on your own computer. The APOS Trainer is operated as a normal HiPAP/HPR system, where a simulator replaces the transceiver and the transponders. The APOS Trainer is suitable for training, planning and demonstration purposes. A typical LBL and SSBL operator presentation is shown in the figure to the right.'}</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'The Essence of APOS Trainer', 'text': 'The APOS Trainer is a versatile tool essential for training personnel in the use of HiPAP and HPR systems. With the full APOS software contained on a CD, including all options except some specific Offshore Loading System functions, and defined with one HiPAP and one HPR 400 transceiver, this solution proposes realistic and comprehensive training experiences. Moreover, the APOS Instruction manual and the Online Help function enhance the learning curve, while features like telemetry communication and calibration of LBL arrays solidify the operational understanding.'}</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative Simulation Capabilities', 'text': 'The APOS Trainer advances beyond usual training paradigms by enabling LBL positioning in the LBL array calibrated by the Trainer and SSBL positioning of transponders. These functionalities facilitate the simulation of precise operations such as the display of deflection based on velocity profile input and ray-trace calculation for sound velocity. Furthermore, the APOS Trainer allows for LBL positioning in an array set up by the user, thereby offering insights into the expected precision of different arrays and assisting in the planning process.'}</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'System and Software Excellence', 'text': 'The HiPAP and HPR 400 Series of systems are both controlled and operated using the APOS software on a Windows NT platform with a standard graphical user interface. The APOS software finds its place in various operational environments, from a stand-alone HiPAP/HPR Operator Station to an integrated solution in dynamic positioning and HiPAP/HPR systems. With requirements such as a personal computer running Windows NT or newer, a capable monitor resolution, and proper network configurations, the APOS Trainer program stands as a testament to technical and educational excellence.'}</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -7799,22 +7811,22 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP 352P is a portable system designed for tracking ROVs, tow fish, divers, and other subsea objects at several thousand metres range. Operating in SSBL mode, it measures the distance and direction to subsea transponders and computes a 3D position in either local or geographical coordinates. The HiPAP 352P’s portability enables easy installation on various surface vessels or units. Its operator station, APOS, offers a full range of functions for acoustic positioning and data communication, while the system itself benefits from the Cymbal acoustic protocol. Designed to accommodate a wide range of transponder channels and cNODE models, the HiPAP 352P excels in performance up to depths of 4000 meters.'}</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Integrated Motion Sensing', 'text': "Featuring built-in motion sensors, the HiPAP 352P compensates for the vessel's roll and pitch movements, enhancing positioning accuracy. Models such as HiPAP 352P-H and HiPAP 352P-5 incorporate MRU-H and MRU-5 motion sensors, respectively. These models require no calibration for roll and pitch alignments but do need to be calibrated in alignment with the vessel’s gyro compass. Meanwhile, the HiPAP 352P-MGC combines a motion sensor and a gyro compass, completely eliminating the need for roll, pitch, and heading alignments calibration."}</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Diverse Operational Demands', 'text': "The HiPAP 352P addresses varying market demands by offering transducers in several models catering to different motion and heading sensors. The system's robust design and sophisticated technology provide users with a dependable acoustic positioning solution. This adaptability allows users to choose the optimal configuration for their specific operational needs, whether for LBL calibration, positioning capabilities, or simply for tracking a variety of subsea objects with precision."}</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Coverage and Range', 'text': 'The HiPAP 352P system boasts notable operational and main coverage areas, ensuring maximum range and angular accuracy. Acoustic positioning and communication are most effective within the main coverage sector, with a range of up to 5000 meters and suggested depth input for efficient operation. In operational tests, the system has demonstrated the capacity to achieve 1000 meters at 80 degrees or near the horizontal orientation. Additionally, the robust signal to noise ratio within the specified signal bandwidth reinforces the reliability of the HiPAP 352P.'}</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -7883,22 +7895,22 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP and HPR operation system is now available as a Trainer version supplied on a CD-ROM for installation on your own computer. The APOS Trainer is operated as a normal HiPAP/HPR system, where a simulator replaces the transceiver and the transponders. The APOS Trainer is suitable for training, planning and demonstration purposes. A typical LBL and SSBL operator presentation is shown in the figure to the right.'}</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Comprehensive Training Tool', 'text': 'The APOS Trainer encompasses a full suite of functionalities designed to facilitate a robust training environment. It comes with a CD containing full APOS software with all options, tailored for a singular HiPAP and one HPR 400 transceiver. Features include an APOS Instruction manual, an Online Help function, sound velocity ray-trace calculation, and telemetry communication with transponders. It allows for the calibration of LBL arrays and use of data output for testing telegram interfaces to external computers, transmitting standard HiPAP/HPR telegrams.'}</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Positional Training', 'text': "In-depth training is vital for precision operations, which is facilitated by the APOS Trainer's capacity for LBL positioning within a calibrated LBL array. It demonstrates the vessel's positioning with transponders while allowing users to set up their own LBL array for examining expected accuracy. Through such simulation, planning for positioning in different arrays becomes more concrete, reinforcing the user's capacity to design optimal LBL arrays."}</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'System Requirements and Operation', 'text': 'To ensure optimal operation of the APOS Trainer program, a personal computer with CD-ROM drive running Windows NT 4 service pack 3 or newer is required, along with a monitor supporting a minimum 800 x 600 resolution. APOS, the Acoustic Positioning Operator System software, which controls HiPAP and HPR 400 Series systems, relies on a network card installed with TCP/IP protocols. The software, featuring a standard Windows graphical user interface, can be operated on an independent HiPAP or HPR Operator Station, an APC 10 computer for stand-alone systems, or a COS 100 unit within integrated systems.'}</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -7942,22 +7954,22 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HiPAP and HPR operation system is now available as a Trainer version supplied on a CD-ROM for installation on your own computer. The APOS Trainer is operated as a normal HiPAP/HPR system, where a simulator replaces the transceiver and the transponders. The APOS Trainer is suitable for training, planning and demonstration purposes. A typical LBL and SSBL operator presentation is shown in the figure to the right.'}</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Training and Simulation', 'text': 'The APOS Trainer, designed for comprehensive HiPAP/HPR operation, serves as a pivotal tool for training, planning, and demonstrating complex tasks. It comes loaded on a CD containing full APOS software with all options, excluding some specialized Offshore Loading System functions. The system includes a range of features: LBL positioning in the LBL array calibrated by the Trainer, an online Help function, sound velocity ray-trace calculation, SSBL positioning of transponders, telemetry communication, calibration of LBL arrays, and data output for testing interfaces to external computers.'}</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Precision and Planning', 'text': 'The APOS Trainer is instrumental in simulating various underwater positioning tasks. It aids in meticulously planning LBL arrays, providing an environment to explore different configurations and their effect on accuracy. Using this tool, operators can foresee the precision of their endeavors, whether they are positioning vessels within an LBL array or relocating SSBL transponders. The calibration of LBL arrays and sound velocity calculations are made simpler, helping operators anticipate and strategize for their missions.'}</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'APOS System Description', 'text': 'Both the HiPAP and HPR 400 Series systems are controlled and operated using the Acoustic Positioning Operator System (APOS) software, which runs on a Windows NT platform and features a standard Windows graphical user interface. Typically, APOS is operated on a HiPAP/HPR Operator Station or an APC 10 computer as a stand-alone system, and alternatively on a COS 100 unit within an integrated Dynamic Positioning (DP) system. The APOS Trainer program requirements include a personal computer with CD-ROM capabilities, a monitor with adequate resolution, and network configurations meeting set protocols.'}</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -8001,22 +8013,22 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The APOS Trainer brings the HiPAP and HPR operation system into an accessible format, offering the system as a Trainer version supplied on a CD-ROM for installation on your own computer. The APOS Trainer is operated as a normal HiPAP/HPR system, where a simulator replaces the transceiver and the transponders. It stands out for its utility in training, planning, and demonstration purposes.'}</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhancing Training with the APOS Trainer', 'text': "The APOS Trainer is not just a simulation; it mirrors the operation of an actual HiPAP/HPR system, integrating seamlessly with existing simulator components. Offering the complete HiPAP and HPR experience, the APOS Trainer is supplied with a CD containing full APOS software equipped with all standard options. This solution is defined with one HiPAP and one HPR 400 transceiver. It also includes features for LBL positioning calibrated by the Trainer and an SSBL transponder's relative positioning, delivering comprehensive simulated operational training."}</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Capabilities and Functionality', 'text': 'Features of the APOS Trainer extend to an array of practical functionalities, ranging from LBL and SSBL positioning, telemetry communication with transponders, to calibration of LBL arrays. The program includes a sound velocity ray-trace calculation and displaying of deflection based on velocity profile input. This suite of functionalities allows users to effectively examine positioning accuracy in different arrays and enables meticulous planning of LBL array configurations for enhanced precision in operations.'}</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Requirements and Integration', 'text': 'To run the APOS Trainer program, minimal system requirements must be met, including a personal computer with CD-ROM drive, running Windows NT 4 service pack 3 or newer, and a monitor with at least 800 x 600 resolution. A network card installed with TCP/IP protocols is also necessary. The APOS Trainer preserves the familiar graphical user interface of the APOS software and normally operates on a standalone system but can integrate into an APC 10 computer or a COS 100 unit in an integrated Dynamic Positioning (DP) and HiPAP/HPR system.'}</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -8060,22 +8072,22 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -8122,22 +8134,22 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'HUGIN is the most successful commercial Autonomous Underwater Vehicle (AUV) available. It combines IHO quality positioning with the highest resolution sensors on the market. HUGIN collects data from many different sensors concurrently, providing a comprehensive geophysical dataset from a single mission. HUGIN is equipped with swappable batteries and removable data storage enabling continuous operations.'}</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible and Comprehensive Data Collection', 'text': 'The HUGIN AUV System is a multi-role vehicle capable of collecting high resolution data for commercial, scientific and defense applications. It is the most flexible AUV available on the market, capable of carrying a wide array of sensors, including synthetic aperture sonars, multi-beam echo sounders, cameras, lasers, sub-bottom profilers and environmental/scientific sensors. Since the introduction in the 1990s, HUGIN AUVs have completed more commercial surveys than any other AUV and continues to deliver World leading performance.'}</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced In-Mission Capabilities', 'text': 'HUGIN also processes data in-mission, providing an autonomous pipe tracking capability, terrain navigation and target recognition. This makes the HUGIN the most flexible and productive platform for everything from geophysical surveys to mine countermeasures.'}</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Continuous Evolution and Deployment Flexibility', 'text': 'HUGIN has been continuously evolving since development began in 1991. From the first commercial survey in 1997, KONGSBERG and our partners at the Norwegian Defense Research Establishment (FFI) have been at the forefront of underwater robotic technology. HUGIN continues to deliver World-class performance and new capabilities and features are added through software updates and vehicle upgrades. HUGIN can be deployed from dedicated vessels, vessels of opportunity or from shore. The complete HUGIN system including operator consoles, launch and recovery system and the AUV itself can be delivered in DNV-certified offshore containers. The containers allow for transport by sea, air and land and mobilization is easy with only an external power connection required. Various container sizes are available to meet the customer needs.'}</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -8190,22 +8202,22 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The small and powerful HWS has been optimized for interface access and the ability to work with high data rates and graphics rendering of real time data from EM multibeam echosounders. The acquisition software Seafloor Information System, SIS, can create Digital Terrain Models (DTMs) from all soundings on-the-fly, and display a full point cloud or DTM in 2D and 3D.'}</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Hydrographic Work Station Capabilities', 'text': 'The HWS also serves as operator station for other KM products: SBP 27/29, TOPAS and EA440/640. It is a maritime certified computer system where all components have been tested together and verified to the standards IEC60945 and E10. The new generation HWS is smaller and faster than ever before, and can be used with all EM systems, SBP 27/29, TOPAS, and EA440/640. Maritime certifications include IEC60945 and E10.'}</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible Installation Options', 'text': 'Four standard installation options are available for the HWS: VESA-mount behind the display, VESA-mount under the desk, 19’’ rack mount fixed shelf, and 19’’ rack mount sliding drawer. Each installation offers unique advantages in terms of accessibility and space management, such as the ability to fasten the HWS under the desk, easy removal of the HWS from a fixed shelf, and the sliding drawer option providing effortless access to all components.'}</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Efficient Data Management and Add-Ons', 'text': 'MOVING THE DATA FROM THE HWS offers different methods such as USB-C for quick data transfer to an external disk, extra network connections for data transfer to another storage in the network, and options to remove the full HWS unit or replace external SSD drives for data offloading ashore. Additionally, HWS add-ons include external power units, SSDs for data transfer, optional network interfaces, and additional RAM, supporting tools like SBP 27/29, TOPAS, and EA single-beam echo sounders in various configurations.'}</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -8277,22 +8289,22 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The HAIN Subsea 7000 with co-located DVL is a fully integrated inertial navigation system for subsea vehicles. The system can be aided from acoustic positioning systems, doppler velocity and pressure sensors. The integrated solution designed for operation on an AUV, ROV, towed fish and any other subsea vehicle down to 7000 meters water depth, consists of an inertial measurement unit, doppler velocity log and onboard navigation processing. The HAIN unit receives the subsea vehicle position aid from an SSBL system on a surface vessel or a sparse LBL system on the subsea vehicle. In addition, to further improve position accuracy, the co-located DVL and pressure sensor 7000m rated can be used as aids to the inertial solution.'}</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Application Potential', 'text': "HAIN Subsea 7000 is designed to provide fast precise position updates with full attitude output for deep sea mining, cable trenching, ROV survey, AUV navigation and towed fish tracking. Seamless compatibility with HiPAP ensures the HAIN Subsea 7000's on board processor interfaces easily without the need for an additional topside computer. The new user-friendly HAIN interface is now accessible on HiPAP and uPAPAPOS operator stations."}</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Positioning Aids', 'text': 'Position aiding to HAIN can be provided by an SSBL system or via Sparse LBL ranges. A cPAPLBL Transceiver can be interfaced to the HAIN directly and measures LBL ranges to cNODE transponders on known seabed reference points. Fast absolute position calibration of seabed reference transponders is possible with an ROV adaptive box-in, with this technique the ROV is positioned with SSBL and HAIN, flying a circle around the seabed transponder while measuring LBL ranges. Relative position accuracy can be further improved with baseline measurements between the seabed transponders.'}</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Streamlined Vehicle Integration', 'text': 'Interfacing made easy: Connection and power to the aiding sensors is made directly via the HAIN unit with 3 x 24VDC and 1 x 12VDC outputs available. Therefore, only one connection is required between the vehicle and the HAIN system, simplifying connection to the vehicle MUX. Attitude output and 1pps time sync is also available from HAIN to multibeam, laser and navigation systems on the vehicle. Industry standard DVLs including Nortek and RDI can be co-located with the HAIN to improve the robustness of the INS position. The units can be pre-calibrated together with the HAIN post processing software prior to mobilization.'}</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -8351,22 +8363,22 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -8456,22 +8468,22 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The navigator’s eyes are always on watch. To replace or assist them a camera platform with uncompromising precision and reliability is needed. KONGSBERG Camera Cluster (KCC) delivers just this, in a compact and hard-wearing housing, with configurable 107 to 215 degrees coverage. We utilize the latest in machine vision CMOS technology, together with powerful edge processing, to enable crystal clear imagery.'}</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Uncompromising Maritime Imagery', 'text': 'KONGSBERG Camera Cluster (KCC) stands as an emblem of uncompromising precision and reliability for maritime navigation. Offering an exemplary broad coverage range that spans from 107 to 215 degrees, KCC is enclosed within a compact and durable housing. It embodies the cutting-edge machine vision CMOS technology along with advanced edge processing, paving the way for images that are exceptionally clear, aiding in maritime safety and surveillance.'}</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Performance Power', 'text': "The KCC 100 4D is designed not only to provide superior imaging but also to ensure efficient power management. Operating within a supply voltage range of 12-30 VDC, the system maintains a moderate mean power consumption of 35 W. KCC's performance is reflected in its ability to deliver image frame rates of 1/2/4 FPS and video frame rates of 24 FPS, using commonly used protocols and compression types such as JPEG, RTP, TCP, RTSP, H.264 and H.265."}</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Specifications and Compliance', 'text': 'The robustness of the KCC 100 4D is evident in its wide operational temperature range, extending from -20°C to +55°C, and a storage temperature range from -30°C to +80°C. Its resilience is further underpinned by an enclosure protection of IP56, demonstrating its capability to withstand challenging maritime environments. Meeting stringent standards and regulations, the KCC aligns with Electromagnetic Compatibility Compliance to EMCD and IEC 60945, and Product Safety Compliance to LVD, emphasizing its reliability and safety in maritime operations.'}</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -8532,22 +8544,22 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The KONGSBERG ProximityView offers dynamic stitching of several KONGSBERG KCC and such delivery a stiched 360 degrees camera coverage of the proximity zone overlaying sensor data into the view, such as: obstacles, distances, velocities, and planned path. The navigator can easily change between a simulated bridge view, birds-eye view, or other configurable views suiting a specific operation.'}</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Visualize the Situation', 'text': "The KONGSBERG ProximityView offers dynamic stitching of several KONGSBERG KCC, delivering a stitched 360 degrees camera coverage of the proximity zone. This coverage includes overlaying sensor data into the view, such as obstacles, distances, velocities, and planned path. It provides the navigator with the flexibility to switch between a simulated bridge view, a bird's-eye view, or other configurable views to best suit specific operating conditions."}</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Connectivity and Expansion Options', 'text': 'The system provides a host of connectivity and expansion options, designed to integrate seamlessly into different operations. It includes 4x Gigabit Ethernet on the rear I/O panel for network connections, 2x USB 3.0 headers for front panel access, 4x USB 3.0 ports on the rear I/O panel for multiple peripheral connections, 1x PS/2 KB/Mouse combo port for flexibility, and 2x Display port for high-resolution output.'}</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Physical Specifications', 'text': 'From a physical standpoint, the KONGSBERG ProximityView Processing Unit is both robust and compact, with dimensions of 90 x 392 x 380 mm, and a weight of 8 kg. The unit requires a supply voltage of 100-240 V AC 50/60 Hz, with a max power consumption of 200 W, and uses a Power Connector C13. These specifications have been carefully determined to meet operational needs while ensuring the ProximityView is ready for diverse environments and applications.'}</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -8591,22 +8603,22 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "The Maritime Broadband Radio (MBR) 144 is a smart antenna crafted for maritime applications where high-speed digital communication and data transfer are essential for effective and safe operations. With integrated antennas and complete enclosure, the MBR 144 is specifically designed for installation on both small manned and unmanned vessels. Featuring an integrated bracket for mounting on vertical or horizontal rails and a built-in GNSS sensor for absolute positioning, it's conveniently crafted with a slim design, simple one-cable connection, and straightforward vessel deployment."}</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Design and Installation', 'text': 'The MBR 144 stands out with its sleek and slim form factor, tailored for ease of deployment on various vessel types. Its design includes an integrated bracket, facilitating quick and effortless installation on vertical or horizontal structures aboard the vessel. Additionally, it boasts a single cable connection system that streamlines setup procedures. The robust enclosure of the MBR 144 is built to withstand the demanding conditions of maritime environments, ensuring durability and reliability for maritime operators.'}</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Exceptional Performance for Maritime Operations', 'text': "Operating within a frequency band configurable range and boasting an omni-directional 360 degrees azimuth antenna coverage, the MBR 144 provides a broad operational range, capable of handling user data throughput from 0.7 to 16.5 Mbps. The device's integrated antennas output a transmit power of up to 2 W with a maximum EIRP of 41 dBm, allowing for reliable and robust data communication over maritime distances. Ensuring high levels of performance, the MBR 144’s technical capabilities make it an indispensable tool for efficient maritime communication."}</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Built for the Maritime Environment', 'text': "Recognizing the challenging conditions of the maritime environment, the MBR 144 is engineered with a durable construction and features an ingress protection rating of IP 66. The unit's operational temperature range spans from -40 °C to +55 °C, ensuring dependable performance in extreme weather conditions. Moreover, to adapt to varying humid conditions at sea, it operates within a humidity range of 20 to 100% RH, solidifying its capability to function in the harsh maritime atmosphere without compromise."}</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -8667,22 +8679,22 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "The Maritime Broadband Radio, known as MBR 144, is a smart antenna developed specifically for maritime applications requiring digital high-speed and reliable communication for efficient and safe operations. Featuring full enclosure with integrated antennas, the MBR 144 is apt for installation on both small manned and unmanned vessels. The unit integrates a bracket for straightforward mounting on vertical or horizontal rails, and employs a built-in GNSS sensor for accurate absolute positioning. The MBR 144's sleek and compact design, coupled with a single-cable connectivity, simplifies deployment on vessels."}</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Effortless Installation and Deployment', 'text': 'The simplistic and efficient design of the MBR 144 promotes easy installation, made possible by an integrated mounting bracket that accommodates both vertical and horizontal rails. This innovation is further complemented by its slim profile, ensuring minimal spatial impact. With only a single cable required for connection, the MBR 144 showcases straightforward deployment, streamlining operational setup on various types of maritime vessels.'}</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Communication Capabilities', 'text': 'MBR 144 provides a seamless communication experience through its omni-directional antenna coverage that spans 360 degrees azimuth, ensuring unobstructed digital transmission across maritime environments. The system supports data transfer rates ranging from 0.7 to 16.5 Mbps, underlining its aptitude for high-speed operations. Its RF specifications are robust as well, with a frequency band stretching from 5725 MHz to 5850 MHz and a channel bandwidth of 20 MHz.'}</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliability and Compliance Standards', 'text': "The MBR 144 is not only built to deliver high performance but also crafted with reliability in mind. This is evidenced by an ingress protection rating of IP 66, which indicates a formidable defense against harsh environmental conditions. It operates within a temperature range of -40 °C to +55 °C and can withstand humidity levels of 20 to 100% RH during operation. Moreover, the MBR 144 complies with essential standards and regulations, including the RED directive 2014/53/EU, various ETSI, IEC, and FCC norms, in addition to DNVGL-CG-0339 and IACS E10. This adherence to regulations assures users of the quality and safety inherent in the MBR 144's design and functionality."}</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -8722,22 +8734,22 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where digital high-speed reliable communication and data transfer is crucial for efficient and safe operation. MBR 144 OEM is the low weight, compact version in the MBR family. Designed for customer specific integration, with a flexible form for easy fit into existing platforms. The antenna connections are connector-based, thus the antennas can be adjusted for the customer specific design.'}</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Integration and Design', 'text': 'MBR 144 OEM is characterized by its low weight and compactness, which makes it an ideal component within the broader MBR family for specialized usage. Facilitating customer specific integration, it boasts a flexible form factor that promotes seamless incorporation into existing platforms. Employing connector-based antenna connections, it allows for adjustments to align with various customer-speciﬁc designs, confirming its adaptability to fulfill tailored requirements.'}</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Efficient Operation and Coverage', 'text': "The MBR 144 OEM offers users a range of data transmission rates from 0.7 to 16.5 Mbps, ensuring high-speed, reliable communication for operational efficiency and safety. It features omnidirectional antenna coverage with a 360-degree azimuth, making it capable of delivering consistent communication irrespective of directional orientatation. This omnidirectional reach is critical for maritime operations where the vessel's orientation can change frequently."}</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Resilience in Maritime Environments', 'text': 'Engineered to endure harsh maritime conditions, the MBR 144 OEM can operate effectively across a wide temperature range from -30 °C to +55 °C and is designed to handle relative humidity from 20 to 100%. Its strategic design for enduring exposure to such environments is indicative of its robust construction, as reiterated by its ingress protection rating of IP41, ensuring that it remains protected against solid objects and limited ingress of water.'}</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -8785,22 +8797,22 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in maritime applications where digital high-speed reliable communication and data transfer are crucial for efficient and safe operations. The MBR 144 Submersible allows for resilient and long-range data exchange for surfaced subsea vehicles. The MBR 144 Submersible is certified for 1000m depth, and has integrated antennas. The sole connection to the MBR 144 Submersible is one connector for power and Ethernet.'}</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Resilient Maritime Communication', 'text': 'The MBR 144 Submersible is a breakthrough in maritime communication, enabling high-speed and dependable data transmission paramount for effective and secure maritime operations. Its specialized design provides unsurpassed resilience and long-range communication capabilities, particularly for surfaced subsea vehicles. Notably, the MBR 144 Submersible stands out with a certification for operation up to a remarkable depth of 1000m, emphasizing its reliability and robustness in challenging underwater environments.'}</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Integrated Design and Connectivity', 'text': "Engineered with integrated antennas, the MBR 144 Submersible epitomizes streamlined connectivity underwater. This smart antenna system simplifies connections by requiring only a single connector that serves dual purposes: powering the unit and enabling Ethernet connectivity. This elegant solution minimizes the complexity of subsea operations and maximizes the reliability of the marine broadband radio's performance."}</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Specifications Overview', 'text': 'The MBR 144 Submersible operates within the frequency band of 5725 MHz to 5850 MHz and boasts a channel bandwidth of 20 MHz, which is complemented by an antenna gain of 7 dBi. Its EIRP can reach up to 36 dBm, and the device supports GMSK modulation. Connectivity is facilitated through an Ethernet/LAN interface, ensuring seamless data transfer. The radio adheres to essential standards and regulations including RED directive 2014/53/EU, FCC ID, EMC, and is pressure rated to 1000m, highlighting its preparedness for rigorous maritime activities.'}</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -8872,22 +8884,22 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio (MBR) 144 Personal is a smart antenna crafted for the maritime environment where high-speed, reliable communication, and data transfer are essential for efficient and safe operations. Its compact design and tilted antennas are ideal for helmet mounting, making it conducive for operations where robust communication is necessary during surveillance and inspection. The device is equipped with integrated antennas and GNSS positioning, with optional accessories such as a dedicated plug-and-play camera for live streaming, and battery packs.'}</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Communication and Positioning', 'text': 'The MBR 144 Personal is engineered to deliver a reliable communication link crucial for maritime personnel engaged in surveillance and inspection tasks. To ensure superior performance, the MBR 144 Personal features omni-directional antenna coverage providing 360 degrees in azimuth, integrated antennas, and GNSS positioning capability. For applications requiring visual data, the system is also available with a dedicated plug-and-play camera for live streaming.'}</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Technical Design', 'text': "With user data transfer rates ranging from 0.7 to 16.5 Mbps and omni-directional antenna coverage, the MBR 144 Personal allows for continuous and expansive communication bandwidth. The unit's robust RF specifications include a frequency band ranging from 4900 to 5900 MHz, up to 2 W Tx power, and a high EIRP of max 40 dBm. Incorporating four internal antenna elements and the efficient GMSK modulation technique, the MBR 144 is designed for optimal performance."}</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable and Compliant Operation', 'text': 'Operating within a wide temperature range of -30 °C to +55 °C and capable of functioning in 20 to 100% relative humidity, the MBR 144 Personal is built to withstand harsh environmental conditions with an IP66 ingress protection rating. It adheres to rigorous standards and regulations including the RED directive 2014/53/EU and various ETSI and IEC standards for electromagnetic compatibility, radio, and environmental resilience, ensuring dependable performance in maritime operations.'}</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -8946,22 +8958,22 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in maritime applications where digital high-speed reliable communication and data transfer are crucial for efficient and safe operations. The MBR 144 Submersible allows for resilient and long-range data exchange for surfaced subsea vehicles. The MBR 144 Submersible is certified for 1000m depth, and has integrated antennas. The sole connection to the MBR 144 Submersible is one connector for power and Ethernet.'}</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Smart and Resilient Communication', 'text': 'The MBR 144 Submersible embodies the pinnacle of underwater communication technology, optimized for the unique demands of maritime applications. Its advanced design ensures robust and dependable high-speed data transfer that is indispensable for the successful execution of efficient and secure marine operations. Engineered to operate at depths reaching 1000m and sporting integrated antennas, the device is a tour de force offering unmatched resilience in submerged environments. Connectivity hassles are eliminated as it requires just a single connector, simplifying its interface to power and Ethernet. This feature signifies a new standard in streamlining data transfer processes below the surface.'}</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Next-generation Broadband Capabilities', 'text': 'Underwater operations demand unparalleled communication speeds, and the MBR 144 Submersible rises to this challenge by facilitating user data transmission ranging from 0.7 to 16.5 Mbps. It is defined by its oomni-directional antenna coverage across a full 360-degree azimuth, leaving no direction untouched. Its RF specifications include a substantial frequency band from 4900 MHz to 5900 MHz, and an antenna gain of 7 dBi, pushing the boundaries of underwater communication. The internal antenna elements numbering four, along with a modulation of GMSK and a configurability for the single 20 MHz channel, ensure that the MBR 144 Submersible stands out as a beacon of modern maritime communication technology.'}</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Built to Weather the Depths', 'text': "Sustainability and durability in extreme conditions are core to the MBR 144 Submersible's construction. Empowered to withstand the crushing pressures of depths up to 1000 meters, the technology is both awe-inspiring and reliable. Functionality does not waver over a wide operating temperature range of -30 °C to +55 °C and an operational humidity from 20 to 100 % RH, which is further testament to its resilient nature. Meeting stringent environmental specifications including a storage humidity recommendation of 20 to 70 % RH, the MBR 144 Submersible's readiness for the depths is unquestionable. Mastery over adverse environments is packed within this piece of technology, giving it the fortitude necessary to persist and perform below the waves."}</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -9021,22 +9033,22 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where digital high-speed reliable communication and data transfer is crucial for efficient and safe operation.'}</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Designed for UAV Integration', 'text': 'With only 85 grams, the MBR 144 UAV is tailored for lightweight UAVs, which require expanded operational range for command and control as well as a payload data link. The overall dimensions of the MBR 144 UAV makes it easy to integrate to many different UAVs with only power and Ethernet connection required. The antenna connections are connector-based, thus the antennas can be adjusted for the specific UAV design.'}</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Performance and Coverage', 'text': 'The MBR 144 offers a user data rate of 1 to 15 Mbps. The antenna coverage is omni-directional 360 degrees azimuth. In the RF specifications, the frequency band ranges from 4900 MHz to 5900 MHz with a channel bandwidth of 20 MHz. The transmission power reaches up to 2 W, and the antenna gain stands at 7 dBi, promoting an EIRP of max 40 dBm, using GMSK modulation. The antenna connectors number is 4.'}</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Power and Connectivity', 'text': 'The power supply voltage for the MBR Unit is at 5 V DC with a maximum power consumption of 25 W. When idle, the power consumption is 7 W. For interfaces, the MBR 144 UAV features an Ethernet/LAN port. Note that the configurable range for the single 20 MHz channel is subject to change without any further notice, indicating ongoing improvements and updates to the MBR 144 UAV system.'}</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -9097,22 +9109,22 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio (MBR) 179 MK2 is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. With beamforming, the MBR 179 provides steerable high-gain antenna direction in an omnidirectional sector, ideal for vessels and moving assets. The narrow fan-shaped antenna diagram ensures a strong link margin is maintained and is continuously updated as the unit remains unaffected by vessel movements.'}</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Gain, Omni-Directional Antenna Coverage', 'text': 'The MBR 179 MK2 delivers omni-directional 360 degrees azimuth antenna coverage. The beamforming capability of the MBR 179 MK2 allows it to focus the transmission, thus providing a steerable high-gain direction even within an omnidirectional sector. Resulting in reliable and potent communication links critical to maritime operations, it constantly adapts to movements, benefiting vessels and movable assets on the sea.'}</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Versatile Operational Performance', 'text': "The MBR 179 MK2 is engineered to perform across a range of applications, offering an operational range of up to 45 km and user data throughput between 0.7 to 16.5 Mbps. This powerful performance capability is maintained by a strong link margin and by the unit's ability to adjust its transmission dynamically—key factors for maintaining continuous and high-quality data transfer amidst the challenges of the maritime environment."}</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental and Regulatory Compliance', 'text': 'Built to endure the harsh conditions of the maritime environment, the MBR 179 MK2 operates well within a temperature range of -40°C to +55°C and is suitable for a humidity range of 20 to 100% RH operating and 20 to 70% RH during storage. It also meets essential industry standards and regulations including conformance to RED directive 2014/53/EU and EMC ETSI, along with environmental and product safety prescriptions. Its robust design is encapsulated by an IP66 ingress protection rating demonstrating its readiness to withstand the elements at sea.'}</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -9172,22 +9184,22 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation.'}</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Communication Capabilities', 'text': 'With beamforming, the MBR 179 provides steerable high-gain antenna direction in an omnidirectional sector, ideal for vessels and moving assets. With a narrow fan-shaped antenna diagram, a strong link margin is maintained and continuously updated as the unit is unaffected by vessel movements.'}</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust Environmental Adaptation', 'text': 'The MBR unit is capable of operating in a wide range of temperatures from -40°C to +55°C and can withstand humidity levels of 20 to 100% RH when operating, and 20 to 70% RH during storage. It boasts an ingress protection rating of IP66, indicating a high level of protection against dust and water.'}</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Compliance and Quality Assurance', 'text': 'The MBR is in conformity with various standards and regulations, including the RED directive 2014/53/EU, possessing FCC ID Q8IM179MK2, and meeting EMC standards ETSI EN 301 843-1 and 843-7. It adheres to safety and environmental protocols such as IEC 60945/EN 60945, DNVGL-CG-0339 (48 V DC), and IACS E10 (48 V DC).'}</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -9231,22 +9243,22 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MBR 179 MK2 Portable is a kit consisting of a MBR 179 MK2 radio, tripod and cables for quick deployment. The MBR Portable is delivered in two transportation hard cases and is perfect to use both on shore and on vessels which requires quick deployment for temporary operation.'}</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized for Effective Operations', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. With beamforming the MBR 179 provides steerable high-gain antenna direction in an omnidirectional sector, ideal for vessels and moving assets. With narrow fan shaped antenna diagram, a strong link margin is maintained and continuously updated as the unit is unaffected of vessel movements.'}</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ready for Deployment', 'text': 'The MBR 179 MK2 Portable enhances maritime communication capabilities by offering a portable solution that is easy to deploy. It accommodates the fast-paced needs of maritime operations requiring high-speed data transmission both on shore and at sea. Moreover, its robust design encapsulated in transportation hard cases assures safe and reliable transport, allowing for optimal performance regardless of the location.'}</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Adaptation and Durability', 'text': 'The MBR unit is engineered to withstand various environmental conditions. It operates efficiently across a wide temperature range from -40°C to +55°C and can withstand humidity levels from 20 to 100% RH during operation, with recommended storage humidity of 20 to 70% RH. The high ingress protection rating of IP66 certifies that the unit is well-protected against dust and powerful water jets, ensuring continuous operation even in harsh maritime conditions.'}</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -9286,22 +9298,22 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MBR 179 MK2 Portable is a kit consisting of a MBR 179 MK2 radio, tripod and cables for quick deployment. The MBR Portable is delivered in two transportation hard cases and is perfect to use both on shore and on vessels which requires quick deployment for temporary operation.'}</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Maritime Communication Redefined', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. With beamforming, the MBR 179 provides steerable high-gain antenna direction in an omnidirectional sector, ideal for vessels and moving assets.'}</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Connectivity', 'text': 'With narrow fan shaped antenna diagram, a strong link margin is maintained and continuously updated as the unit is unaffected of vessel movements.'}</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Portable Design', 'text': 'The MBR 179 MK2 Portable is designed to be robust and easy to transport, ensuring it can be quickly deployed in various maritime environments. It comes in two transportation hard cases, with the MBR unit weighing 8.8 kg and the cases weighing 17.6 kgs and 20.4 kgs respectively, making the system highly portable while maintaining durability.'}</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -9360,22 +9372,22 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio (MBR) 189 MK2 is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. This innovative technology is equipped with real-time beamforming, allowing the MBR 189 to adjust the antenna direction for every IP datagram transmitted within a sector of 100° x 100°. The operational sector can be increased by mounting multiple radios together, enabling up to 360° azimuth coverage. The MBR 189 is ideally suited for both maritime land-to-sea communication and for ground stations managing manned and unmanned aircraft operations.'}</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Efficiency Operation', 'text': "With advanced technology ensuring high-speed communication, the MBR 189 MK2 operates within a significant range of up to 50 km. It achieves user data transmission rates ranging from 0.7 to 16.5 Mbps. The MBR 189's adaptive beamforming technology is an asset that enhances the operational efficiency and safety of maritime as well as aerial communication systems. Its ability to form beams in real-time permits seamless and robust information exchange across critical service sectors."}</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Expansive Antenna Coverage', 'text': 'The MBR 189 MK2 offers impressive flexibility in terms of antenna coverage. A single MBR unit provides 100° azimuth x 100° elevation, but the coverage can be significantly expanded by linking multiple units. Two MBR 189 units cover an azimuth of 180°, three units expand to 270°, and with four units, the system achieves full 360° azimuth coverage. This adaptability makes the MBR an excellent choice for comprehensive area communication systems, providing versatile solutions to meet the demands of various operational settings.'}</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable Design and Compliance', 'text': 'The design of the MBR 189 MK2 meets strict environmental specifications with an operational temperature range from -40°C to +55°C, and it can handle a range of humidity from 20 to 100% RH during operation. The MBR unit is well-protected against the elements, meeting the IP66 ingress protection standard. Additionally, the MBR adheres to a series of standards and regulations, including the RED directive, EMC, radio standards, product safety, environmental standards, and DNVGL and IACS guidelines for maritime equipment. This resilience and compliance guarantee that the MBR is safe, reliable, and suitable for use in harsh maritime and aerial environments.'}</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -9443,22 +9455,22 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio MBR 189 MK2 is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation.'}</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimal Connectivity', 'text': 'With real-time beamforming, the MBR 189 adjusts the antenna direction for every IP datagram transmitted within a sector of 100° x 100°. This operational sector can be increased by mounting multiple radios together, giving up to 360° azimuth coverage.'}</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Application', 'text': 'The MBR 189 is suitable for maritime land-to-sea and vessel-to-vessel communication. It ensures robust and reliable data transfer crucial in maritime operations.'}</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Conformity and Standards', 'text': 'The MBR 189 MK2 is in conformity with RED directive 2014/53/EU and has the FCC ID Q8IM189MK2. It adheres to several EMC and Environmental standards, including ETSI EN 301 843-1, ETSI EN 301 843-7, and IEC/EN 60945, ensuring its safe operation within the maritime environment.'}</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -9498,22 +9510,22 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MBR 189 MK2 Portable is a kit consisting of a MBR 189 MK2 radio, tripod and cables for quick deployment. The MBR Portable is delivered in two transportation hard cases and is perfect to use both on shore and on vessels which requires quick deployment for temporary operation.'}</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust and Dependable Maritime Communication', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. With real-time beamforming, the MBR 189 adjusts the antenna direction for every IP datagram transmitted within a sector of 100° x 100°. This operational sector can be increased by mounting multiple radios together, giving up to 360° azimuth coverage.'}</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Maritime Connectivity', 'text': 'The MBR 189 is suitable for maritime land-to-sea and vessel-to-vessel communication, offering a flexible and effective solution for establishing robust links in a variety of maritime environments.'}</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Convenient Portability and Deployment', 'text': 'The MBR 189 MK2 Portable provides an ideal solution for situations that demand rapid setup and reliable maritime communication. The inclusion of two transportation hard cases facilitates the safe and practical transportation and storage of the equipment, ensuring the MBR Portable is always ready for immediate and temporary operational deployment.'}</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -9570,22 +9582,22 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MBR 189 MK2 Portable is a kit consisting of a MBR 189 MK2 radio, tripod and cables for quick deployment. The MBR Portable is delivered in two transportation hard cases and is perfect to use both on shore and on vessels which requires quick deployment for temporary operation.'}</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Maritime Communications', 'text': 'The Maritime Broadband Radio is a smart antenna designed for use in any application where resilient high-speed communication and high-capacity data transfer are crucial for efficient and safe operation. With real-time beamforming, the MBR 189 adjusts the antenna direction for every IP datagram transmitted within a sector of 100° x 100°. This operational sector can be increased by mounting multiple radios together, giving up to 360° azimuth coverage.'}</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Adaptable and Robust Design', 'text': 'The MBR 189 is suitable for maritime land-to-sea communication and for ground stations for manned and unmanned aircraft operations. It offers the flexibility needed for a wide range of operations, thanks to its quick deployment capability, making it an ideal choice for scenarios that demand reliable and fast establishment of communication links.'}</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Practical Portability and Protection', 'text': 'Ensuring the ease of transportation and the safety of the equipment, the MBR Portable is securely encased in two hard transportation cases. These cases are designed to protect and facilitate the delivery of the radio and associated components to any operation site, whether located on the shore or aboard a vessel.'}</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -9645,22 +9657,22 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Maritime Broadband Radio (MBR) 144 OEM is a low weight, compact variant in the MBR lineup, perfected for customer specific integration. Emphasizing a flexible form factor for seamless fit into existing platforms, the MBR 144 OEM features connector-based antenna connections to allow for customisable designs. This smart antenna is integral for applications that depend on high-speed, reliable communication and data transfer to enhance efficiency and safety during operations.'}</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Design and Performance', 'text': 'MBR 144 OEM stands out as the lightweight and compact version of the MBR series, ensuring easy integration into various platforms while facilitating customization for specific design requirements. The antenna operates with an omnidirectional 360-degree azimuth coverage and allows for a user data rate from 0.7 to 16.5 Mbps. Its power consumption is economical, requiring only 25 W at maximum and 6 W during idle, effectively reducing operational energy requirements.'}</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Robust Technical Capabilities', 'text': 'Catering to demanding communication standards, the MBR 144 OEM functions within a frequency band of 4900 MHz to 5900 MHz and provides a configurable range for the single 20 MHz channel. It utilizes GMSK modulation and has a transmission power capability of up to 2 W. The unit is equipped with 4 SMA antenna connectors, and can interface through Ethernet/LAN with an option for a second LAN connection.'}</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Durability and Compliance', 'text': 'The MBR 144 OEM is engineered to withstand harsh environmental conditions ranging from -30 °C to +55 °C and can operate within a relative humidity range from 20 to 100%. Its storage humidity is recommended to be within 20 to 70% RH. The MBR 144 OEM complies with the necessary RED directive 2014/53/EU and maintains conformity with various ETSI, IEC, and EN standards and regulations, highlighting its robustness and reliability for maritime operations.'}</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -9727,22 +9739,22 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The ME70 is a unique multibeam echo sounder that unites the quantitative functionality of split-beam echo sounders with the resolution and extended sampling volume inherent to multibeam systems. Purpose-built for water column data acquisition, it targets a range of subjects from fish and marine mammals to methane gas seeps and seafloor vegetation. The ME70 is optimized for fishery research applications, operating within 70 to 120 kHz and boasting 800 transmitting and receiving channels. Enhancing capabilities further, the standard system includes bathymetry functionality, furnishing high-resolution seabed mapping.'}</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Multibeam Scientific Echo Sounder', 'text': "The ME70 Multibeam scientific echo sounder excels in its operational flexibility. The system's suite includes a broad fan of stabilized beams ideal for fish behavior studies, fish school characterization, and similar research activities. A sector of beams can be designated as split beams to collect data for single target analysis like target strength measurements and tracking. Calibrated narrow split beams with reduced sidelobe levels and brief pulse durations make for accurate biomass estimation even near the bottom."}</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Functional Utility', 'text': "To augment the ME70 multibeam scientific echo sounder's utility value, two additional systems are on offer: a Bathymetric processor system for sophisticated seabed mapping and an Element Data Logger designed for high-volume element data collection. The bathymetry option transforms the ME70 from a specialized scientific instrument to a comprehensive multibeam echo sounder for seabed mapping, integrating extra hardware into the basic setup. Definitions of the ME70's publicly accessible output format are detailed in the product’s interface description and can be post-processed using either this documentation or commercial software applications like Echoview."}</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Sophisticated Operation and User Interface', 'text': 'The ME70 places emphasis on a suite of key functionalities ensuring sophisticated operation within its intuitive interface. It delivers control over transceiver input, sensor input, and information display, alongside capabilities for raw data recording with a network interface and replay of recorded echo data. Designed with low self-noise and options for remote control, data subscription, and custom user setting configurations, the ME70 promises clear and easily interpretable echo data. Comprising 25 transceiver boards, it offers a formidable 800 individual channels for comprehensive data acquisition.'}</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -9799,22 +9811,22 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'MULTI FUNCTION DISPLAY. This Multi Function Display (MFD 307) 7” is a maritime 10 finger capacitive touch panel computer. It can be used together with a variety of Kongsberg navigation products with a relevant application layer installed. It has been tested and approved according to IEC 60945. The design allows for different mounting solutions.'}</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Versatile Integration and Approvals', 'text': 'Some navigation products are wheel marked. For wheel marked products the display will include a software which is type approved in line with a performance standard. The MFD 307 PANEL COMPUTER is quick to install and easy to operate. Panel mount (flush), flange mount, DIN rail mount and RAM bracket mount are the available options for installation flexibility.'}</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seamless Communication and Optional Support', 'text': 'The communication between the display and the relevant navigation equipment is via Ethernet and/or serial line (RS-422). The serial line support is an optional variant of the product. The MFD 7” is available as OEM with Linux installed as a platform for third party applications and products, illustrating the MFD 307’s adaptability as a maritime panel computer.'}</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durable Design and Easy Operation', 'text': 'The MFD 307 PANEL COMPUTER is designed for diverse maritime environments and includes a variety of mounting solutions to suit different vessels and preferences, ensuring that users experience an easy operation. Its tested and approved build according to respected international standards emphasizes its reliability for maritime operations.'}</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -9893,22 +9905,22 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "The MGC (Motion Sensor &amp; Gyro Compass) is maintenance free when operated as an IMO type approved gyro compass and no field maintenance is required. However, recalibration considerations arise if the MGC is used as a roll and pitch sensor in addition to being a heading device, which is dependent on the sensor unit's use and operation mode."}</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Recalibration Requirements', 'text': 'The need for recalibration of the MGC sensor unit is determined by the application and operation mode it is configured for. A recalibration is recommended to maintain specified performance as changes occur in the internal sensors over time. Potential inaccuracies may grow without recalibration due to factors such as thermal cycling, vibration, and shock.'}</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Validity of Calibration Certificate', 'text': "Each MGC comes with an individual Calibration Certificate signaling compliance with the test requirements for the specific type of MGC, including the calibration date, but excludes an expiry date. Over time, without recalibration, there's increased uncertainty if the MGC remains within its original specifications."}</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'MGC Recalibration Process', 'text': 'If recalibration is necessary, the process involves contacting Kongsberg Customer Support for an RMA (Return Material Authorization) and following designated procedures. Turnaround time for recalibration is typically four weeks after the MGC is received, with an initial inspection within the first five days, although service needs uncovered during calibration may extend this timeframe.'}</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -9954,22 +9966,22 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'MRU 2, the fifth generation roll and pitch motion sensor, is designed for high accuracy roll and pitch measurements in marine applications. This unit, which must be fixed in a specific direction relative to the ship, is particularly suited for applications with a limited roll and pitch range. It is essential for many uses such as offshore riser monitoring systems, dynamic positioning systems, telecommunication antenna systems, and motion damping systems on high-speed crafts.'}</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Design and Output', 'text': 'The MRU 2 outputs both static and dynamic roll and pitch angles, along with corresponding angular rate vectors. Furthermore, it delivers surge and sway accelerations. Offering digital I/O protocols, MRU data can be accessed via Ethernet interface and serial lines which enable the easy distribution of data to multiple users on board. The advanced output options include two individually configurable serial lines, Ethernet/UDP, and ASCII-based NMEA 0183 proprietary sentences with data presented as IEEE 32-bit floats or scaled integers.'}</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Sensing Functionality', 'text': 'Boasting two highly precise accelerometers and MEMS angular rate gyros, MRU 2 is distinguished for its reliability that stems from solid state sensors without rotational or mechanical parts prone to wear. It comes with Windows-based software for configuration and data presentation. When positioned high up in a ship, such as on the bridge, the MRU 2 outperforms inclinometers and standard Vertical Reference Units due to its capability to suppress horizontal accelerations affecting roll and pitch measurements.'}</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durability and High Performance', 'text': 'The MRU 2 is a testament to durability and performance in maritime motion sensing. With a static accuracy of 0.08° RMS and dynamic accuracy for a ±5° amplitude of 0.1° RMS for roll and pitch orientation, it provides reliable data for marine operations. It also features a Mean Time Between Failures (MTBF) based on service history of 100000 hours and is constructed from robust anodized aluminum, guaranteeing long-term service in the demanding marine environment.'}</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -10041,22 +10053,22 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'MRU 3 is the fifth generation roll, pitch and heave motion sensor designed especially for heave compensation applications, such as for use with echosounders, fishing sonars and offshore cranes. This product stands out by delivering precise heave measurements that adhere to IHO standards, providing functionality critical for maritime operations.'}</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Sensor Technology for Precision', 'text': "This cost-effective MRU 3 model is built on 3-axis Micro-Electro-Mechanical-Structures (MEMS) sensors, providing accurate and reliable measurements for both linear acceleration and angular rate, thanks to solid state sensors with no rotational or mechanical wear-out parts. The MRU 3 also comes with a Windows-based configuration and data presentation software, which allows for defining vector arms from the MRU's mounted location to the centre of gravity (CG) and two configurable monitoring points. These precise outputs and configuration options make the MRU an invaluable tool for maritime operations."}</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Superior Data Integration and Output', 'text': 'MRU 3 stands out with its ability to deliver real-time roll, pitch, and heave measurements along with linear acceleration across three axes. The unit outputs heave position and velocity and the angular rate vectors for roll and pitch. With the latest PFreeHeave algorithm, MRU 3 can output correct and phase-free heave data, an advantage for applications such as seabed mapping. Utilizing external speed and heading input together with time synchronization features, the MRU 3 ensures improved accuracy even during vessel turns and accelerations.'}</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Connectivity for Various Applications', 'text': "Ensuring versatility for users, the fifth generation MRU is equipped with Ethernet interface and serial lines that allow for easy data distribution to multiple users on board the vessel. The unit boasts a high data output rate and compatibility with various digital I/O protocols, ensuring seamless operation with commonly used survey equipment. In addition, the MRU 3 features selectable communication protocols in its configuration software, underscoring the sensor's adaptability to specific maritime data systems and requirements."}</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -10139,22 +10151,22 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MRU 5 represents the pinnacle of marine motion sensing technology - embodying a specially designed fifth-generation device that excels in delivering high precision motion measurements within marine applications. It stands out in its ability to offer highly accurate roll, pitch, and heave measurements for the most demanding users.'}</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High Precision Applications', 'text': 'Primed for excellence, the MRU 5 is the optimal sensor for various motion compensatory functions used in multi-beam echo sounders, offshore cranes, hydroacoustic positioning systems, and dynamic motion monitoring on offshore structures. Its unparalleled roll and pitch accuracy of 0.02° RMS within a ±5° amplitude is proven and documented, ensuring reliable performance on any surface vessel or subsea vehicle.'}</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Sensor Technology and Configurability', 'text': 'Integrating three top-tier accelerometers with three premier Kongsberg Seatex developed MEMS gyros of MRG type, the MRU 5 exhibits low noise characteristics alongside exceptional bias stability and gain accuracy. This high reliability is attributed to the use of solid-state sensors, which circumvents any mechanical wear. Adding to its feature set, this unit comes with specialized Windows-based configuration and data presentation software, which allows for the precise definition of vector arms to the center of gravity and two individually configurable monitoring points.'}</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Data Output and Complementary Algorithms', 'text': 'The MRU 5 is proficient in the output of critical motion-related variables, such as roll, pitch, and yaw angles as well as angular rate vectors across various adjustable frames. Furthermore, with the employment of the cutting-edge PFreeHeave algorithm, it overcomes the perils of long swell conditions and is ideal for applications that can utilize a delayed heave signal, commonly observed in seabed mapping operations. External speed and heading inputs are also accepted to augment the accuracy of heave, roll, and pitch under dynamic conditions.'}</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -10194,22 +10206,22 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MRU 5+ product is upgraded with the best MEMS based gyro technology available. With exceptional low angle noise and bias stability, the product is ideal for integrated INS/GNSS systems and demanding survey applications.'}</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Precision and Reliability', 'text': 'The MRU 5+ provides documented roll and pitch accuracy of 0.008° and angle noise less than 0.002°. Every unit is delivered with an individual calibration certificate documenting this accuracy. This is made possible by use of accurate inertial sensors including three rate gyros and linear accelerometers of excellent tactical navigation grade performance. Very high reliability is achieved by using solid-state sensors with no moving parts and the proven MRU electrical and mechanical construction.'}</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Motion Sensing Technology', 'text': 'The PFreeHeave algorithm uses past measurements to output a correct and phase-free heave from MRU 5+. It has an advantage in long swell conditions and for applications that can utilize a heave signal that is delayed some minutes, typical for seabed mapping applications. Additionally, a new MEMS based gyro is developed by Kongsberg Seatex AS called MRG5 (Mru Rate Gyro) model 5. The MRG5 is optimized for use in high-end applications. The MRU rate gyro combines very low noise, excellent bias stability and outstanding gain accuracy and is the best MEMS rate gyro available for maritime applications.'}</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Integration and Application Flexibility', 'text': 'Interfacing the MRU 5+ to various sonar systems is made easy by including data protocols for the most commonly used multibeam echo sounder systems in the software. Using the configuration cable and the Windows version of the configuration software, MRC+, a series of simple menu prompts allow the user to choose the optimum configuration for his application. The MRU 5+ and the MRC+ software are flexible and can accommodate a wide variety of application types.'}</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -10283,22 +10295,22 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MRU D is the fifth generation roll and pitch motion sensor specially designed for marine applications, ideal for roll and pitch measurements on board ships. The sensor is paramount within voyage recording, dynamic positioning systems, fishing sonars, and telecommunication antenna systems. Its precise orientation requirements and limited range make it best suited for applications where consistent roll and pitch data are necessary. For applications requiring unrestricted mounting orientation or range, other MRU models with three-axis sensors are recommended.'}</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Design and Performance', 'text': 'For proper functioning, the MRU D unit must be mounted with the connector oriented vertically, and is best paired with systems that have a restricted range in roll and pitch motions. The accuracy of roll and pitch measurements remains unfazed even when the sensor is positioned away from the vessel Center of Gravity (CG) thanks to its ability to reduce the impact of horizontal acceleration on performance. This advanced suppression ability sets the MRU D apart from standard inclinometers, pendulous units, and Vertical Reference Units. Moreover, every MRU D device comes with a Calibration Certificate, affirming its tested precision and compliance with stipulated standards.'}</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Adaptability and Convenience', 'text': "Data from the MRU D is readily available through distinct communication channels including serial lines and an Ethernet interface, ensuring easy distribution to multiple onboard users. The data outputs are adjustable and can be transmitted in different formats such as IEEE 32-bit floats or scaled integers. Additionally, the sensor can furnish NMEA 0183 proprietary sentences, illustrating its compatible use within varied digital interfaces. The MRU D is accompanied by user-friendly Windows-based configuration software that, when set up with the correct vector relation to the vessel's Center of Gravity, enhances the sensor's output precision."}</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Data Output Features', 'text': 'The MRU D is equipped to deliver real-time roll and pitch information, maintaining a high data output rate of up to 200 Hz. It demonstrates high reliability with no scheduled maintenance and the absence of parts prone to mechanical wear. Despite its robustness, the MRU D maintains a small and efficient form factor with lightweight design and modest power consumption. This sensor supports different communication protocols, which can be selected through its configuration software, providing versatility for onboard integration without the need for an export license.'}</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -10338,22 +10350,22 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'MRU E is the fifth generation roll, pitch, and heave motion sensor with an extended temperature range, making it ideal for marine applications. It is designed to function in ambient temperatures ranging from -25 to +70°C. Suitable for installation in various locations such as open decks, cabinets, or bulkheads, MRU E is an essential component for systems that require accurate motion measurements.'}</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized for Helideck Monitoring Systems', 'text': 'The MRU can be strategically positioned directly beneath the helideck center to measure 3-axes linear accelerations along with roll, pitch, and heave, crucial for Helideck Monitoring Systems. It serves to inform about the helideck location when it is apart from accommodation and the hull areas. Complying with HCA requirements, the MRU E measures helideck acceleration to calculate the Motion Severity Index (MSI), an important safety metric in marine operations.'}</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Specialized Algorithms for Enhanced Performance', 'text': 'The MRU E utilizes the PFreeHeave algorithm to deliver a precise and phase-free heave measurement based on past data. This functionality is particularly beneficial in long swell conditions, and is essential for applications such as seabed mapping that can accommodate a slight delay in the heave signal. To ensure the greatest accuracy in heave, roll, and pitch, especially during turns and accelerations, the sensor accepts external inputs, including separate speed and heading information via serial lines or Ethernet.'}</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliable Data and Communication', 'text': 'Incorporating solid state sensors to ensure high reliability, MRU E avoids moving parts by using three accelerometers and three MEMS angular rate gyros. With specialized mounting brackets designed for outdoor use, this sensor stands up to harsh marine conditions, including weather and sea spray. The fifth-generation MRU offers data via Ethernet interface and serial lines, supporting easy data distribution and a variety of survey equipment protocols, enhancing operational efficiency and flexibility onboard vessels.'}</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -10421,22 +10433,22 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'MRU H, the versatile heave compensator, represents the fifth generation MRU specially designed for heave compensation applications. As an ideal sensor for a range of marine applications requiring highly accurate heave measurements, this unit enhances the precision in environments with extreme horizontal accelerations.'}</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhanced Applications and Output Variables', 'text': 'The MRU H is an essential instrument constructed for precise motion measurements in marine environments. With applications that stretch from offshore cranes to echo sounders, it is also valuable for ship motion monitoring, helideck motion monitoring, hydroacoustic positioning systems, and hull stress monitoring. Its output encompasses significant data such as roll, pitch, and heave alongside linear acceleration in 3-axes, enabling accurate heave position, velocity, and acceleration in adjustable frames with additional outputs like angular rate vectors.'}</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Functionality and Algorithm Utilization', 'text': 'Embodying three accurate accelerometers and MEMS angular rate gyros, the MRU H achieves remarkable reliability with no rotational or mechanical wear-out components. A distinctive feature of its function is the PFreeHeave algorithm, which uses historical measurements to deliver a precise, phase-free heave signal. This is especially beneficial in conditions of long swell or for seabed mapping applications that can utilize slightly time-lagged heave signals.'}</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Seamless Configuration and Data Integration', 'text': "Accompanied by user-friendly Windows-based configuration software, the MRU H allows for meticulous calibration of monitoring points and alignment with the vessel's center of gravity. It offers multi-point heave measurement outputs and compatibility with various protocols for seamless data sharing across multiple users. This capability underscores its adaptability to diverse operational needs while ensuring widespread accessibility through established data communication standards."}</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -10476,22 +10488,22 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The MRU S roll, pitch and heave motion sensor is specially designed for fish finding equipment. It incorporates advanced Micro-Electro-Mechanical-System (MEMS) sensors for both linear acceleration and angular rate, ensuring high reliability with solid state sensors that have no rotational or mechanical wear-out parts. Designed to perform even in rough weather conditions, MRU S provides vital vessel motion data for an undisturbed display on the fish finding equipment.'}</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Enhancing Sonar Efficiency', 'text': "Typically utilized for real-time compensation of roll, pitch, and heave data in fishery sonars and echosounders, the MRU S significantly improves the quality of underwater acoustic images. The output variables like roll, pitch, and heave, along with linear acceleration and angular rate, contribute to a clear and reliable display irrespective of wave motion induced distortions. The sensor's performance is crucial for operations conducted in challenging sea conditions."}</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Connectivity and Output', 'text': 'The MRU S is capable of delivering data through an Ethernet interface and serial lines, providing flexibility for on-board data distribution among multiple users. Customizable output protocols support a variety of sonar equipment and enable simultaneous heave measurements at different points via a single serial line or Ethernet port. This versatility ensures that the MRU S can integrate seamlessly with a diverse array of marine electronic systems.'}</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliability and Customization', 'text': 'This cost-effective sensor offers a high data output rate, crucial for real-time applications, and is complemented by a small form factor, lightweight and low power consumption. Supplied with a Calibration Certificate and a 2-year warranty, the MRU S guarantees accuracy and dependability. The accompanying Windows-based configuration software permits users to personalize communication protocols and compensate for lever arm effects to adjustable monitoring points.'}</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -10566,22 +10578,22 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "The MS70 is a high resolution Multibeam scientific sonar with very low sidelobe levels. It is designed for collection of data from the water column. The MS70 offers a new dimension to fishery research. As a school of fish changes shape and density constantly, the MS70 is the best possible tool to understand these dynamics with remote sensing. The MS70 was the world's first quantitative multibeam sonar for fishery research applications."}</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Sonar Capabilities', 'text': 'The MS70 Multibeam scientific sonar is designed for high operating flexibility. It provides an acoustic matrix of stabilized and calibrated beams for biomass estimation, fish school characterization and behaviour studies. Within the bandwidth of the transducer, the limits for beam steering, and the minimum achievable beam opening, you can select the directions, frequencies, and opening angles for the beams. You can set up the system to fit your requirements, and it will provide you with a real-time display for quality control of the current data acquisition.'}</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'School of Fish Detection and Analysis', 'text': "The MS70 allows characterization and volume estimation of a school of fish using only one single transmission. Schools of fish can be tracked, followed, and studied using multiple consecutive transmissions. As a consequence of the horizontal transmission using narrow beams, the MS70 allows you to detect and characterize schools of fish even very close to the sea surface. A typical screen capture is provided, showing a school of herring in both horizontal and vertical views, demonstrating the system's practical utility in fishery research."}</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Features of the MS70', 'text': 'It offers unique features for modern research vessels and environmental monitoring installations that require high quality scientific data. The frequency range of 70 to 120 kHz, a horizontal operating sector of 60°, and a vertical operating sector of 45°, along with low self-noise and remote control capabilities, positions the MS70 as a leader in its class. Its clear and easily comprehensive echo data, intuitive user interface, and definition and saving of user settings accentuate its ease of operation.'}</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -10621,22 +10633,22 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "The Flexview, KONGSBERG's latest advancement in multibeam sonar technology, is designed specifically for small observation class ROVs where compact size and light weight are key selection criteria. Delivering superior image quality and coverage, the Flexview multibeam sonar provides high-quality distortion-free images over a 140° sector, reducing the time it takes to search for and locate targets. Two versions of the Flexview are available."}</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative Design and Functionality', 'text': 'The Flexview’s removable transducer is the first of its kind, offering field replacement of a damaged transducer in the unlikely event of a catastrophic impact. It also allows for potential new transducer configurations to be exchanged in the future, depending on the job being performed. Mosaic image merged from 7 passes.'}</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Frequency Flexibility', 'text': 'The Flexview is offered in two versions to suit varying operational needs. The Flexview – FLEXVIEW HF (High Frequency) version provides 70 m coverage over a 140° sector, yielding higher resolution images at short range. Conversely, the Flexview – 500 kHz version affords 200 m coverage over the same sector, ensuring high-resolution images at longer ranges. Both versions maintain the ideal suitability for small observation class ROVs.'}</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence and Adaptability', 'text': 'Not only do both versions of the Flexview generate distortion-free images at a high update rate, but they also feature a user-friendly interface and a low-profile wet mateable connector. With CHIRP and Doppler modes of operation available, operators stand to gain significant time savings in a variety of applications including search and recovery, marine engineering, site inspection, environmental monitoring, site clearance, and underwater science.'}</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -10676,22 +10688,22 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The innovative design of the M3 Sonar® uses two sets of complementary transducers which allow it to generate both imaging and bathymetric data with the same head. Unique to the M3 Sonar® is the patented eIQ (enhanced image quality) mode of operation that generates multibeam images with unprecedented clarity.'}</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Imaging and Bathymetry', 'text': 'Multibeam sonar - M3 Sonar empowers users by generating imaging and bathymetric datasets from one sonar head. It achieves single-beam image quality with the speed of multibeam. Offering GeoTIFF output, the system can create real-time mosaic using third-party software, compliant to IHO Special Order &amp; 1A. With Linear FM, CW and Doppler pulses, the benefits of this sonar include a high update rate, significant time savings, uniform large coverage area, MultiMode capability, low power consumption and user-friendly operation.'}</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Flexible Configuration and Outputs', 'text': 'The M3 Sonar has the ability to configure applications using complex pulses like interleaving active pings and passive listening modes, Doppler, and multiple true-zoom windows with linear FM and CW imaging modes of operation. Data outputs are compatible with various third party software such as Caris, EIVA, Hypack, and QINSy. In addition, the ability to produce real-time 3D point clouds enables rapid target or object detection, ideal for shallow water surveys on USV/ASV/ROV and dual head deployment.'}</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'High-Level Precision and Compliance', 'text': 'IHO compliance of the M3 Sonar ensures vertical accuracy meeting the full ±60° sector for Order 1 surveys and at least ±55° for Special Order. Special Order target detection (1m cube) is met to 20m and Order 1A target detection (2m cube) is maintained to 40m. Applications of M3 Sonar are varied and include Marine Engineering &amp; Site Inspection (MESI), Search &amp; Recovery (SAR)/Security, Underwater Vehicle Instrumentation (UVI), and Environmental Monitoring.'}</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -10743,22 +10755,22 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "NavLab, known for its consistent software enhancements and active versioning, introduces its software release notes for several significant improvements and additions, particularly starting with Release 4.5.2. New capabilities such as added 'preproc' and documentation for ZUPT sensor, latitude-sensor for pressure to depth configuration, and a range of fixes and improvements have been implemented. Regular updates like these ensure the software remains at the cutting edge of navigation and positioning technology."}</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Improvements', 'text': "NavLab's commitment to continuous improvement is evident from its array of advancements. Noteworthy improvements include descriptive status messages in HAIN's status plot, the ability to perform proportional pressure to depth calculations, and sensor customization options enhancing the overall user experience. The latitude sensor now utilizes the first valid position sensor or is configurable, ensuring more accurate depth calculations. Furthermore, program stability has been enhanced with a fix that prevents crashes when changing sensor selections."}</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Notable Fixes and Enhancements', 'text': 'Release 4.5.1 brought important fixes such as the prevention of pressure error display in the absence of CTD profiles and the ability to export at different frequencies. Increments in performance, improved user interface displays, and wild-point plot updates are some of the speed and functional advancements made in this release cycle. One of the key highlights includes the repair of installation issues encountered in P-code, streamlining the setup process substantially.'}</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advancements in Usability', 'text': "Release 4.5.0.0 introduced changes to licensing dongles that enhance security and software management. With an aim to elevate user interaction, a new user interface now exhibits improved status and progress oversight. Further, Release 4.4.2's inclusion of a Simulator and ZUPT as a sensor are prime examples of NavLab's dedication to expand functionality. Release 4.2.1 saw improvements like Tide level being added as a separate sensor, refining pressure to depth calculations."}</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -10816,22 +10828,22 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -10880,22 +10892,22 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Kongsberg Blue Insight is an open and flexible digital infrastructure product designed to meet the increasing demand for accurate information from the oceans, focusing on internet security and seamless integration. The Blue Insight automates the data stream from a wide range of sensors and platform types and visualizes them in a common framework. The solution facilitates modern data processing and machine learning, providing new understanding and in-depth knowledge.'}</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Key Benefits of Blue Insight', 'text': 'Blue Insight offers a one-stop solution that provides a real-time overview across platforms and data types. It is highly flexible and scalable, suitable for both small and large organizations, and fosters an open ecosystem built on FAIR data principles. Furthermore, Blue Insight facilitates deployment of customized machine learning algorithms and ensures cybersecurity, adding substantial value to any organization in need of robust and reliable ocean data management.'}</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Blue Insight Core Module', 'text': 'The Blue Insight Core module provides solutions for secure interactions between sensor platforms, cloud storage, and data management enabled by the industrialized Internet of Things modules found in the Kognifai digital ecosystem. It includes required common functionality to prepare data for automated analytics and advanced data handling, along with a basic visualization framework with dashboard functionalities and graph view of data. This foundational module integrates with existing IT systems and is essential for deploying other Blue Insight modules.'}</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Specialized Modules of Blue Insight', 'text': 'Blue Insight features specialized modules tailored to enhance the functionality of the core system. Sensor Fusion is an on-premise application optimizing data from sensors for streamlined cloud distribution. The Data Forwarder module handles data conversion and sharing across platforms. Sensor Remote offers a web interface for remote sensor control, while Ocean View allows for real-time and historic data visualization. The Analytics module provides in-depth data handling and machine learning infrastructure for sophisticated ocean data analysis and algorithm deployment.'}</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -10939,22 +10951,22 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The PI Portable Hydrophone is provided for temporary use. The portable hydrophone is if you wish to use your catch monitoring system right away without docking for hydrophone installation.'}</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease of Use', 'text': 'You can connect the hydrophone directly into the connector on the receiver, and lower the hydrophone over the rail. The hydrophone has an omnidirectional beam and a 50 meter integrated cable.'}</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Durability and Convenience', 'text': 'The cable is sheathed in polyurethane providing robust external protection to complement its 150 kg tensile strength. The cable is supplied on a reel for convenient retrieval and storage.'}</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Support and Contact Information', 'text': "The 'Simrad' brand name is owned by Kongsberg Maritime. All Simrad products are thus supported by Kongsberg Maritime. We offer world wide support and training on our professional fish finding and… Simrad contact informationHere is the relevant contact information for Simrad professional fish finding and underwater science systems."}</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -10994,22 +11006,22 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'As the name implies, the Simrad PI Purse Seine hydrophone is designed for use by purse seiners. The purpose of the hydrophone is to provide the best possible communication with the wireless sensors located on your purse or danish seine.'}</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Reception Features', 'text': 'You can use one or two hydrophones pointing towards the net. Both are hull-mounted. The hydrophone has a 90 degrees horizontal beam and a 30 degrees vertical beam. This provides the catch monitoring system with optimal reception from the wireless sensors on a purse seine. The beam pattern is especially suited for purse seining. The wide coverage area reduces the need for careful alignment.'}</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Comprehensive Support and Updates', 'text': 'Stay in touch for product information and software updates. Join us on Facebook, follow us on Twitter, and visit us on LinkedIn. The "Simrad" brand name is owned by Kongsberg Maritime. All Simrad products are thus supported by Kongsberg Maritime. We offer world wide support and training on our professional fish finding and…'}</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Purchase and Contact Information', 'text': 'Where to buy Simrad products: If you want to purchase Simrad equipment you can rely on a world wide sales organization. Support Simrad Products: Simrad contact information: Here is the relevant contact information for Simrad professional fish finding and underwater science systems.'}</t>
         </is>
       </c>
       <c r="G142" t="inlineStr"/>
@@ -11041,22 +11053,22 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The Simrad PI Trawl Hydrophone is dedicated for bottom and pelagic trawlers, designed to provide the best possible communication with the wireless sensors located on your pelagic or bottom trawls.'}</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Optimized Hydrophone Placement', 'text': 'For effective utilization, you can use one or two hydrophones pointing towards the aft of the vessel, but it is critical to pay attention to the noise generated by the propellers. Each hydrophone is meticulously hull-mounted to ensure quality communication.'}</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Beam Pattern Design', 'text': 'The Trawl hydrophone is engineered with a 50 degrees horizontal beam and a 30 degrees vertical beam, providing the catch monitoring system with optimal reception from the sensors on a bottom or pelagic trawl. This beam pattern, particularly suited for trawling, offers wide coverage and reduces the need for careful alignment.'}</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Support and Customer Engagement', 'text': "The 'Simrad' brand, owned by Kongsberg Maritime, ensures that all Simrad products are supported by Kongsberg Maritime’s world-wide support and training services. For additional product information and software updates, engage with us on social media platforms like Facebook, Twitter, and LinkedIn, or visit our official website."}</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -11096,22 +11108,22 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'M3 SONAR PHS is a state-of-the-art SHALLOW-WATER PORTABLE HYDROGRAPHIC SURVEY SYSTEM designed for a variety of undersea mapping and survey applications. Efficient and reliable, it features an M3 Sonar with a 500 kHz operating frequency and a depth rating of 500 meters, ideal for capturing detailed data in shallow water environments.'}</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'M3 Sonar Capabilities', 'text': 'M3 Sonar operates at a frequency of 500 kHz, capable of scanning depths ranging from 0.2 to 50 meters. It boasts a swath width of 120° and sharp beam widths offering a transmitter angle of 3° and receiver angle of 1.6°. With the ability to generate up to 256 beams, the sonar uses both Continuous Wave (CW) and Frequency-Modulated (FM) pulse forms. This advanced system achieves an effective pulse length ranging from 10 μs to 10 ms and can achieve a maximum ping rate of 40 Hz, all encased within durable materials like Hard Anodized Aluminum, Stainless Steel 316, and Elastomeric Polyurethane.'}</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Advanced Integration and Portability', 'text': "The M3 Sonar Interface Unit enhances the survey system with its splashproof design, serving as a junction box and supplying power seamlessly to all external sensors, including the sonar head. This integration simplifies cable management and enhances the system's portability, ensuring all equipment functions effectively in the demanding field conditions."}</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Precision Positioning and Mounting Solutions', 'text': 'Seapath 130 Series is a compact solution providing Integrated INS/GNSS for Heading, Attitude and Positioning, with no accuracy degradation during movements. This includes 120 channel dual frequency GPS/GLONASS receivers and an array of correction options. The Series offers different models, such as the Seapath 130-3 and 130-H, with varying levels of accuracy for roll and pitch, and the positioning system is complemented by the MRU-3 and MRU-H units, offering fine angle resolution and heave accuracy. The Pole Mount (USM Compact) is a durable over the side compact pole mount providing a secure base for the sonar head, MRU, and speed sound sensor.'}</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -11227,22 +11239,22 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'Every PX family sensor is equipped with a custom-made Li-Ion battery, which is a vital component for their operation. To facilitate the charging of this battery, the PX MultiSensor Charger has been specifically designed. This charger is an integral piece of equipment that ensures the PX sensors are powered and ready for use.'}</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Charging Necessities', 'text': "The PX MultiSensor Charger is essential as it must be used to charge all PX family sensors. It's important to charge the catch monitoring sensors between operations to maintain their functionality. The design includes a special plug that prevents shortcuts or incorrect connections, providing a safer charging experience."}</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Automatic Charging and Battery Care', 'text': "The charging process is fully automatic, requiring minimal intervention. When the sensor is fully charged, the charging current is restricted to prolong the battery's lifespan. It's recommended to perform charging within a temperature range of +5 to +45°C (+41 to +113°F) to ensure optimal battery care."}</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Safety Measures and Usage Parameters', 'text': 'The battery charger is exclusively for use with the sensor battery of the PX family, highlighting the specificity of the product. Charging the sensor below 0°C (32°F) is not advised; however, the charger incorporates a safely mechanism that protects the sensor during attempted charges in sub-zero temperatures.'}</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -11282,22 +11294,22 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'RADIUS 2000 is a high precision relative positioning reference system designed for DP applications requiring robust and reliable relative positioning. It is a fully solid state system with low maintenance costs, developed for multiple users leveraging the same transponders simultaneously.'}</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative technology', 'text': 'RADius is an inventive system based on radar principles, consisting of solid state components and advanced signal processing which allows for simultaneous and continuous measurements to any practical number of transponders. With the capability to support multiple sensor heads, RADius can operate as an omnidirectional system providing full 360˚ signal acquisition and prevention of blind angles. It is equipped with an intuitive touch-ready HMI for ease of use during operations.'}</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Excellence', 'text': 'The RADius system delivers operational excellence with autodetecting transponders, a wide vertical operational sector of 100°, and the ability to measure accurate range and bearing to any transponder within a range of up to 550 metres. Additionally, the system furnishes a variety of transponders suitable for any operation that demands a robust and dependable relative positioning solution.'}</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Reliability and Certification', 'text': "Ensuring continuity and high availability, RADius is recognized for its no moving parts, easy installation, and capability to operate under all weather conditions. Moreover, the system's transponders are compliant with multiple certification standards, including ATEX, IECEx, Inmetro, and UL, thus making them suitable for use in hazardous offshore environments."}</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -11343,22 +11355,22 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'RADius is based on radar principles and the system is developed for DP applications in need of robust and reliable relative positioning. It is a fully solid state system with low maintenance costs.'}</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Innovative Technology', 'text': 'The implementation of RADius is fully solid state and relies on interferometric measurements of reflected radar signals from various passive transponders within the nearby area. Each reflected signal incorporates a unique ID, enabling separate identification of different targets. Advanced signal processing capabilities of RADius allow for simultaneous and continuous measurements to any practical number of transponders, fostering an environment where multiple users can leverage the same transponders simultaneously.'}</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Ease-of-Use HMI', 'text': 'RADius features a highly intuitive touch-ready Human Machine Interface (HMI) developed collaboratively with seasoned DP operators. This user-friendly interface delivers the functionality for operators to quickly and effectively assess the quality of their positioning during operations. The HMI offers a selection of color palettes to cater to varying light conditions, as well as a night display mode, ensuring better visibility and usability.'}</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Operational Features', 'text': "RADius boasts the capability to detect and accurately measure the range and bearing to any transponder within a span of up to 550 meters, subject to the target's transponders. A suite of operational features includes autodetecting transponders, wide opening angles for stable maneuvering in close operations, and the diversity of retroreflective transponders available to suit different operational demands, signaling a reliable and robust relative positioning solution."}</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -11433,22 +11445,22 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius 550X transponder is a part of the short-distance relative positioning system RADius, developed for use in applications where the need for a robust and highly accurate relative positioning system is crucial. The lightweight portable transponder is easy to deploy on targets for applications that require range and bearing during operation.'}</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'EX certified', 'text': 'The RADius 550X low power transponder is an intrinsically ATEX safe product (category 2) suitable to be installed in hazardous locations where there may be an explosive mixture of flammable gases belonging to gas groups IIB and/or IIA. The transponder can be used in hazardous zones 1 and 2. IECEx classification is Ex ib IIB T4 Gb.'}</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Battery powered', 'text': 'The RADius 550X is powered from an intrinsically safe encapsulated battery with an integral current limiting resistor and has no wired connection to external equipment.'}</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Unique ID', 'text': 'The transponders are coded with unique IDs ensuring reliable identification and tracking of vessels in demanding environments. Several interrogators can approach the same transponders, ensuring multi-user capabilities. Up to five transponders can be tracked simultaneously by the interrogator. The transponder is suited with dip switches for easy setting of the transponder ID.'}</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -11527,22 +11539,22 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius 600X transponder is a part of the short-distance relative positioning system RADius, developed for use in applications where the need for a robust and highly accurate relative positioning system is crucial. RADius 600X is suitable for large installations like offshore platforms, FPSOs and similar where DP operated vessels typically will approach the installation.'}</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'EX Certified', 'text': 'The RADius 600X high gain transponder is an intrinsically ATEX safe product (category 2) suitable to be installed in hazardous locations where there may be an explosive mixture of flammable gases belonging to gas groups IIB and/or IIA. The transponder can be used in hazardous zones 1 and 2. Temperature class is T4.'}</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Fixed Power', 'text': 'The RADius 600X is powered from a power supply located in a safe (non-hazardous) location and an EX type approved zener barrier is used to limit the delivered energy to the hazardous location to a safe level. The barrier - located in a safe area - will prevent any hazardous voltage or excessive current from reaching the hazardous zone. For long cable runs an alternative approved power solution can be delivered.'}</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Unique ID', 'text': 'The transponders are coded with unique IDs ensuring reliable identification and tracking of vessels in demanding environments. Several interrogators can approach the same transponders, ensuring multi-user capabilities. Up to five transponders can be tracked simultaneously by the interrogator.'}</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -11607,22 +11619,22 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius 700 transponder is a part of the short-distance relative positioning system RADius for use in applications where the need for a robust and highly accurate relative positioning system is crucial. RADius 700 has an operating range of up to 1000 metres.'}</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Easy to Deploy and Operate', 'text': 'The RADius 700 transponder is easily deployed as the unit runs on internal batteries, thus, no cable connection is necessary. The replaceable internal Lithium battery has an estimated life time of three years. ON/OFF switching is easily done by inserting/removing the activation plug at the back of the transponder. The operating sector of the unit is 90° horizontally and vertically.'}</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Unique ID and Tracking', 'text': 'The transponders are coded with unique IDs ensuring reliable identification and tracking in demanding environments. Several interrogators can approach the same transponders, ensuring multi-user capabilities. Up to five transponders can be tracked simultaneously by the interrogator. The transponder is suited with dip-switches for easy setting of the transponder ID.'}</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Conditions and Compliance', 'text': 'The RADius 700 transponder is designed to operate robustly in a variety of environmental conditions. It has a humidity operational range of 100% RH and a storage recommendation of 60% RH. The ingress protection rating is IP 66, making it highly resistant to dust and water. It operates in temperatures ranging from -40 °C to +60 °C while the recommended storage temperature ranges from +5 °C to +30 °C. Compliance with the Radio Equipment Directive (RED) 2014/53/EU ensures adherence to regulatory standards.'}</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -11684,22 +11696,22 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius 700X transponder is a part of the short-distance relative positioning system RADius, developed for use in applications where the need for a robust and highly accurate relative positioning system is crucial. RADius 700X is suitable for large installations like offshore platforms, FPSOs and similar where DP operated vessels typically will approach the installation, and where ATEX certification is required.'}</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'EX Certified', 'text': 'The RADius 700X transponder is an intrinsically ATEX safe product (category 2) suitable to be installed in hazardous locations where there may be an explosive mixture of flammable gases belonging to gas groups IIB and/or IIA. The transponder can be used in hazardous zones 1 and 2. IECEx classification is Ex ib IIB T4 Gb.'}</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Battery Powered', 'text': 'The RADius 700X is powered from an intrinsically safe encapsulated battery with an integral current limiting resistor and has no wired connection to external equipment.'}</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Unique ID', 'text': 'The transponders are coded with unique IDs ensuring reliable identification and tracking of vessels in demanding environments. Several interrogators can approach the same transponders, ensuring multi-user capabilities. Up to five transponders can be tracked simultaneously by the interrogator. The transponder is suited with dip switches for easy setting of the transponder ID.'}</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -11770,22 +11782,22 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius 800X transponder is a part of the short-distance relative positioning system RADius, developed for use in applications where the need for a robust and highly accurate relative positioning system is crucial. The system comprises an interrogator, installed on a vessel, operating in the 5.5 GHz band and transponders which are deployed on the target. The RADius 800X has an operating range of up to 1000 metres, and is suitable for fixed installations on typical a platform or an FPSO.'}</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Main Components', 'text': 'The main parts of the RADius 800X transponder equipment are: The transponder consisting of the transponderelectronic unit located behind a plastic cover (cover transparent to radio frequency used - 5.5 to 5.6 GHz), and the connection box with terminals for the DC voltage cable and a DIP switch for setting the Transponder Identification code. The Field Power Unit, with the intrinsically safe DC/DC PSD1004 power supply, located in the proximity of the transponder equipment. The safe area equipment: The Phoenix QUINT AC/DC power supply and the PSD1001C DC/DC barrier and power supply.'}</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'ATEX Certification and Unique ID', 'text': 'ATEX certification ATEX category 2 G product, gas group II B, temperature class T4, specified ambient temperature rating -20 °C to +60 °C. Unique ID The transponders are coded with unique IDs ensuring reliable identification and tracking of vessels in demanding environments. Several interrogators can approach the same transponders, ensuring multi-user capabilities. Up to five transponders can be tracked simultaneously by the interrogator.'}</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Environmental Specifications', 'text': 'Transponder and Field Power Unit Operating humidity 20 to 100 % RH Storage humidity 20 to 70 % RH. RADius 800X transponder electronic unit with IP 66 ingress protection, and connection box IP 66 ingress protection. PSD1001C power supply is also IP 66 protected with an operating temperature range of -20 °C to +60 °C, and a storage temperature range of +5 °C to +40 °C.'}</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -11863,22 +11875,22 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': 'The RADius replacement battery pack for RADius 550X and RADius 700X transponders consists of a primary cell and a series resistor and is non-rechargeable. The battery pack is intrinsically safe. The cell with its infallible resistor is completely moulded inside a stainless steel container. For use and instructions of the battery pack, refer to the RADius 550X and RADius 700X Instruction Manuals.'}</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Battery Longevity and Storage', 'text': 'The storage time of the RADius replacement battery for EX Transponders extends over 10 years at temperatures below +30 °C. Crafted with a Thionylchloride lithium battery, it endures a self-discharge rate of 1 to 2 % per year at room temperature. Recommended long-term storage conditions maintain a temperature below +30 °C, while short-term storage ranges from +5 °C to +40 °C.'}</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Electrical and Mechanical Integrity', 'text': 'With a no-load voltage of Max 3.67 V and an infallible integrated current limiting resistor of 390 R, the battery ensures electrical reliability. It can deliver a maximum output current of 10.1 mA, with 39.4 mW as the available power from the pack. Comprised of a non-rechargeable 19 Ah capacity, the battery encased in stainless steel, with the cell and resistor moulded inside with 3M Scotch-Weld™ Epoxy Adhesives type DP190 Grey, assures mechanical robustness.'}</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Certifications and Environmental Compliance', 'text': 'Accredited with ATEX, IECEx, and Inmetro certificates, the RADius battery pack meets high safety standards. Operational temperatures range from -25 to +60 °C and it possesses an Ingress protection rating of IP66, indicating a high level of protection against dust and water. Humidity resilience is strong, capable of withstanding 99 % non-condensing environments. Notably, while the bare battery cell is classified under UN 3090/3091 for transport, its secure encapsulation may exempt it from specific regulations.'}</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -11951,22 +11963,22 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': 'Introduction', 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>{'heading': "I don't know", 'text': "I don't know"}</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">

</xml_diff>